<commit_message>
Cypher Need Fix: Reply Nodes between Professor & Committee
</commit_message>
<xml_diff>
--- a/dataset/MISCCU.xlsx
+++ b/dataset/MISCCU.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,132 +437,127 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>研究生:</t>
+          <t>Author</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>研究生_外文</t>
+          <t>Author_Eng</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>論文名稱</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>論文名稱_外文:</t>
+          <t>Title_Eng</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>指導教授</t>
+          <t>Advisor</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>指導教授_外文</t>
+          <t>Advisor_Eng</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>口試委員</t>
+          <t>Oral_Defense_Committee</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>口試委員_外文</t>
+          <t>Oral_Defense_Committee_Eng</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>學位類別</t>
+          <t>degree</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>校院名稱</t>
+          <t>Institution</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>系所名稱</t>
+          <t>Department</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>學門</t>
+          <t>Narrow_Field</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>學類</t>
+          <t>Detailed_Field</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>論文出版年</t>
+          <t>Publication_Year</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>畢業學年度</t>
+          <t>Graduated_Academic_Year</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>語文別</t>
+          <t>language</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>論文頁數</t>
+          <t>number_of_pages</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>中文關鍵詞</t>
+          <t>keyword_chi</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>外文關鍵詞</t>
+          <t>keyword_eng</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>相關次數</t>
+          <t>Hits</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>點閱</t>
+          <t>Download</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>下載</t>
+          <t>Fav</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>書目收藏</t>
+          <t>Abstract</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>摘要</t>
+          <t>Cited</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>引用</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>連結網址</t>
+          <t>Thesis_URL</t>
         </is>
       </c>
     </row>
@@ -665,35 +660,34 @@
           <t>Graph Database、Concurrency Control、deadlock prevention、serializability</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>點閱:33</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>點閱:32</t>
+          <t>8</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
         <is>
           <t xml:space="preserve">
 2019 年繼 1987 年對關聯式資料庫的結構化查詢語言(SQL)標準成為國際標準組織(ISO)的資料庫查詢語言標準後，第二種資料庫查詢語言標準圖查詢語言(GQL)被提案至 ISO，為填補對圖形資料庫查詢語句(就像 SQL 之於關聯式資料庫)的不足。有鑑於 GQL 是新出的標準，尚未有其他人做過並行控制的研究，本研究設計了一套應用於圖形資料庫上的並行控制系統。該系統分為資料管理與鎖定狀態管理兩部分。資料儲存模型利用資料粒度將系統中的資料儲存區分為四層，其中第三層採用了紅黑樹結構降低了執行成本。並行控制機制採用雙版本的二階段鎖定，並用等-死法做為確保可序列化與死結預防的輔助機制。</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 Crawford, B.(2016). Granular Security In A Graph Database. Unpublished doctoral&lt;br/&gt;dissertation, Naval Postgraduate School, Monterey, California, United States.&lt;br/&gt;Lomet, D. (1995). Private Lock Management (Cambridge research laboratory&lt;br/&gt;technical report series No. 92/9). Cambridge, United Kingdom: University of&lt;br/&gt;Cambridge, Cambridge research laboratory.&lt;br/&gt;Alex, H., Steven ,S., &amp;amp; Steven, H.(2005). On deadlock, livelock, and forward&lt;br/&gt;progress (Tech. Rep. No. 633). Cambridge, United Kingdom: University of&lt;br/&gt;Cambridge, Computer Laboratory.&lt;br/&gt;Batra, S., &amp;amp; Tyagi, C. (2012). Comparative analysis of relational and graph databases.&lt;br/&gt;International Journal of Soft Computing and Engineering (IJSCE), 2(2), 509-512.&lt;br/&gt;Cahill, M. J., Rohm, U., &amp;amp; Fekete, A. D. (2009, December). Serializable Isolation for&lt;br/&gt;Snapshot Databases. ACM Transactions on Database Systems, 34(4), 20:1-20:42.&lt;br/&gt;Wu, H., Chin, W. N., &amp;amp; Jaffar, J. (2002, January). An efficient distributed deadlock avoidance&lt;br/&gt;algorithm for the AND model. IEEE Transactions on Software Engineering, 28(1), 18-29.&lt;br/&gt;Jabal, A. A., &amp;amp; Bertino, E. (2016, October). SimP: Secure Interoperable MultiGranular Provenance Framework. Paper presented at the International&lt;br/&gt;Conference on eScience, Baltimore, Maryland, United States.&lt;br/&gt;Lin, W. K., &amp;amp; Nolte, J. (1983). Basic Timestamp, Multiple Version Timestamp,&lt;br/&gt;and Two-Phase Locking. Paper presented at International Conference on Very&lt;br/&gt;Large Data Bases, Florence, Italy. 109-119.&lt;br/&gt;Mohamed, M., Badawy, M., &amp;amp; El-Sayed, A. (2016). Survey on Concurrency&lt;br/&gt;Control Techniques. Communications on Applied Electronics, 5(1), 28-31.&lt;br/&gt;Robinson, I., Webber, J., &amp;amp; Eifrem, E. (2015). Graph databases. Sebastopol,&lt;br/&gt;CA, United States: O’Reilly Media, Inc.&lt;br/&gt;Son, S. H., &amp;amp; David, R. (1994, November). Design and Analysis of A Secure&lt;br/&gt;Two-Phase Locking Protocol. Paper presented at the International Computer&lt;br/&gt;Software and Applications Conference, Taipei, Taiwan.374-379&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/r8yap3</t>
         </is>
@@ -798,35 +792,34 @@
           <t>Chatbot、Word2Vec、Word vector、TF-IDF、SVM</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>點閱:41</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>點閱:40</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
         <is>
           <t xml:space="preserve">
     隨著深度學習和自然語言處理的技術不斷進步，加上電子商務及即時通訊軟體的普及，促使問答聊天機器人的需求不斷提高。然而，使用者輸入的訊息千奇百怪，而且一個問題的表達方式可能有好幾種，甚至許多時候還會超出預設問答集本身的範圍，使得聊天機器人運用於常見問答更具複雜性及挑戰性。    本論文設計並提出一個基於檢索的一般性聊天機器人系統，利用大量電影及影集字幕的簡短對話來做為開放式問答集的來源，並以開放式問答集來處理超出預設問答集的情況。我們在聊天機器人的系統架構中使用Word2Vec預訓練的詞向量模型及TF-IDF（Term Frequency-Inverse Document Frequency）來得到每一個加權字詞向量，接著算出每一個問題文本的平均加權向量，再透過支援向量機（Support Vector Machine, SVM）分類模型、餘弦相似度方法、開放式問答集、推播通知和錯誤處理，建構出一個問答聊天機器人系統，具有語義層面上的檢索能力，且會隨著使用時間越久，回覆的準確度也將隨之提高。最後本論文以兩個不同領域的商家來實做客服問答聊天機器人，根據情境任務及問卷的分析結果顯示約八成的受測者認為可以快速且正確的取得一般問題的答案。期望可以透過本論文提出的聊天機器人系統，能做為第三方開發問答聊天機器人所參考的依據，並且能夠得到不錯的表現結果。</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 [1]Bickmore, T. W., Schulman, D., &amp;amp; Sidner, C.（2013）. Automated interventions for multiple health behaviors using conversational agents. Patient education and counseling, 92（2）, 142-148.&lt;br/&gt;[2]Cameron, A. F., &amp;amp; Webster, J. J. C. i. H. b. (2005). Unintended consequences of emerging communication technologies: Instant messaging in the workplace. 21(1), 85-103.&lt;br/&gt;[3]Caselles-Dupré, H., Lesaint, F., &amp;amp; Royo-Letelier, J.（2018, September）. Word2vec applied to recommendation: Hyperparameters matter. In Proceedings of the 12th ACM Conference on Recommender Systems, 352-356.&lt;br/&gt;[4]Collobert, R., Weston, J., Bottou, L., Karlen, M., Kavukcuoglu, K., &amp;amp; Kuksa, P.（2011）. Natural language processing（almost）from scratch. Journal of machine learning research, 12（ARTICLE）, 2493− 2537.&lt;br/&gt;[5]Graf, B., Krüger, M., Müller, F., Ruhland, A., &amp;amp; Zech, A.（2015, November）. Nombot: simplify food tracking. In Proceedings of the 14th International Conference on Mobile and Ubiquitous Multimedia, 360-363.&lt;br/&gt;[6]Djaballah, K. A., Boukhalfa, K., &amp;amp; Boussaid, O. (2019, December). Sentiment Analysis of Twitter Messages using Word2vec by Weighted Average. In 2019 Sixth International Conference on Social Networks Analysis, Management and Security(SNAMS), 223-228.&lt;br/&gt;[7]Higashinaka, R., Imamura, K., Meguro, T., Miyazaki, C., Kobayashi, N., Sugiyama, H., Hirano, T., Makino, T., Matsuo, Y.（2014, August）. Towards an open-domain conversational system fully based on natural language processing. In Proceedings of COLING 2014, the 25th International Conference on Computational Linguistics: Technical Papers, 928-939.&lt;br/&gt;[8]Kerly, A., Ellis, R., &amp;amp; Bull, S.（2008, April）. CALMsystem: a conversational agent for learner modelling. In International Conference on Innovative Techniques and Applications of Artificial Intelligence,  Applications and Innovations in Intelligent Systems, 89-102.&lt;br/&gt;[9]Kowsher, M., Alam, M. A., Uddin, M. J., Islam, M. R., Pias, N., &amp;amp; Saifullah, A. R. M.（2019, July）. Bengali Informative Chatbot. In 2019 International Conference on Computer, Communication, Chemical, Materials and Electronic Engineering（IC4ME2）, 1-7&lt;br/&gt;[10]Lester, J., Branting, K., &amp;amp; Mott, B.（2004）. Conversational agents. The Practical Handbook of Internet Computing, 220-240.&lt;br/&gt;[11]Lo, R. T.-W., He, B., &amp;amp; Ounis, I.（2005）. Automatically building a stopword list for an information retrieval system. In Journal on Digital Information Management: Special Issue on the 5th Dutch-Belgian Information Retrieval Workshop（DIR）.&lt;br/&gt;[12]Manning, C., &amp;amp; Schutze, H.（1999）. Foundations of statistical natural language processing, Cambridge, MA.: MIT press.&lt;br/&gt;[13]Mikolov, T., Chen, K., Corrado, G., &amp;amp; Dean, J.（2013）. Efficient estimation of word representations in vector space. arXiv preprint arXiv:1301.3781.&lt;br/&gt;[14]Mikolov, T., Sutskever, I., Chen, K., Corrado, G. S., &amp;amp; Dean, J.（2013）. Distributed representations of words and phrases and their compositionality. In Advances in neural information processing systems, 3111–3119.&lt;br/&gt;[15]Razzaghnoori, M., Sajedi, H., &amp;amp; Jazani, I. K.（2018）. Question classification in Persian using word vectors and frequencies. Cognitive Systems Research, 47, 16-27.&lt;br/&gt;[16]Rumelhart, D. E., Hinton, G. E., &amp;amp; McClelland, J. L.（1986）. A general framework for parallel distributed processing. Parallel distributed processing: Explorations in the microstructure of cognition, 1（45-76）, 26.&lt;br/&gt;[17]Sharma, V., Goyal, M., &amp;amp; Malik, D.（2017）. An intelligent behaviour shown by chatbot system. International Journal of New Technology and Research, 3（4）, 2454-4116.&lt;br/&gt;[18]Shevat, A.（2017）. Designing Bots: Creating Conversational Experiences. California, CA: O'Reilly Media, Inc.&lt;br/&gt;[19]Singh, S. P., Kearns, M. J., Litman, D. J., &amp;amp; Walker, M. A. （2000）. Reinforcement learning for spoken dialogue systems. In Advances in Neural Information Processing Systems., 956-962.&lt;br/&gt;[20]Thada, V., &amp;amp; Jaglan, V.（2013）. Comparison of jaccard, dice, cosine similarity coefficient to find best fitness value for web retrieved documents using genetic algorithm. International Journal of Innovations in Engineering and Technology, 2（4）, 202-205.&lt;br/&gt;[21]Wang, H., Lu, Z., Li, H., &amp;amp; Chen, E.（2013, October）. A dataset for research on short-text conversations. In Proceedings of the 2013 Conference on Empirical Methods in Natural Language Processing, 935-945.&lt;br/&gt;[22]Warschauer, M., &amp;amp; Healey, D.（1998）. Computers and language learning: An overview. Language teaching, 31（2）, 57-71.&lt;br/&gt;[23]Weizenbaum, J.（1966）. ELIZA---a computer program for the study of natural language communication between man and machine. Communications of the ACM, 9（1）, 36-45.&lt;br/&gt;[24]Wu, Y., Li, Z., Wu, W., &amp;amp; Zhou, M.（2018）. Response selection with topic clues for retrieval-based chatbots. Neurocomputing, 316, 251-261.&lt;br/&gt;[25]Young, S., Gašić, M., Thomson, B., &amp;amp; Williams, J. D.（2013）. Pomdp-based statistical spoken dialog systems: A review. Proceedings of the IEEE, 101（5）, 1160-1179.&lt;br/&gt;[26]Zadrozny, W., Budzikowska, M., Chai, J., Kambhatla, N., Levesque, S., &amp;amp; Nicolov, N.（2000）. Natural language dialogue for personalized interaction. Communications of the ACM, 43（8）, 116-120.&lt;br/&gt;[27]Zhang, D., Xu, H., Su, Z., &amp;amp; Xu, Y.（2015）. Chinese comments sentiment classification based on word2vec and SVMperf. Expert Systems with Applications, 42（4）, 1857-1863.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/4x4cm4</t>
         </is>
@@ -931,35 +924,33 @@
           <t>5G、data visualization、text exploration</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>點閱:116</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>點閱:115</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
         <is>
           <t xml:space="preserve">
 在資訊發逹的年代，每個人隨時都可透過網路來搜尋資訊，搜尋引擎下達關鍵字之後，眾多資訊排列而出，使用者在這些龐大的資料下，難以短時間查得真正適合的相關資訊，且接觸的資訊過多會使人注意力無法集中，要尋找符合自己所需的資料是費時又困難的。本研究以5G為搜尋的主題，利用網路爬蟲搜集2016年至2019年間的新聞網站文章，並藉由文字探勘技術提取與主題關聯性較高的關鍵字，相關聯關鍵字集成為一知識庫，並依據搜集資料的特徵，設計具互動性及主題關聯性的視覺化圖形，讓主題相關聯的資訊易於理解與獲得；本研究針對想關注議題提供提醒功能，只依據有興趣、想關注的議題提供通知訊息，透過個人訊息管理策略來過濾並簡化訊息，可以減少資訊過載問題。</t>
         </is>
       </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="Z4" t="inlineStr">
-        <is>
-          <t>&lt;div style="padding:10px;text-align:left;"&gt;
-英文文獻&lt;br/&gt;Aizawa, A. J. I. P., &amp;amp; Management. (2003). An information-theoretic perspective of tf–idf measures. 39(1), 45-65.&lt;br/&gt;Anand, A., De Veciana, G., &amp;amp; Shakkottai, S. (2018). Joint scheduling of URLLC and eMBB traffic in 5G wireless networks. Paper presented at the IEEE INFOCOM 2018-IEEE Conference on Computer Communications.&lt;br/&gt;Andrews, J. G., Buzzi, S., Choi, W., Hanly, S. V., Lozano, A., Soong, A. C., et al. (2014). What will 5G be? , 32(6), 1065-1082.&lt;br/&gt;Bao, F., &amp;amp; Chen, J. (2014). Visual framework for big data in d3. js. Paper presented at the 2014 IEEE Workshop on Electronics, Computer and Applications.&lt;br/&gt;Bertino, E., Guerrini, G., &amp;amp; Merlo, I. (2000). Trigger inheritance and overriding in an active object database system. IEEE Transactions on Knowledge and Data Engineering, 12(4), 588-608.&lt;br/&gt;Bockelmann, C., Pratas, N., Nikopour, H., Au, K., Svensson, T., Stefanovic, C., et al. (2016). Massive machine-type communications in 5G: Physical and MAC-layer solutions. 54(9), 59-65.&lt;br/&gt;Demšar, J., Curk, T., Erjavec, A., Gorup, Č., Hočevar, T., Milutinovič, M., et al. (2013). Orange: data mining toolbox in Python. The Journal of Machine Learning Research, 14(1), 2349-2353.&lt;br/&gt;Edmunds, A., &amp;amp; Morris, A. (2000). The problem of information overload in business organisations: a review of the literature. International journal of information management, 20(1), 17-28.&lt;br/&gt;Friederici, A. D. J. T. i. c. s. (2002). Towards a neural basis of auditory sentence processing. 6(2), 78-84.&lt;br/&gt;Hao, L., &amp;amp; Hao, L. (2008). Automatic identification of stop words in chinese text classification. Paper presented at the Computer Science and Software Engineering, 2008 International Conference on.&lt;br/&gt;Kabra, N., Patel, J. M., Yu, J.-B., Nag, B., &amp;amp; Chen, J.-J. (2004). Method and apparatus for parallel execution of trigger actions: Google Patents.&lt;br/&gt;Kirk, A. (2012). Data Visualization: a successful design process: Packt Publishing Ltd.&lt;br/&gt;Ma, W.-Y., &amp;amp; Chen, K.-J. (2003). Introduction to CKIP Chinese word segmentation system for the first international Chinese Word Segmentation Bakeoff. Paper presented at the Proceedings of the second SIGHAN workshop on Chinese language processing-Volume 17.&lt;br/&gt;Mahto, D. K., &amp;amp; Singh, L. (2016). A dive into Web Scraper world. Paper presented at the 2016 3rd International Conference on Computing for Sustainable Global Development (INDIACom).&lt;br/&gt;Osseiran&lt;/div&gt;</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/2y6v68</t>
         </is>
@@ -1064,10 +1055,14 @@
           <t>Electronic Medical Record、Information security、Database、Data Loss Prevention、Data Mask</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>點閱:138</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>點閱:136</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1076,23 +1071,18 @@
         </is>
       </c>
       <c r="X5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 隨著科技的進步，醫療院所的病歷資料開始電子化，資訊科技帶來了便利性，隨之產生了許多資訊安全的問題。近年來電子病歷的資訊安全議題都備受重視，許多研究都有相關的探討，但本研究發現許多的研究議題都主要著重在防護外部的威脅，內部人員的疏失等研究相對較少，但近幾年的新聞事件中，由人員所引發的資料外洩問題頻頻出現，為改善此問題，因此本研究擬定了一個資訊安全防護方法，著重在內部人員洩漏資訊的問題防護。  本研究著重於資料遮罩以及資料遮罩，建置可用不同符號來遮蔽的資料遮罩，以及監控資料庫軌跡動作的觸發程序，針對新增、刪除、修改監控是誰做、如何做、何時、為了甚麼等，並且建立觸發程序的副本，使用該副本可以快速建立每個資料表的觸發程序，另外還可以透過SQL工具來儲存使用者的訪問記錄，最後用網頁的方式來呈現整體的資訊安全防護運作模式。藉由本研究規劃的資訊安全策略，加強電子病歷資料庫的內部防護，改善資料外洩的問題再度發生。</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 中央研究院 資訊服務處（民國107）。資安課程。民國108年1月28日，取自：https://its.sinica.edu.tw/site/datas/detail/12595/38/167/282/0&lt;br/&gt;王平、林文暉、郭溥村、王子夏與盧永翔（民99）。雲端運算服務之資安風險與挑戰。Communications of the CCISA，16(4)。&lt;br/&gt;安資捷(股)公司（民國105）。Informatica DDM 動態資料遮罩。民國108年1月28日，取自：http://www.amxecure.com/index.php/products-solutions/tactics-policy-services/db-security/168-informatica-ddm&lt;br/&gt;吳昭儀（民106）。ISO27001 最新版標準條文介紹，民國108年1月28日，取自：https://its.sinica.edu.tw/uploads/editor/files/20170426-ISO27001.pdf&lt;br/&gt;周彥妤（民國107年06月20日）。北市聯醫外洩愛滋病患3000筆個資 坦言有疏失。自由時報。&lt;br/&gt;林孝儒（民國107年09月12日）。紐約醫院爆個資外洩，98名病患資訊被看光。蘋果日報。&lt;br/&gt;施惟堯（民105）。A4: 基於屬性加密演算法之電子病歷系統的身分認證, 授權與存取控制機制。交通大學電機工程系所學位論文，1-74。&lt;br/&gt;洪彬益（民103）。導入資料外洩防護系統關鍵影響因素之多重個案研究。交通大學管理學院資訊管理學程學位論文，1-79。&lt;br/&gt;陳怡均（民國107年10月10日）。50萬個資外洩Google＋關閉。工商時報。&lt;br/&gt;陳衍良（民104）。如何防止醫院員工違反電子病歷隱私保護政策。義守大學醫務管理學系學位論文，1-51。&lt;br/&gt;陳維揚（民105）。以ISO27001探討醫院資訊安全系統。中正大學資訊管理系醫療資訊管理研究所學位論文，1-46。&lt;br/&gt;傅家妤（民國107年05月19日）。紅髮艾德入院「個資外洩」，醫院員工遭開除。ETtoday新聞雲。&lt;br/&gt;曾昭宏（民國95）。認識資訊安全標準”BS7799””ISO27001”。民國95年12月05日，取自：https://www.cga.gov.tw/GipOpen/wSite/ct?xItem=33830&amp;amp;ctNode=4336&amp;amp;mp=999033&lt;br/&gt;曾愽睿（民107）。運用時間戳記之安全存取機制於電子病歷系統。東海大學電機工程學系學位論文，1-44。&lt;br/&gt;黃仁俊與張軒齊（民107）。雲端外儲系統資料保護機制。資訊安全通訊，24(3)，1-15。&lt;br/&gt;楊漢湶. (2012). 電子病歷與病人隱私權保護. 澄清醫護雜誌, 8(1), 4-8。&lt;br/&gt;資訊安全網頁。附錄A資通安全管理規範。民國108年1月28日，取自：http://auis.epage.au.edu.tw/ezfiles/288/1288/img/2505/149554988.pdf.&lt;br/&gt;樊國楨、劉家志與黃健誠（民99）。資訊安全護理之一: 終端護理。資訊安全通訊，16(1), 4-25。&lt;br/&gt;衛生福利部資訊處（民107）。民107年12月10日，取自：https://emr.mohw.gov.tw/pmointro.aspx&lt;br/&gt;衛生福利部電子病歷交換中心（民104）。民107年12月10日，取自：https://eec.mohw.gov.tw/?PAGE=Overview&lt;br/&gt;鄭翠碧（民國108年06月24日）。伊院護士疑洩612求診者私隱 院方邀「外援」處理投訴。香港01。&lt;br/&gt;魯明德（民102）。電子病歷安全防護。清流月刊，1。&lt;br/&gt;叡揚資訊 資安事業處（民國104）。金融機構DLP導入案例 預防資料外洩風險。民國108年1月28日，取自：https://www.gss.com.tw/index.php/focus/security/1431-gss-0118-dlp&lt;br/&gt;臉書承認遭駭客攻擊 5000萬用戶有個資外洩風險（民國107年9月29日）。自由時報。&lt;br/&gt;Adrian Michael Booth, and Manmeet Singh Bhasin (2009). Real-time enterprise data masking. U.S. Patent Application No. 12/287, 324.&lt;br/&gt;Basavaraj Biradar (2016). INSERTED and DELETED Logical Tables in Sql Server. Retrieved September 16, 2018, from http://sqlhints.com/2016/02/28/inserted-and-deleted-logical-tables-in-sql-server/&lt;br/&gt;Brisebois, M., &amp;amp; Johnstone, C. (2017). System and method for data loss prevention across heterogeneous communications platforms. U.S. Patent No. 9,578,060. Washington, DC: U.S. Patent and Trademark Office.&lt;br/&gt;Farkash, Ariel, Igor Gokhman, and Sivan Rabinovich.(2018). Dynamic data masking of post-output database data. U.S. Patent No. 9,911,003.Washington, DC: U.S. Patent and Trademark Office.&lt;br/&gt;Garg, Sushil. (2017). Survey on Cloud Computing and Data Masking Techniques.&lt;br/&gt;GK, Ravi Kumar, B. Justus Rabi, and T. N. Manjunath. (2012). A study on dynamic data masking with its trends and implications.&lt;br/&gt;Iain Fergusson (2006). System and method for dynamic data masking. U.S. Patent Application No. 10/957,971.&lt;br/&gt;Kristen M Krysko, Noah M Ivers, Jacqueline Young, Paul O’Connor, and Karen Tu (2015). Identifying individuals with multiple sclerosis in an electronic medical record. Multiple Sclerosis Journal, 21(2), 217-224.&lt;br/&gt;Mansfield-Devine, S. (2014). Network Security. Masking sensitive data, 2014(10), 17-20.&lt;br/&gt;Medvedev, I. (2017). Systems and methods for data loss prevention while preserving privacy. U.S. Patent No. 9,740,877. Washington, DC: U.S. Patent and Trademark Office.&lt;br/&gt;OWASP(2017). OWASP Top Ten 2017. Retrieved, October 30, 2019 from https://www.owasp.org&lt;br/&gt;Shukla, M., Joseph, J., Vidhani, K., Banahatti, V. M., and Lodha, S.(2015) Dynamic data masking. U.S. Patent No. 9,171,182. Washington, DC: U.S. Patent and Trademark Office.&lt;br/&gt;Simon Liu, and Rick Kuhn (2010). Data loss prevention. IT professional, 12(2).&lt;br/&gt;Steven Patrick Pomroy, Robert Raymond Lake, Trevor Anthony Dunn(2011). Data masking system and method. U.S. Patent No. 7,974,942.&lt;br/&gt;Stevestein(2018). SQL Server Management Studio (SSMS) - SQL Server. Retrieved, October 16, 2018 from https://docs.microsoft.com/en-us/sql/ssms/sql-server-management-studio-ssms?view=sql-server-2017&amp;amp;viewFallbackFrom=sql-server-201&lt;br/&gt;Tomoyoshi Takebayashi, Hiroshi Tsuda, Takayuki Hasebe, and Ryusuke Masuoka (2010). Data loss prevention technologies. Fujitsu Scientific and Technical Journal, 46(1), 47-55.&lt;br/&gt;VanMSFT. (2017). Security Center for SQL Server Database Engine and Azure SQL Database - SQL Server. Retrieved September 16, 2018 from https://docs.microsoft.com/en-us/sql/relational-databases/security/security-center-for-sql-server-database-engine-and-azure-sql-database?view=sql-server-2017&lt;br/&gt;Yui K. Ho, William C. Moyer, and Joseph A. Gutierrez (1994). Data processor with concurrent static and dynamic masking of operand information and method therefor. U.S. Patent No. 5,319,763.&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
+      <c r="Z5" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/q222jc</t>
         </is>
@@ -1197,35 +1187,34 @@
           <t>Reversed Engineering、Electronic Medical Records</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>點閱:63</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>點閱:63</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
         <is>
           <t xml:space="preserve">
 資訊產業日益發達，各行各業中的紙本文件電子化已經是情勢所趨，而在醫療產業中紙本文件很大的比例為病歷紀錄，所以由紙本病歷轉化為電子病歷更是重要的目標，可以提升醫療的服務效率、降低醫療成本以及改善醫療品質，但我國的醫療資訊系統多為自行開發或委託廠商開發，導致開發後的內容不盡相同，容易發生資訊孤島的狀況，在開發的過程中也會耗費大量的人力、時間與成本。本研究以逆向工程的方式分析衛生福利部公告之電子病歷單張，進而得到電子病歷單張中所包含的資訊，以此做為開發醫療資料庫的依據。逆向工程開發的步驟不同於一般開發流程，是由完整的結果反向解析其中的內容，以了解醫療資料庫中需要包含的內容與架構。以此作法除了可以加速開發速度、降低過程中所造成的人力、金錢與時間，也可以得到較為完整且標準的資料庫。本研究也與醫療資訊系統之資料庫進行實際的比對，其結果發現本研究所產出的醫療資料庫架構相當接近目前所使用的醫療資料庫。</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr">
+      <c r="Y6" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 DIGITIMES企劃（民103）。臨床資料庫管理與應用。民國108年9月25日，取自：https://www.digitimes.com.tw/iot/article.asp?cat=158&amp;amp;cat1=&amp;amp;cat2=&amp;amp;id=0000402369_n112wgd271iutk833ihk5&lt;br/&gt;中央健康保險署高屏業務組（民107）。健保醫療資訊雲端查詢系統。民國108年1月29日，取自：https://www.nhi.gov.tw/Resource/Registration/7241_21070629%E5%81%A5%E4%BF%9D%E9%86%AB%E7%99%82%E8%B3%87%E8%A8%8A%E9%9B%B2%E7%AB%AF%E6%9F%A5%E8%A9%A2%E7%B3%BB%E7%B5%B1%E7%B0%A1%E5%A0%B1.pdf&lt;br/&gt;中華民國護理師護士公會全國聯合會（民107年12月）。107年12月台閩地區護理人員統計表。民國107年12月15日，取自：http://www.nurse.org.tw/publicUI/H/H10201.aspx?arg=8D659CC635DE1BC071&lt;br/&gt;行政院衛生署（民98年12月24日）。醫院資訊系統規範2.0。台北市：行政院。民國107年12月15日，取自：http://www.doh.gov.tw/ufile/doc/醫院資訊系統規範推動計畫.pdf&lt;br/&gt;吳仁和與林信惠（民101）。系統分析與設計理論與實務應用（五版）。台北市：智勝文化。&lt;br/&gt;李依䤴（民102）。電子病歷交換與其對醫院績效之前因探討：雲端運算觀點。中正大學醫療資訊管理研究所碩士論文，台灣博碩士論文知識加值系統，嘉義縣。&lt;br/&gt;李淑宜、歐淑儀與張宏泰（民104）。實施電子病歷廢除紙本保存之效益分析-以南部某醫學中心為例。病歷資訊管理，13(2)，1-18。&lt;br/&gt;林思廷、王帝皓、蕭正英、劉裕明、陳曾基與胡育文（民107）。整合多套放射腫瘤與醫療資訊系統以實現病歷電子化。放射治療與腫瘤學，25(1)，21-32。&lt;br/&gt;胡毓萍、李佳琳、劉宇倫、張啟明與莊人祥（民105）。運用醫院電子病歷進行傳染病通報之效益評估。醫療資訊雜誌，25(1)，23-31。&lt;br/&gt;徐嫦娥與簡郁沛（民99）。電子病歷之發展及法規政策。病歷資訊管理，9(2)，1-18。&lt;br/&gt;郭光明、余明玲與黃興進（民99）。如何成功導入電子病歷系統：醫院觀點。病歷資訊管理，9(2)，19-36。&lt;br/&gt;陳俞琪與張博論（民105）。應用健康資訊科技於慢性腎臟病持續性照護之契機與反思。護理雜誌，63(2)，12-18。&lt;br/&gt;陳楚杰（民92）。醫院組織與管理（十版）。台北市：宏翰文化。&lt;br/&gt;黃興進（民91）。醫療資訊管理系統研究議題之探討。資訊管理學報，9(S)，101-116。&lt;br/&gt;黃興進、余明玲、劉忠峰（民95）。醫療資訊管理概論（初版）。嘉義市：台灣健康資訊管理學會。&lt;br/&gt;楊沛墩、陳彥臣與黃援傑（民100）。電子病歷推動現況及檢討建言。病歷資訊管理10(2)，1-11。&lt;br/&gt;劉建材、許明輝、楊沛墩與馮容莊（民101）。台灣醫療機構實施電子病歷之探討。領導護理，13(2)，2-11。&lt;br/&gt;衛生福利部中央健康保險署（民105）。民國108年1月29日，取自：https://www.nhi.gov.tw/Content_List.aspx?n=B900CECCFF6A2198&amp;amp;topn=CA428784F9ED78C9&lt;br/&gt;衛生福利部中央健康保險署（民107）。民國108年1月29日，取自：https://www.nhi.gov.tw/Content_List.aspx?n=8FD3AB971F557AD4&amp;amp;topn=CA428784F9ED78C9&lt;br/&gt;衛生福利部統計處（民107）。106年度醫療服務量。民國107年1月30日，取自：https://dep.mohw.gov.tw/DOS/lp-4033-113.html&lt;br/&gt;衛生福利部資訊處（民107）。民國107年12月15日，取自：https://emr.mohw.gov.tw/introduction.aspx&lt;br/&gt;衛生福利部電子病歷交換中心（民107）。民國107年12月15日，取自：https://eec.mohw.gov.tw/?PAGE=EMRH&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22105PCCU0396008%22.&amp;amp;searchmode=basic" target="_blank"&gt;簡毅（民106）。以結構內容相似度為基礎之Android惡意軟體偵測。中國文化大學資訊管理研究所碩士論文，博碩士論文網，臺北市。&lt;/a&gt;&lt;br/&gt; &lt;br/&gt;Alshamrani, A. and Bahattab, A. (2015). A comparison between three SDLC models waterfall model, spiral model, and Incremental/Iterative model. International Journal of Computer Science Issues (IJCSI), 12(1), 106.&lt;br/&gt;Arthur, J.D., Nance, R.E. and Balci, O. (1993). Establishing software development process control: technical objectives, operational requirements, and the foundational framework. Journal of Systems and Software, 22(2), 117-128.&lt;br/&gt;Coronel, C. and Morris, S. (2016). Database systems: design, implementation, &amp;amp; management. Cengage Learning.&lt;br/&gt;Dhayashankar, J. M. and Ramani, A. V. (2017). A Perspective Survey on Software and Database Reverse Engineering Methodologies. International Journal of Engineering Science, 15469.&lt;br/&gt;Dick, R.S., Steen, E.B. and Detmer, D.E. (1997). The Computer-Based Patient Record: Revised Edition: An Essential Technology for Health Care. Washington (DC): National Academies Press (US).&lt;br/&gt;Elghadhafi, H. A., Abdelaziz, T. M. and Maatuk, A. M. (2018). A Novel Approach for Improving the Quality of Software Code using Reverse Engineering. In Proceedings of the Fourth International Conference on Engineering &amp;amp; MIS 2018, 31. ACM.&lt;br/&gt;Falter, T., Hutzel, D. and Baeuerle, S. (2016). U.S. Patent No. 9,430,523. Washington, DC: U.S. Patent and Trademark Office.&lt;br/&gt;Genero, M., Piattini, M. and Calero, C. (2002). Empirical validation of class diagram metrics. In Empirical Software Engineering, 2002. Proceedings. 2002 International Symposium n (pp. 195-203). IEEE.&lt;br/&gt;Glaser, J., Teich, J. M. and Kuperman, G. (1996). Impact of information events on medical care. In Proceedings and abstracts of the 1996 Healthcare Information and Management Systems Society Annual Conference, 1-9.&lt;br/&gt;Haux, R. (2006). Health information systems–past, present, future. International journal of medical informatics, 75(3-4), 268-281.&lt;br/&gt;Jardim, S.V. (2013). The electronic health record and its contribution to healthcare information systems interoperability. Procedia Technology, 9, 940-948.&lt;br/&gt;Matharu, G.S., Mishra, A., Singh, H. and Upadhyay, P. (2015). Empirical study of agile software development methodologies: A comparative analysis. ACM SIGSOFT Software Engineering Notes, 40(1), 1-6.&lt;br/&gt;Raghupathi, W. (1997). Health care information systems. Communications of the ACM, 40(8), 80-83.&lt;br/&gt;Teich, J. M., Merchia, P. R., Schmiz, J. L., Kuperman, G. J., Spurr, C. D. and Bates, D. W. (2000). Effects of computerized physician order entry on prescribing practices. Archives of internal medicine, 160(18), 2741-2747.&lt;br/&gt;Uslu, A.M. and Stausberg, J. (2008). Value of the electronic patient record: An analysis of the literature. Journal of Biomedical Informatics, 41, 675-682.&lt;br/&gt;Waegemann, C.P. (2000). Spotlight on healthcare: Document imaging in healthcare: One piece of puzzle in creating electronic patient record systems, Inform, 14(1), 8-10.&lt;br/&gt;Wellsandt, S., Cattaneo, L., Cerri, D., Terzi, S., Corti, D., Norden, C. and Ahlers, R. (2019). Life Cycle Management for Product-Service Systems. In Models, Methods and Tools for Product Service Design, 29-43. Springer, Cham.&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/ru358m</t>
         </is>
@@ -1330,35 +1319,34 @@
           <t>Mind Map、Clinical Decision Support System (CDSS)、Knowledge Base、Acute Stroke、Acute Myocardial Infarction (AMI)、Major Trauma、Severe Sepsis</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>點閱:108</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>點閱:108</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
         <is>
           <t xml:space="preserve">
 近年來，醫院急診室因醫護人力吃緊、民眾濫用急診，加上醫院未落實急診檢傷分類、分級醫療制度等因素，而導致病人停留急診室的時間拉長，而使得急診壅塞的問題產生，其不僅造成需緊急救治的急重症患者受到影響，無法在有效的時間內接受適當的治療，錯失黃金的救援時間，而導致病人病情惡化，甚至死亡，也容易造成醫療資源的浪費。有鑑於此，本研究認為若能建置一套急重症照護決策知識庫，提供急重症照護流程指引內容，作為急診醫護人員決策時的參考依據，將能簡化急診醫護人員的作業流程、提高臨床工作效率，對於需緊急救治的急重症患者也能提供更完善的醫療服務。本研究是以心智圖作為知識表達的工具，利用心智圖中文字、符號、數字、線條、顏色等技巧來呈現四大急重症（急性腦中風、急性心肌梗塞、重大外傷、嚴重敗血症）個別的處置流程，希望藉由心智圖的方式呈現出內容更加多元、豐富，但更節省時間、方便理解的新系統說明文件參照模式，以協助系統開發人員在與醫院急診醫護人員進行溝通時，能使雙方更加瞭解彼此的需求，使系統開發人員在最後建置此知識庫的過程中，更有效的架設出一套符合急診醫護人員實際需求的急重症照護決策系統，使醫療資源更有效的被利用。</t>
         </is>
       </c>
-      <c r="Z7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 英文文獻&lt;br/&gt;Alavi, M., &amp;amp; Leidner, D. E. (2001). Knowledge management and knowledge management systems: Conceptual foundations and research issues. MIS quarterly, 107-136.&lt;br/&gt;Baker, S. P., O'Neill, B., Haddon Jr, W., &amp;amp; Long, W. B. (1974). The injury severity score: a method for describing patients with multiple injuries and evaluating emergency care. Journal of Trauma and Acute Care Surgery, 14(3), 187-196.&lt;br/&gt;Barquist, E., Pizzutiello, M., Tian, L., Cox, C., &amp;amp; Bessey, P. Q. (2000). Effect of trauma system maturation on mortality rates in patients with blunt injuries in the Finger Lakes Region of New York State. Journal of Trauma and Acute Care Surgery, 49(1), 63-70.&lt;br/&gt;Beckman, T. (1997, July). A Methodology for knowledge management. In IASTED (Chair), Artificial intelligence and soft computing. International Association of Science and Technology for Development (IASTED) AI and Soft Computing Conference, Canada: Banff.&lt;br/&gt;Benbya, H., &amp;amp; Belbaly, N. A. (2005). Mechanisms for knowledge management systems effectiveness: an exploratory analysis. Knowledge and Process Management, 12(3), 203-216.&lt;br/&gt;Bone, R. C., Balk, R. A., Cerra, F. B., Dellinger, R. P., Fein, A. M., Knaus, W. A., Schein, R. M., &amp;amp; Sibbald, W. J. (1992). The ACCP/SCCM Consensus Conference Committee: American College of Chest Physicians/Society of Critical Care Medicine Consensus Conference: Definitions for sepsis and organ failure and guidelines for the use of innovative therapies in sepsis. Crit Care Med, 20, 864-874.&lt;br/&gt;Booker, C.C., &amp;amp; Andrews, P.N. (2013). A discussion of clinical decision support services. Clin Obstet Gynecol, 56(3), 446-52.&lt;br/&gt;Bull, J. P. (1975). The injury severity score of road traffic casualties in relation to mortality, time of death, hospital treatment time and disability. Accident Analysis &amp;amp; Prevention, 7(4), 249-255.&lt;br/&gt;Cardoso, L. T., Grion, C. M., Matsuo, T., Anami, E. H., Kauss, I. A., Seko, L., &amp;amp; Bonametti, A. M. (2011). Impact of delayed admission to intensive care units on mortality of critically ill patients: a cohort study. Critical Care, 15(1), 1.&lt;br/&gt;Castillo, R. S., &amp;amp; Kelemen, A. (2013). Considerations for a successful clinical decision support system. Computers Informatics Nursing, 31(7), 319-326.&lt;br/&gt;Chalfin, D. B., Trzeciak, S., Likourezos, A., Baumann, B. M., Dellinger, R. P., &amp;amp; DELAY-ED study group. (2007). Impact of delayed transfer of critically ill patients from the emergency department to the intensive care unit. Critical care medicine, 35(6), 1477-1483.&lt;br/&gt;Cowan, R. M., &amp;amp; Trzeciak, S. (2004). Clinical review: emergency department overcrowding and the potential impact on the critically ill. Critical care, 9(3), 291.&lt;br/&gt;Davies, J., Fensel, D., &amp;amp; Van Harmelen, F. (2003). Towards the semantic web. Ontology-Driven Knowledge Management.&lt;br/&gt;Dellinger, R. P., Levy, M. M., Rhodes, A., Annane, D., Gerlach, H., Opal, S. M., Sevransky, J. E., Sprung, C. L., Douglas, I. S., Jaeschke, R., Osborn, T. M., Nunnally, M. E., Townsend, S. R., Reinhart, K., Kleinpell, R. M., Angus, D. C., Deutschman, C. S., Machado, F. R., Rubenfeld, G. D, Webb, S., Beale, R. J., Vincent, J. L., Moreno, R., &amp;amp; The Surviving Sepsis Campaign Guidelines Committee including The Pediatric Subgroup. (2013). Surviving Sepsis Campaign: international guidelines for management of severe sepsis and septic shock, 2012. Intensive care medicine, 39(2), 165-228.&lt;br/&gt;Derlet, R. W., &amp;amp; Richards, J. R. (2000). Overcrowding in the nation’s emergency departments: complex causes and disturbing effects. Annals of emergency medicine, 35(1), 63-68.&lt;br/&gt;Derlet, R. W., &amp;amp; Richards, J. R. (2002). Emergency department overcrowding in florida, new york, and texas. Southern medical journal, 95(8), 846-850.&lt;br/&gt;Fromm Jr, R. E., Gibbs, L. R., Mccallum, W. G., Niziol, C., Babcock, J. C., Gueler, A. C., &amp;amp; Levine, R. L. (1993). Critical care in the emergency department: A time-based study. Critical care medicine, 21(7), 970-976.&lt;br/&gt;Garg, A. X., Adhikari, N. K., McDonald, H., Rosas-Arellano, M. P., Devereaux, P. J., Beyene, J., Sam, J., &amp;amp; Haynes, R. B. (2005). Effects of computerized clinical decision support systems on practitioner performance and patient outcomes: a systematic review. Jama, 293(10), 1223-1238.&lt;br/&gt;Gibson, C. M., Pride, Y. B., Frederick, P. D., Pollack Jr, C. V., Canto, J. G., Tiefenbrunn, A. J., Weaver, W. D., Lambrew, C. T., French, W. J., Peterson, E. D., &amp;amp; Rogers, W. J. (2008). Trends in reperfusion strategies, door-to-needle and door-to-balloon times, and in-hospital mortality among patients with ST-segment elevation myocardial infarction enrolled in the National Registry of Myocardial Infarction from 1990 to 2006. American heart journal, 156(6), 1035-1044.&lt;br/&gt;Gordon, J. A., Billings, J., Asplin, B. R., &amp;amp; Rhodes, K. V. (2001). Safety net research in emergency medicine proceedings of the academic emergency medicine consensus conference on “The Unraveling Safety Net”. Academic Emergency Medicine, 8(11), 1024-1029.&lt;br/&gt;Gory, B., Eldesouky, I., Sivan-Hoffmann, R., Rabilloud, M., Ong, E., Riva, R., Gherasim, D. N., Turjman, A., Nighoghossian, N., &amp;amp; Turjman, F. (2016). Outcomes of stent retriever thrombectomy in basilar artery occlusion: an observational study and systematic review. J Neurol Neurosurg Psychiatry, 87(5), 520-525.&lt;br/&gt;Hacke, W., Kaste, M., Fieschi, C., Toni, D., Lesaffre, E., Von Kummer, R., Boysen, G., Bluhmki, E., Höxter, G., Mahagne, M. H., &amp;amp; Hennerici, M. (1995). Intravenous thrombolysis with recombinant tissue plasminogen activator for acute hemispheric stroke: the European Cooperative Acute Stroke Study (ECASS). Jama, 274(13), 1017-1025.&lt;br/&gt;Hacke, W., Kaste, M., Fieschi, C., Von Kummer, R., Davalos, A., Meier, D., Larrue, V., Bluhmki, E., Davis, S., Donnan, G., Schneider, D., Diez-Tejedor, E., &amp;amp; Trouillas, P. (1998). Randomised double-blind placebo-controlled trial of thrombolytic therapy with intravenous alteplase in acute ischaemic stroke (ECASS II). The Lancet, 352(9136), 1245-1251.&lt;br/&gt;Halpern, N. A., &amp;amp; Pastores, S. M. (2010). Critical care medicine in the United States 2000–2005: an analysis of bed numbers, occupancy rates, payer mix, and costs. Critical care medicine, 38(1), 65-71.&lt;br/&gt;Hashmi, A., Ibrahim-Zada, I., Rhee, P., Aziz, H., Fain, M. J., Friese, R. S., &amp;amp; Joseph, B. (2014). Predictors of mortality in geriatric trauma patients: a systematic review and meta-analysis. Journal of Trauma and Acute Care Surgery, 76(3), 894-901.&lt;br/&gt;Healy, S., &amp;amp; Tyrrell, M. (2011). Stress in emergency departments: experiences of nurses and doctors. Emergency nurse, 19(4).&lt;br/&gt;Herring, A. A., Ginde, A. A., Fahimi, J., Alter, H. J., Maselli, J. H., Espinola, J. A., Sullivan, A. F., &amp;amp; Camargo Jr, C. A. (2013). Increasing critical care admissions from US emergency departments, 2001–2009. Critical care medicine, 41(5), 1197.&lt;br/&gt;Jeng, J. S., Lee, T. K., Chang, Y. C., Huang, Z. S., Ng, S. K., Chen, R. C., &amp;amp; Yip, P. K. (1998). Subtypes and case-fatality rates of stroke: A hospital-based stroke registry in Taiwan (SCAN-IV). Journal of the neurological sciences, 156(2), 220-226.&lt;br/&gt;Joint Commission on Accreditation of Healthcare Organizations (2006). Meeting the Joint Commission's 2007 National Patient Safety Goals. Oakbrook Terrace, IL: Joint Commission on Accreditation of Healthcare Organizations.&lt;br/&gt;Jung, S., Jung, C., Bae, Y. J., Choi, B. S., Kim, J. H., Lee, S. H., Chang, J. Y., Kim, B. J., Han, M. K., Bae, H. J., Kwon, B. J., &amp;amp; Cha, S. H. (2016). A comparison between mechanical thrombectomy and intra-arterial fibrinolysis in acute basilar artery occlusion: single center experiences. Journal of stroke, 18(2), 211.&lt;br/&gt;Kellermann, A. L. (2006). Crisis in the emergency department. New England Journal of Medicine, 355(13), 1300-1303.&lt;br/&gt;Levy, M. M., Evans, L. E., &amp;amp; Rhodes, A. (2018). The surviving sepsis campaign bundle: 2018 update. Intensive care medicine, 44(6), 925-928.&lt;br/&gt;Li, C. H., Khor, G. T., Chen, C. H., Huang, P., &amp;amp; Lin, R. T. (2008). Potential risk and protective factors for in-hospital mortality in hyperacute ischemic stroke patients. The Kaohsiung journal of medical sciences, 24(4), 190-196.&lt;br/&gt;McDermott, F. T., Cordner, S. M., Cooper, D. J., Winship, V. C., &amp;amp; Consultative Committee on Road Traffic Fatalities in Victoria. (2007). Management deficiencies and death preventability of road traffic fatalities before and after a new trauma care system in Victoria, Australia. Journal of Trauma and Acute Care Surgery, 63(2), 331-338.&lt;br/&gt;Mendonça, E. A. (2004). Clinical decision support systems: perspectives in dentistry. Journal of dental education, 68(6), 589-597.&lt;br/&gt;Mento, A. J., Martinelli, P., &amp;amp; Jones, R. M. (1999). Mind mapping in executive education: applications and outcomes. Journal of Management Development, 18(4), 390-416.&lt;br/&gt;Michael, L. N. (2011). National Trauma Data Bank Annual Report 2011. Chicago, IL: American College of Surgeons. 5-6.&lt;br/&gt;Pinto, D. S., Kirtane, A. J., Nallamothu, B. K., Murphy, S. A., Cohen, D. J., Laham, R. J., Cutlip, D. E., Bates, E. R., Frederick,  P. D., Miller, D. P., CarrozzaJr, J. P., Antman, E. M., Cannon, C. P., &amp;amp; Gibson, C. M. (2006). Hospital Delays in Reperfusion for ST-Elevation Myocardial Infarction Implications When Selecting a Reperfusion Strategy. Circulation, 114(19), 2019-2025.&lt;br/&gt;Pitts, S. R., Pines, J. M., Handrigan, M. T., &amp;amp; Kellermann, A. L. (2012). National trends in emergency department occupancy, 2001 to 2008: effect of inpatient admissions versus emergency department practice intensity. Annals of emergency medicine, 60(6), 679-686.&lt;br/&gt;Quaddus, M., &amp;amp; Xu, J. (2005). Adoption and diffusion of knowledge management systems: field studies of factors and variables. Knowledge-based systems, 18(2-3), 107-115.&lt;br/&gt;Rhodes, A., Evans, L. E., Alhazzani, W., Levy, M. M., Antonelli, M., Ferrer, R., Kumar, A., Sevransky, J. E., Sprung, C. L., Nunnally, M. E., Rochwerg, B., Rubenfeld, G. D., Angus, D. C., Annane, D., Beale, R. J., Bellinghan, G. J., Bernard, G. R., Chiche, J. D., Coopersmith, C., De Backer, D. P., French, C. J., Fujishima, S., Gerlach, H., Hidalgo, J. L., Hollenberg, S. M., Jones, A. E., Karnad, D. R., Kleinpell, R. M., Koh, Y., Lisboa, T. C., Machado, F. R., Marini, J. J., Marshall, J. C., Mazuski, J. E., McIntyre, L. A., McLean, A. S., Mehta, S., Moreno, R. P., Myburgh, J., Navalesi, P., Nishida, O., Osborn, T. M., Perner, A., Plunkett, C. M., Ranieri, M., Schorr, C. A., Seckel, M. A., Seymour, C. W., Shieh, L., Shukri, K. A., Simpson, S. Q., Singer, M., Thompson, B. T., Townsend, S. R., Van der Poll, T., Vincent, J. L., Wiersinga, W. J., Zimmerman, J. L., &amp;amp; Dellinger, R. P. (2017). Surviving sepsis campaign: international guidelines for management of sepsis and septic shock: 2016. Intensive care medicine, 43(3), 304-377.&lt;br/&gt;Richardson D. B. (2006). Increase in patient mortality at 10 days associated with emergency department overcrowding. Medicine Journal of Australia, 184(5), 213-216.&lt;br/&gt;Russell, J. A. (2006). Management of sepsis. New England Journal of Medicine, 355(16), 1699-1713.&lt;br/&gt;Singer, M., Deutschman, C. S., Seymour, C. W., Shankar-Hari, M., Annane, D., Bauer, M., Bellomo, R., Bernard, G. R., Chiche, J. D., Coopersmith, C. M., Hotchkiss, R. S., Levy, M. M., Marshall, J. C., Martin, G. S., Opal, S. M., Rubenfeld, G. D., van der Poll, T., Vincent, J. L., &amp;amp; Angus, D. C. (2016). The third international consensus definitions for sepsis and septic shock (sepsis-3). Jama, 315(8), 801-810.&lt;br/&gt;Spencer, J. R., Anderson, K. M., &amp;amp; Ellis, K. K. (2013). Radiant thinking and the use of the mind map in nurse practitioner education. Journal of Nursing Education, 52(5), 291-293.&lt;br/&gt;Sprivulis, P.C., Da Silva, J.A., Jacobs, I.G., Frazer, A.R.L., &amp;amp; Jelinek, G.A. (2006). The association between hospital overcrowding and mortality among patients admitted via Western Australian emergency departments. Medical Journal of Australia, 184(5), 208-212.&lt;br/&gt;The European Ad Hoc Consensus Group. (1997). Optimizing Intensive Care in Stroke: A European Perspective. A Report of an Ad Hoc Consensus Group Meeting. Cerebrovascular Diseases, 7(2), 113-128.&lt;br/&gt;The National Institute of Neurological Disorders and Stroke rt-PA Stroke Study Group. (1995). Tissue plasminogen activator for acute ischemic stroke. New England Journal of Medicine, 333(24), 1581-1587.&lt;br/&gt;Tiwana, A. (2002). The knowledge management toolkit: orchestrating IT, strategy, and knowledge platforms. Pearson Education India.&lt;br/&gt;Troltsch, R., &amp;amp; Arand, M. (2013). Polytrauma–Klinisches Management in Schockraum und OP. Lege artis-Das Magazin zur ärztlichen Weiterbildung, 3(03), 162-164.&lt;br/&gt;Trzeciak, S., &amp;amp; Rivers, E. P. (2003). Emergency department overcrowding in the United States: an emerging threat to patient safety and public health. Emergency medicine journal, 20(5), 402-405.&lt;br/&gt;Von Krogh, G., Ichijo, K., &amp;amp; Nonaka, I. (2000). Enabling knowledge creation: How to unlock the mystery of tacit knowledge and release the power of innovation. Madison Avenue, NY: Oxford University Press.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;中文文獻&lt;br/&gt;方宜珊、黃國石（民104）。圖解基本護理學。臺北市：五南書局。&lt;br/&gt;吳仁和、林信惠（民106）。系統分析與設計—理論與實務應用(第七版)。台北市：智勝。&lt;br/&gt;吳柏勳、郭嘉琪（民105）。「急」刻救援－急性腦中風病人面臨施打rt-PA的急診護理經驗。澄清醫護管理雜誌，12(1)，61-72。&lt;br/&gt;吳國江（民93）。應用心智管理軟體在生活科技之教學。生活科技教育月刊，37(2)，48-58。&lt;br/&gt;謝玲芬、王麗幸（民94）。知識管理資訊系統評估模式之建構。中華管理學報，23-33。&lt;br/&gt;李欣蓉譯（民94）。圖像化學習:在不同課程領域使用圖像組織Graphic Organizers。（原作者Bromley, K., Irwin-De Vitis, L., &amp;amp; Modlo, M.）。臺北市：遠流。(原著出版年：1995年)&lt;br/&gt;劉京偉譯（民89）。知識管理的第一本書。（原作者Arthur Andersen Business Consulting）。臺北市：商周。(原著出版年：1996年)&lt;br/&gt;李建瑩、施宏哲（民104）。敗血症之血流動力學治療。藥學雜誌，31(1)，76-81。&lt;br/&gt;周中興（民106）。靜脈血栓溶解劑治療缺血性腦中風之限制與突破。腦中風會訊，24(1)，7-10。&lt;br/&gt;林少琳（民98）。血行力學之支持治療－輸液治療、升壓劑及強心劑。重症醫學雜誌，10(1)，21-26。&lt;br/&gt;林世崇、呂炎原、徐漢仲（民102）。心肌梗塞之重新定義與臨床分類。內科學誌，24(1)，1-11。&lt;br/&gt;林東清（民98）。知識管理。台北市：智勝。&lt;br/&gt;林玫君（民104）。活用心智圖：基本護理快學通。臺北市：華杏。&lt;br/&gt;林芳如、黃勝堅、吳春桂、黃美玲、林亞陵、蘇玲華、蔡紋苓、林宏茂等人（民99）。重症生命末期無效醫療之探討。中華民國急救加護醫學會雜誌，21(S)，1-8。&lt;br/&gt;林珊如（民90）。企業環境、資訊使用與知識管理。圖書資訊學刊，(16)，101-115。&lt;br/&gt;林浚仁、林永煬（民106）。急性梗塞性腦中風動脈內取栓術－最新發展與未來展望。腦中風會訊，24(1)，11-13。&lt;br/&gt;林登圳、謝佳玲、曾恿娟、林青慧（民93）。台中市事故傷害防制推動概況。台灣醫界，47(8)。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22098NTU05522004%22.&amp;amp;searchmode=basic" target="_blank"&gt;邱千慈（民99）。某醫學中心臨床決策支援系統對重複用藥之影響。國立臺灣大學臨床藥學研究所碩士論文，未出版，台北市。&lt;/a&gt;&lt;br/&gt;哈多吉（民102）。利用健保資料探討送醫層級及轉診模式與急重症病患預後之相關性--以重大創傷以及急性心肌梗塞病患為例。國立臺灣大學健康政策與管理研究所學位論文，未出版，台北市。&lt;br/&gt;哈多吉（民102）。創傷嚴重度指標計算方式之比較－國內外文獻回顧。財團法人中華緊急救護技術員協會醫誌，3(2)，25-31。&lt;br/&gt;胡瑋珊譯（民88）。知識管理。（原作者Thomas H. Davenport &amp;amp; Laurence Prusak）。新北市：中國生產力中心。(原著出版年：1998年)&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22100TIT05677001%22.&amp;amp;searchmode=basic" target="_blank"&gt;范薰月（民99）。數位心智圖教學運用於高職學生英文字彙記憶之研究。國立臺北科技大學技術及職業教育研究所碩士論文，未出版，台北市。&lt;/a&gt;&lt;br/&gt;孫志彬、杜政欣（民98）。應用本體論發展產品設計知識庫－開發手機設計知識庫為例。機械技師學刊，2(4)，46-51。&lt;br/&gt;孫志麟（民92）。教師專業成長的另類途徑：知識管理的觀點。國立臺北市師範學院學報，16(1)，229-251。&lt;br/&gt;孫易新（民103）。心智圖法理論與應用。新北市：商周出版。&lt;br/&gt;孫易新（民104）。案例解析！超高效心智圖法入門：輕鬆學會用心智圖作學習筆記、工作管理、提升記憶和創意發想。新北市：商周出版。&lt;br/&gt;崔祐堃（民105）。急性缺血性腦中風動脈內取栓治療-簡介、現況、與展望。腦中風會訊，23(3)，11-14。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22104DYU00030010%22.&amp;amp;searchmode=basic" target="_blank"&gt;張文淵（民105）。心智圖教學法融入國小自然領域教學對學習態度與學習成效之研究。大葉大學工業工程與管理學系碩士論文，未出版，彰化縣。&lt;/a&gt;&lt;br/&gt;張文蕙、許麗齡（民101）。糖尿病足部檢查實務創作。護理雜誌，59(6)，98-103。&lt;br/&gt;張吉成、周談輝（民93）。知識管理與創新。新北市：全華圖書。&lt;br/&gt;張敏、林璟淑、張元玫、李亭亭（民97）。護理資訊應用簡介－某醫院護理資訊系統推行之經驗分享。護理雜誌，55(3)，75-80。&lt;br/&gt;張寓智、劉祥仁、陳俊榮、胡漢華、葉炳強、邱德發等人（民97）。急性缺血性腦中風之一般處理原則指引。Acta Neurologica Taiwanica，17(4)，275-294。&lt;br/&gt;曹祐慈、林少琳（民98）。皮質類固醇與活化蛋白質C在敗血症之臨床應用。重症醫學雜誌，10(1)，27-35。&lt;br/&gt;梁亞文、蔡哲宏、陳文意（民100）。非緊急急診病人特性及其相關因素探討。台灣公共衛生雜誌，30(5)，505-516。&lt;br/&gt;郭金玉、陳麗娜、孫紅（民104）。臨床決策支援系統在急診診療護理中的應用。中國護理管理，15(8)，988-990。&lt;br/&gt;陳永隆、莊宜昌（民94）。知識價值鏈（更新版）。台北市：中國生產力中心。&lt;br/&gt;陳安芝（民101）。經驗分享：rt-PA的「鐘點戰」。腦中風會訊，19(1)，8-9。&lt;br/&gt;陳秀枝（民98）。與國際接軌－談台灣護理資訊現況與發展。護理雜誌，56(3)，5-11。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22095CHPI0392012%22.&amp;amp;searchmode=basic" target="_blank"&gt;陳明義（民96）。急診室醫療品質指標資訊系統建置與應用。中華大學資訊工程學系碩士班碩士論文，未出版，新竹市。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22095YM005798002%22.&amp;amp;searchmode=basic" target="_blank"&gt;陳威龍（民96）。以心律變異度預測急診室敗血症病人是否發生敗血性休克。陽明大學醫學院急重症醫學研究所碩士論文，未出版，台北市。&lt;/a&gt;&lt;br/&gt;陳家聲、方文昌、蔡儀華（民94）。企業員工知識分享效能之質性研究－以知識接收者的觀點。人力資源管理學報，5(1)，29-51。&lt;br/&gt;陳素宜、孫易新譯（民96）。心智魔法師：大腦使用手冊Use your Head。（原作者Tony Buzan）。臺北縣：耶魯國際文化。(原著出版於年：2003)&lt;br/&gt;陳瑞杰（民101）。重大外傷病人照護。醫療品質雜誌，6(4)，19-23。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22104YUNT0615036%22.&amp;amp;searchmode=basic" target="_blank"&gt;黃郁修（民105）。心智圖教學對中學生英文閱讀理解和學習態度的影響。國立雲林科技大學應用外語系碩士論文，未出版，雲林縣。&lt;/a&gt;&lt;br/&gt;黃素雲、洪慧娟、蔡崇煌、王素美、胡蓮珍（民104）。心智圖軟體在醫護教育的應用。澄清醫護管理雜誌，11(2)，30-38。&lt;br/&gt;劉美玲、楊秋菊（民97）。一位急性心肌梗塞併發心因性休克病人之加護護理經驗。長庚護理，19(2)，274-283。&lt;br/&gt;劉蘊芳譯（民88）。7 Brains－怎樣擁有達文西的七種天才How to think like Leonardo da Vinci: Seven steps to genius every day。（原作者Michael J. Gelb）。臺北市：大塊文化。(原著出版年：1998年)&lt;br/&gt;蔡啟達（民104）。圖解教育學。台北市：五南。&lt;br/&gt;鄭玉琳、林梅芳、蔡斌智（民97）。嚴重敗血症治療概論。藥學雜誌，24(3)，31-36。&lt;br/&gt;鄭建興（民96）。2006年重要的腦中風相關臨床試驗。Acta Neurologica Taiwanica，16(2)，111-120。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22090NTPTC284003%22.&amp;amp;searchmode=basic" target="_blank"&gt;錢秀梅（民90）。心智圖教學方案對身心障礙資源班學生創造力影響之研究。國立台北師範學院國民教育研究所特殊教育教學碩士論文，未出版，台北市。&lt;/a&gt;&lt;br/&gt;謝孟倉（民107年）。急性梗塞性腦中風取栓術與血壓控制。腦中風會訊，25(2)，12-13。&lt;br/&gt;謝恬、阮明淑（民95）。台灣知識管理系統比較分析初探。教育資料與圖書館學，43(4)，487-508。&lt;br/&gt;鍾月枝、鄭高珍（民99）。加護病房中長期醫療資源使用和死亡率分析。醫務管理期刊，11(1)，33-44。&lt;br/&gt;蘇麗智、簡淑真、劉波兒、蘇惠珍、林靜娟、呂麗卿、陳明莉、羅筱芬、李淑俐、林淑燕、賴秋絨、邱淑玲、陳淑齡、謝珮琳、林玉惠、黃月芳、葉秀珍、李家琦、李美雲、歐倫君（民100）。實用基本護理學(上冊)(第七版)。臺北市：華杏。&lt;br/&gt;龔文亮（民95）。個人化智慧型健檢決策支援系統。政治大學資訊管理研究所學位論文，未出版，台北市。 ‎&lt;br/&gt;&lt;br/&gt;網路文獻&lt;br/&gt;台灣急診醫學會（民101）。急診五級檢傷分類標準及增修內容。民105年05月18日，取自：https://www.sem.org.tw/tsem../files/boardMsg/00000907.pdf&lt;br/&gt;台灣急診醫學會（民101）。急診檢傷目的與發展五級檢傷的歷程。民105年05月18日，取自：http://www.sem.org.tw/tsem/download/?fID=00000908&amp;amp;k=news&lt;br/&gt;台灣急診醫學會（民104）。公告寄發各急救責任醫院『台灣急診檢傷及急迫度量表』單機版光碟。民105年12月27日，取自：http://www.sem.org.tw/tsem../?doActionValueID=1531&amp;amp;menuID=1179069063&amp;amp;doAction=detail#none&lt;br/&gt;台灣腦中風學會（民102年09月12日）。靜脈血栓溶解劑治療急性缺血性腦中風指引。民106年04月11日，取自：https://www.stroke.org.tw/GoWeb2/include/pdf/07%20guideline_002.pdf&lt;br/&gt;行政院公報資訊網（民94年07月21日）。預告廢止本部「機器腳踏車駕駛人及附載座人戴安全帽實施及宣導辦法」【公告】。臺北市：交通部。民108年05月12日，取自：https://gazette.nat.gov.tw/EG_FileManager/eguploadpub/eg011140/ch06/type3/gov50/num2/Eg.htm&lt;br/&gt;吳博儒（無日期）。iStroke 中風臨床決策支援系統。105年12月25日，取自：https://www.itri.org.tw/chi/Content/MSGPic01/contents.aspx?&amp;amp;SiteID=1&amp;amp;MmmID=620605426112545320&amp;amp;CatID=620613176371050363&amp;amp;MSID=654720264343447472&lt;br/&gt;吳碧娥（民104年05月20日）。推動智慧醫療解放醫護人力 別讓台灣淪為「血汗醫院」。北美智權報。105年12月21日，取自：http://www.naipo.com/Portals/1/web_tw/Knowledge_Center/Industry_Economy/publish-372.htm&lt;br/&gt;吳靜美（民97年01月15日）。心肌梗塞奪命一瞬間。好健康會刊，3。民108年05月12日，取自：https://www.twhealth.org.tw/journalView.php?cat=22&amp;amp;sid=370&amp;amp;page=6&lt;br/&gt;林口長庚紀念醫院外傷急重症中心（民104年07月31日）。林口長庚紀念醫院外傷年報。民105年11月08日，取自：https://www1.cgmh.org.tw/intr/intr2/c3290/traumareport103.pdf&lt;br/&gt;林怡廷（民106年08月15日）。世界第一的急診 為何出現四大亂象。天下雜誌，629。民108年05月18日，取自：https://www.cw.com.tw/article/article.action?id=5084419&lt;br/&gt;邱玉珍（民105年10月15日）。細菌感染勿輕忽 小心敗血症的威脅。好健康會刊，38。民108年05月12日，取自：https://www.twhealth.org.tw/journalView.php?cat=7&amp;amp;sid=114&amp;amp;page=1&lt;br/&gt;徐展鵬、鍾睿元、陳威龍、陳健驊（民107年02月26日）。敗血症新指南下，急診醫師必需改變的醫療措施。台灣急診醫學通訊，1。民108年05月11日，取自：https://www.sem.org.tw/EJournal/Detail/7&lt;br/&gt;殷偉賢（民103年09月23日）。心肌梗塞 打通血管不能拖。聯合新聞網。民105年12月13日，取自：http://health.udn.com/health/story/5977/368208&lt;br/&gt;缺血性腦中風指引2013。民108年04月26日，取自：https://www.stroke.org.tw/GoWeb2/include/pdf/07%20guideline_002.pdf&lt;br/&gt;張雅雯（民107年04月15日）。高血壓標準趨嚴 如何避免血壓「高人一等」。好健康會刊，44。民108年04月23日，取自：https://www.twhealth.org.tw/journalView.php?cat=1&amp;amp;sid=3&amp;amp;page=1&lt;br/&gt;許超群（民103年）。敗血性休克－可能快速惡化並危及生命的醫療急症。105年12月17日，取自：http://www.kmuh.org.tw/www/kmcj/data/10301/8.htm&lt;br/&gt;許碩穎（民103年12月15日）。急診室暴力頻傳　醫：「急診」非快速門診。健康醫療網。民105年12月26日，取自：http://www.healthnews.com.tw/index.php/news/article/18684/%E6%80%A5%E8%A8%BA%E5%AE%A4%E6%9A%B4%E5%8A%9B%E9%A0%BB%E5%82%B3%e3%80%80%E9%86%AB%E6%80%A5%E8%A8%BA%E9%9D%9E%E5%BF%AB%E9%80%9F%E9%96%80%E8%A8%BA/?keyword=E680A5E8A8BAE6AAA2E582B7&lt;br/&gt;陳文鍾、馬惠明、石崇良、方震中、蔡光超、林子忻、蔡力凱、許瓊元、張維典（民98）。建立台灣地區急傷重症病患到院前救護及急診醫療臨床路徑標準作業流程與品質管理指標研究。行政院衛生署九十七年度委託科技研究計劃研究報告。民105年12月15日，取自政府研究資訊系統GRB網頁： http://grbsearch.stpi.narl.org.tw/search/planDetail?id=1571729&amp;amp;docId=0&lt;br/&gt;陳芳毓（民105年07月06日）。工作愈複雜，愈要提升思考力！6步驟學會心智圖思考法。經理人月刊。民105年12月13日，取自：https://www.managertoday.com.tw/articles/view/2575&lt;br/&gt;黃秋峰（民97）。活化型蛋白質C對於敗血症治療的臨床應用。長庚校訊，70。民105年12月17日，取自：http://enews.cgu.edu.tw/files/15-1068-43461,c7440-1.php?Lang=zh-tw&lt;br/&gt;新光醫療財團法人新光吳火獅紀念醫院（民101）。冠狀動脈氣球擴張術。新光醫院20週年杏林常新特刊：健康QR code。民105年12月15日，取自：http://www.skh.org.tw/information/20years.pdf&lt;br/&gt;嘉義基督教醫院（民100）。AMI小組 掌握黃金90分鐘搶救心肌梗塞病患。民105年12月13日，取自：http://www.cych.org.tw/cychweb/cych2/messenger_show.aspx?p_id=643&lt;br/&gt;臺安醫院（民102年06月01日）。淺談冠狀動脈疾病。民105年12月13日，取自：http://www.tahsda.org.tw/newsletters/?p=2809&lt;br/&gt;衛生福利部（民104年03月24日）。有關社會大眾關心健保實施20年醫療支出及醫療品質議題、醫護人力問題以及在少子女化及高齡化趨勢下，健保財務問題等之說明。民105年12月22日，取自：http://www.mohw.gov.tw/cp-16-20866-1.html&lt;br/&gt;衛生福利部（民106年01月17日）。急性缺血性中風，健保增列t-PA治療處置給付。民108年07月22日，取自：https://www.mohw.gov.tw/cp-2621-568-1.html&lt;br/&gt;衛生福利部（民97年09月11日）。騎車環保又健身 安全注意不能少。民108年05月12日，取自：https://www.mohw.gov.tw/fp-3163-28229-1.html&lt;br/&gt;衛生福利部中央健康保險署（民104年05月25日）。修正_2014年版_ICD-10-CM-PCS_全民健康保險急診品質提升方案(104.05.25公告新增)。臺北市：衛生福利部。民105年11月08日，取自：https://www.nhi.gov.tw/Resource/bulletin/5759_1040005319-7[1].pdf&lt;br/&gt;衛生福利部中央健康保險署（民105年02月26日）。多管齊下提升急診醫療照護適當性，盼各界攜手同努力。民105年11月14日，取自：https://www.mohw.gov.tw/cp-2624-19541-1.html&lt;br/&gt;衛生福利部中央健康保險署（民105年03月16日）。重大傷病證明卡申請與換發注意事項。民105年12月16日，取自：http://www.nhi.gov.tw/webdata/webdata.aspx?menu=20&amp;amp;menu_id=712&amp;amp;webdata_id=406&lt;br/&gt;衛生福利部中央健康保險署（民106年04月14日）。推動分級醫療，落實雙向轉診，健保署邀醫界、民眾齊努力。民108年05月17日，取自：https://www.nhi.gov.tw/News_Content.aspx?n=FC05EB85BD57C709&amp;amp;s=1AB48E2FDC1545B6&lt;br/&gt;衛生福利部中央健康保險署（民107年09月27日）。公告修訂含 rt-PA（如Actilyse ）成分藥品之藥品給付規定【公告】。台北市：衛生福利部。民108年07月28日，取自：https://www.nhi.gov.tw/BBS_Detail.aspx?n=F362D4AAE872CDDE&amp;amp;sms=D6D5367550F18590&amp;amp;s=F7B104025FF203BC&lt;br/&gt;衛生福利部中央健康保險署（民107年12月22日）。精進急診重大疾病品質，急診效率再提升，各界攜手齊努力。民108年07月18日，取自：https://www.nhi.gov.tw/News_Content.aspx?n=FC05EB85BD57C709&amp;amp;s=6A86BFCDA357D618&lt;br/&gt;衛生福利部中央健康保險署（民108年01月25日）。全民健康保險急診品質提升方案(108.02.01起修正)-劃線版。臺北市：衛生福利部。民108年03月22日，取自：https://www.nhi.gov.tw/Content_List.aspx?n=D496152DDA8646D0&amp;amp;topn=D39E2B72B0BDFA15&lt;br/&gt;衛生福利部中央健康保險署（民108年07月03日）。醫療服務給付項目及支付標準網路查詢服務-急性缺血性腦中風處置費。民108年07月25日，取自：https://www.nhi.gov.tw/query/Query2_Detail.aspx?Ser_id=6056&lt;br/&gt;衛生福利部中央健康保險署（民108年07月03日）。醫療服務給付項目及支付標準網路查詢服務-急性缺血性腦中風機械取栓術。民108年07月28日，取自：https://www.nhi.gov.tw/query/Query2_Detail.aspx?Ser_id=5092&lt;br/&gt;衛生福利部中央健康保險署（民108年07月12日）。厝邊好醫師 社區好醫院。民108年07月28日，取自：https://www.nhi.gov.tw/Content_List.aspx?n=77E733B4D7F423AC&amp;amp;topn=0B69A546F5DF84DC&lt;br/&gt;衛生福利部中央健康保險署（民95年06月06日）。正確量測體溫方法。民105年12月06日，取自：http://www.nhi.gov.tw/webdata/webdata.aspx?menu=6&amp;amp;menu_id=168&amp;amp;webdata_id=1548&lt;br/&gt;衛生福利部中央健康保險署（民97年07月30日）。運用創傷嚴重程度分數(Injury Severity Score, ISS)評估創傷嚴重程度(97.07.30更新)。臺北市：衛生福利部。民105年04月11日，取自：https://www.nhi.gov.tw/Content_List.aspx?n=3AE7F036072F88AF&amp;amp;topn=D39E2B72B0BDFA15&lt;br/&gt;衛生福利部全民健康保險會（民107年07月25日）。106年全民健康保險年度監測結果報告書。民108年07月28日，取自：https://dep.mohw.gov.tw/NHIC/lp-3531-116.html&lt;br/&gt;衛生福利部全民健康保險會（民108年07月01日）。107年全民健康保險會年報。民108年07月28日，取自：https://dep.mohw.gov.tw/NHIC/cp-1660-48267-116.html&lt;br/&gt;衛生福利部國民健康署（民107年10月16日）。搶救腦中風 謹記「臨微不亂」。民108年07月18日，取自：https://www.hpa.gov.tw/Pages/Detail.aspx?nodeid=1405&amp;amp;pid=9644&lt;br/&gt;衛生福利部國民健康署（民93年03月）。高血壓防治手冊--高血壓偵測、控制與治療流程指引。民105年12月12日，取自：https://health99.hpa.gov.tw/media/public/pdf/21446.pdf&lt;br/&gt;衛生福利部國民健康署（民95年06月19日）。92-94年腦中風防治計畫研究成果。民108年05月14日，取自：https://www.hpa.gov.tw/Pages/Detail.aspx?nodeid=631&amp;amp;pid=1186&lt;br/&gt;衛生福利部統計處（民102年06月17日）。台灣死因統計自動化基本介紹。民108年06月19日，取自：https://dep.mohw.gov.tw/DOS/lp-2542-113.html&lt;br/&gt;衛生福利部統計處（民103年12月27日）。102年度全民健康保險醫療統計年報。民107年12月27日，取自：https://dep.mohw.gov.tw/DOS/np-1965-113.html&lt;br/&gt;衛生福利部統計處（民105年05月20日）。103年度全民健康保險醫療統計年報。民106年07月25日，取自：https://dep.mohw.gov.tw/DOS/np-1941-113.html&lt;br/&gt;衛生福利部統計處（民106年01月17日）。104年度全民健康保險醫療統計年報。民106年07月25日，取自：https://dep.mohw.gov.tw/DOS/np-1919-113.html&lt;br/&gt;衛生福利部統計處（民106年12月28日）。105年度全民健康保險醫療統計年報。民107年10月13日，取自：https://dep.mohw.gov.tw/DOS/np-3717-113.html&lt;br/&gt;衛生福利部統計處（民107年09月10日）。106年死因統計年報電子書。民108年06月18日，取自：https://dep.mohw.gov.tw/DOS/cp-3960-43792-113.html&lt;br/&gt;衛生福利部統計處（民107年12月26日）。106年度全民健康保險醫療統計年報。民107年12月27日，取自：https://dep.mohw.gov.tw/DOS/np-4267-113.html&lt;br/&gt;衛生福利部統計處（民108年01月24日）。106年死因統計年報。民108年03月22日，取自：https://dep.mohw.gov.tw/DOS/cp-3960-42867-113.html&lt;br/&gt;衛生福利部統計處（民108年06月21日）。107年死因記者會簡報。民108年06月23日，取自：https://dep.mohw.gov.tw/DOS/lp-4472-113.html&lt;br/&gt;衛生福利部統計處（民108年06月21日）。107年死因結果摘要表。民108年06月23日，取自：https://dep.mohw.gov.tw/DOS/cp-4472-48035-113.html&lt;br/&gt;衛生福利部醫事司（民106年11月01日）。公告修正急診五級檢傷分類基準(105.1.1施行)【公告】。台北市：衛生福利部。民108年07月22日，取自：https://dep.mohw.gov.tw/DOMA/cp-2710-38118-106.html&lt;br/&gt;衛生福利部醫事司（民107年04月11日）。107年度醫院緊急醫療能力分級評定基準及評分說明與評量方法。民107年10月14日，取自：https://dep.mohw.gov.tw/doma/cp-984-40677-106.html&lt;br/&gt;衛生福利部醫事司（民107年11月09日）。公告修正急診五級檢傷分類基準(總表-表六及兒童版)(107.5.1施行)【公告】。台北市：衛生福利部。民108年03月24日，取自：https://dep.mohw.gov.tw/DOMA/cp-2710-40920-106.html&lt;br/&gt;衛生福利部醫事司（民108年07月05日）。公告修正急診五級檢傷分類基準(成人非外傷)(108.6.11施行)【公告】。台北市：衛生福利部。民108年07月22日，取自：https://dep.mohw.gov.tw/DOMA/cp-2710-48412-106.html&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
+      <c r="Z7" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/gm677n</t>
         </is>
@@ -1463,35 +1451,34 @@
           <t>big data、medical indicators、performance、big data information systems</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>點閱:262</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>點閱:260</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
         <is>
           <t xml:space="preserve">
 資訊科技已經明顯的改變現代人的觀念並創造新的生活習慣。隨著時代快速的變遷，網路時代發達，民眾對於醫療照護品質觀念也跟著改變，高品質的醫療服務已成為民眾的就醫基本共識，使得不論是醫療院所或是長照機構經營更加的困難。如何提升經營績效指標且持續更新，不僅在有更好的效率更有助於及早除錯、即時修正，還可以避免沿用錯誤的資料影響決策規劃。績效管理的最終目的是提高生產率和效率，可以讓高階主管專注在自己業務不需耗費人工時間審核資料數據內容。本研究主要利用大數據視覺化系統因應醫療機構高階主管資訊系統之經營指標數據為例。大數據被認為是未來技術最重要的領域之一，且正在迅速引起許多行業的關注，因它可以為企業提供高價值的決策來源。這些發現促使研究人員和管理人員能夠同時了解大數據技術可以為公司帶來的最大潛在收益，並採取相對應行動，從最大限度提高投資回報率，並從大數據中獲取高價值，這是一舉數得的行動。本研究採取專家問卷，問卷受測者為機構負責人及醫療機構績效組主管，醫療機構涵蓋範圍較廣相較於長照機構較為複雜，但對於利用大數據系統呈現數據方式對於高階主管而言，不論是醫療機構或是長照機構，都可以隨時掌握機構內部之營運狀況，除此之外也能縮短人工作業時間及錯誤率，利用資訊系統不儘可以加快醫療機構經營指標的分析也能加快高階主管進行決策。主管資訊系統在管理上除了可以提供高階主管及機構負責人有較佳的管控功能之外，對於醫療評鑑資料蒐集方面也能快速完成。經過第一次專家訪談及第二次專家驗證後，將經營績效指標問卷分為五大項中分為五個細項，結果顯示依據醫療機構與長照機構經營績效指標上差異相當大，雖然同為醫療產業，經營指標與管理指標所注重程度較為不同，在二十五項細項指標中只有三項相同指標，其他二十二項為差異項，從中得知同為醫療產業但經營管理層面有相當大差異性。</t>
         </is>
       </c>
-      <c r="Z8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 中文參考文獻&lt;br/&gt;36大數據(民國104年3月18日)。盤點55個最實用的大數據可視化分析工具。民國104年3月18日，取自： http://www.36dsj.com/archives/24173。&lt;br/&gt;王美慧、陳瑞龍、林憬、江克儉(民94)。醫院績效衡量之研究-以花蓮某區域醫院為例。顧客滿意學刊，1(2)，107-130。&lt;br/&gt;朱正一(民95)。醫務管理:制度,組織與實務。華泰文化事業股份有限公司。&lt;br/&gt;阮玉梅(民88)。長期照護。國立空中大學，未出版，新北市。&lt;br/&gt;段伴虬、溫育慧(民105)。 長期照護機構經營管理成功關鍵因素之探討-以南投縣某機構為例。福祉科技與服務管理學刊，4(2)，317-318。&lt;br/&gt;侯榮英、張文信、蕭智維、江宜靜(民99)。運用商業智慧系統建構視覺化會計圖表應用於醫院管理-以南部某醫院為例。醫務管理期刊，11(3)，75-87。&lt;br/&gt;吳思華(民89)。策略九說(第三版)。臺北市：臉譜出版。&lt;br/&gt;梁定澎(民92)。決策支援系統與企業智慧。智勝文化出版，臺北市。&lt;br/&gt;徐慧娟、薛亞聖(民90)。 醫院管理指標的性質與應用。Hospital，p29-41。&lt;br/&gt;孫本初、鍾京佑(民94). 治理理論之初探政府。 市場與社會治理架構。公共行政學報，(16)， 107-135。&lt;br/&gt;莊文忠(民97)。績效衡量與指標設計:方法論上的討論。公共行政學報，(29)，61-91。&lt;br/&gt;陳澤義、陳啟斌 (民95)。企業診斷與績效評估:平衡計分卡之運用。台北市:華泰。&lt;br/&gt;张挺(民94)。我国医疗机构的竞争优势和基本竞争战略。中国卫生资源，11(4)，154-155。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22095NCCU5388102%22.&amp;amp;searchmode=basic" target="_blank"&gt;陳立基(民95)。台灣地區老人安養護機構經營管理關鍵成功因素。政治大學經營管理碩士學程 (EMBA)學位論文，1-109。&lt;/a&gt;&lt;br/&gt;張明裕、梁凡偉（民95）。以 AHP 法分析線上遊戲作置入式行銷廣告模式之研究。未出版。南台科技大學，未出版，台南市。&lt;br/&gt;http://www. aea-taiwan. org/SEAIT2013/papers/IT09. pdf.&lt;br/&gt;褚志鵬(民98)。層級分析法 (AHP) 理論與實作。 國立東華大學企業管理學系 教授， 民國九十八年.&lt;br/&gt;曾郁薇 (民102)。用於發展高階主管資訊系統之改良式醫院績效評估架構。國立台北護理健康大學，未出版，台北市。&lt;br/&gt;黃昱霖、吳宗翰、林峰正、衷嵐焜(民102)。巨量資料視覺化之研究.:&lt;br/&gt;黃怡詔、簡禎富、劉志明、賴威齊、劉昕昶(民93)。建構網際網路環境下之醫院主管資訊系統及其實證研究。工業工程學刊，21(2)，101-112。&lt;br/&gt;楊鎮維、方世杰、黃維民。(民94)醫療機構經營策略與營運績效之研究: 社會性套系觀點。福爾摩莎醫務管理雜誌，1(2)，124-133。&lt;br/&gt;餘明玲、薛亞聖、黃興進(2005)。影響醫院資訊系統績效評估之關鍵因素:高階主管觀點之實證研究，台灣公共衛生雜誌,24(1)，22-32。&lt;br/&gt;廖詩漢(民105)。以 QlikView 對醫療資料庫作大數據分析-以某護理之家為例。中正大學資訊管理學系學位論文，1-118。&lt;br/&gt;劉籹君、黃興進、廖則竣 (民99)。決策支援系統使用績效之實證研究:結合任務-科技適配與資訊系統成功模式。電子商務學報，12(3)，407-430。&lt;br/&gt;賴威齊(2003)。以平衡計分卡為基礎建構網際網路環境下之醫院高階主管資訊系統及其實證研究。元培醫事科技大學，未出版，新竹市。&lt;br/&gt;蕭文(民82)。醫院管理資訊系統，台本市：書華。&lt;br/&gt;簡禎富、林鼎浩、徐紹鐘、彭誠湧(民90)。建構半導體晶圓允收測試資料挖礦架構及其實證研究。Journal of the Chinese Institute of Industrial Engineers，18(4)，37-48。&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;英文參考文獻&lt;br/&gt;Azad, M. M., Amin, M. B., &amp;amp; Alauddin, M. (2012). Executive information system. International Journal of Computer Science and Network Security (IJCSNS),12(5), 106.&lt;br/&gt;Badawy, M., El-Aziz, A. A., Idress, A. M., Hefny, H., &amp;amp; Hossam, S. (2016). A survey on exploring key performance indicators.Future Computing and Informatics Journal.&lt;br/&gt;Chow, H. W., Ling, G. J., Yen, I. Y., &amp;amp; Hwang, K. P. (2016). Building brand equity through industrial tourism. Asia Pacific Management Review.&lt;br/&gt;Chen, X., &amp;amp; Jin, R. (2017). Statistical modeling for visualization evaluation through data fusion. Applied ergonomics.&lt;br/&gt;Dess, G. G., &amp;amp; Robinson, R. B. (1984). Measuring organizational performance in the absence of objective measures: the case of the privately‐held firm and conglomerate business unit. Strategic management journal,5(3), 265-273.&lt;br/&gt;Davenport, T. (2014). Big data at work: dispelling the myths, uncovering the opportunities. harvard Business review Press.&lt;br/&gt;Eroshkin, S. Y., Kameneva, N. A., Kovkov, D. V., &amp;amp; Sukhorukov, A. I. (2017). Conceptual System in the Modern Information Management. Procedia Computer Science, 103, 609-612.&lt;br/&gt;Fernandes, B. H. R. (2006). Competências e desempenho organizacional: o que há além do Balanced Scorecard. Saraiva.&lt;br/&gt;Freeman, E., Knapp, M., &amp;amp; Somani, A. (2017). Long-term care organization and financing.&lt;br/&gt;Franková, P., Drahošová, M., &amp;amp; Balco, P. (2016). Agile Project Management Approach and its Use in Big Data Management. Procedia Computer Science, 83, 576-583.&lt;br/&gt;Gandomi, A., &amp;amp; Haider, M. (2015). Beyond the hype: Big data concepts, methods, and analytics. International Journal of Information Management, 35(2), 137-144.&lt;br/&gt;Gupta, M., &amp;amp; George, J. F. (2016). Toward the development of a big data analytics capability. Information &amp;amp; Management, 53(8), 1049-1064.&lt;br/&gt;Gong, M., Simpson, A., Koh, L., &amp;amp; Tan, K. H. (2016). Inside out: The interrelationships of sustainable performance metrics and its effect on business decision making: Theory and practice. Resources, Conservation and Recycling.&lt;br/&gt;Ivascu, M. (2016). Improving the Managerial Performance in Health Care Systems. Procedia Economics and Finance, 39, 777-784.&lt;br/&gt;Kaganski, S., Majak, J., Karjust, K., &amp;amp; Toompalu, S. (2017). Implementation of key performance indicators selection model as part of the Enterprise Analysis Model. Procedia CIRP, 63, 283-288.&lt;br/&gt;Kayyali, B., Knott, D., &amp;amp; Van Kuiken, S. (2013). The big-data revolution in US health care: Accelerating value and innovation. Mc Kinsey &amp;amp; Company, 2(8), 1-13.&lt;br/&gt;Kokangül, A., Polat, U., &amp;amp; Dağsuyu, C. (2017). A new approximation for risk assessment using the AHP and Fine Kinney methodologies. Safety science, 91, 24-32.&lt;br/&gt;Lungu, I. C. and Bara, A., "Executive Information Systems’ Multidimensional Models",&lt;br/&gt;Revista Informatica Economica,vol. 3 , no.43, 2007.&lt;br/&gt;Lukoianova, T., &amp;amp; Rubin, V. L. (2014). Veracity roadmap: Is big data objective, truthful and credible.&lt;br/&gt;Muthuveloo, R., Shanmugam, N., &amp;amp; Teoh, A. P. (2017). The impact of tacit knowledge management on organizational performance: Evidence from Malaysia. Asia Pacific Management Review.&lt;br/&gt;Pramanik, M. I., Lau, R. Y., Demirkan, H., &amp;amp; Azad, M. A. K. (2017). Smart health: Big data enabled health paradigm within smart cities. Expert Systems with Applications, 87, 370-383.&lt;br/&gt;Peral, J., Maté, A., &amp;amp; Marco, M. (2017). Application of Data Mining techniques to identify relevant Key Performance Indicators. Computer Standards &amp;amp; Interfaces, 50, 55-64.&lt;br/&gt;Parmenter, D. (2012). Key performance indicators for government and non profit agencies: implementing winning KPIs. John Wiley &amp;amp; Sons.&lt;br/&gt;Parmenter, D. (2015). Key performance indicators: developing, implementing, and using winning KPIs. John Wiley &amp;amp; Sons.&lt;br/&gt;Rockart, J.F. and Treacy, M.E., “The CEO goes on-line,” Harvard Business Review 60, 1982, pp.82-88.&lt;br/&gt;Ruan, G., &amp;amp; Zhang, H. (2017). Closed-loop Big Data Analysis with Visualization and Scalable Computing. Big Data Research, (8), 12-26.&lt;br/&gt;Raguseo, E. (2018). Big data technologies: An empirical investigation on their adoption, benefits and risks for companies. International Journal of Information Management, 38(1), 187-195.&lt;br/&gt;Seward, J. B. (2017). Paradigm Shift in Medical Data Management: Big Data and Small Data∗.&lt;br/&gt;Sagiroglu, S., &amp;amp; Sinanc, D. (2013, May). Big data: A review. In Collaboration Technologies and Systems (CTS), 2013 International Conference on (pp. 42-47). IEEE.&lt;br/&gt;Sanchez, O. P., &amp;amp; Terlizzi, M. A. (2017). Cost and time project management success factors for information systems development projects. International Journal of Project Management, 35(8), 1608-1626.&lt;br/&gt;van der Geer, E., van Tuijl, H. F., &amp;amp; Rutte, C. G. (2009). Performance management in healthcare: performance indicator development, task uncertainty, and types of performance indicators. Social science &amp;amp; medicine, 69(10), 1523-1530&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA8" t="inlineStr">
+      <c r="Z8" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/cr4zjb</t>
         </is>
@@ -1596,35 +1583,34 @@
           <t>ankylosing spondylitis、medication non- adherence</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>點閱:77</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>點閱:77</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 僵直性脊椎炎（ankylosing spondylitis）是一個自體免疫及慢性發炎關節疾病，導致脊椎關節的沾黏，伴隨脊柱關節疼痛和僵直症狀。由於脊柱附近肌腱、韌帶等軟組織發炎而造成脊柱自發性融合，形成無法彎曲的「竹節樣脊柱」。僵直性脊椎炎的主要治療方法為藥物，目標以控制病情及維持日常生活功能為主，因此，遵循醫囑規則服藥極為重要。本研究目的在了解僵直性脊椎炎未順從性服藥之相關因素。本研究於南部某區域教學醫院的過敏免疫風濕中心門診進行問卷調查，收案日期為民國2016年11月4日至2017年1月24日，有效樣本206人。藥物順性採用「藥物佔有率」（Medication Possession Ratio, MPR）作為指標，從研究對象的電子病歷回溯前二年服用（1）非類固醇抗炎止痛劑藥物、（2）生物製劑及（3）合併非類固醇抗炎止痛劑藥物和生物製劑兩種藥物的治療處方。藥物佔有率  80%以上界定為藥物順從，藥物佔有率&lt; 80% 者界定為藥物未順從。數據以羅吉斯迴歸分別分析三個藥物未順從的依變項與人口學特徵、健康狀況、脊椎X光片變化、僵直性脊椎炎疾病嚴重度和生活品質之關聯。研究結果顯示僵直性脊椎炎病患使用非類固醇抗炎止痛劑藥物的藥物佔有率為0.80、使用生物製劑的藥物佔有率為0.78、而合併非類固醇抗炎止痛劑藥物和生物製劑兩種藥物的藥物佔有率為0.76。多變項羅吉斯迴歸分析顯示：（1）在非類固醇抗炎止痛劑藥物方面，沒有規律運動者比有規律運動者呈現顯著較高風險的未順從性（勝算比 = 1.99、95%信賴區間 = 1.10–3.59、P = 0.023）、（2）在生物製劑藥物方面，身體質量指數類別為肥胖者比類別為正常和過低者呈現顯著較低風險的未順從性（勝算比 = 0.27、95%信賴區間 = 0.08–0.97、P = 0.045）、（3）在合併非類固醇抗炎止痛劑藥物和生物製劑兩者方面，沒有規律運動者比有規律運動者呈現較高風險的未順從性（勝算比 = 1.76、95%信賴區間 = 1.00–3.11、P = 0.051）。但脊椎X光片變化分級、僵直性脊椎炎疾病嚴重度和生活品質則與藥物未順從性無顯著關聯。綜合而言，本研究的僵直性脊椎炎病患，藥物佔有率未能完全達到0.80的理想標準。建議護理人員針對沒有規律運動者，加強服藥順從性的衛教。</t>
         </is>
       </c>
-      <c r="Z9" t="inlineStr">
+      <c r="Y9" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 中文：&lt;br/&gt;王政為與楊榮森（民102）。僵直性脊椎炎之診斷、治療與併發症。台灣醫學，17（6），687－694。&lt;br/&gt;何振珮與李哲夫（民103）。服藥遵從行為中文量表之信、效度測量。臺灣臨床藥學雜誌，22（2），139－147。&lt;br/&gt;何振珮、尤瑞鴻、劉采艷與李哲夫（民104）。東部某醫院影響高血壓病人服藥遵從行為因素之探討。護理暨健康照護研究，11（1），23－32。&lt;br/&gt;李智、趙藝璞與胡秀英（民105） 。多病共存與老年高血壓患者服藥不遵從行為之相關性研究。護理雜誌，63（5），65－75。&lt;br/&gt;林幸誼、陳靜雯、翁麗雀、陳瑪莉、林秀珍與余光輝（民101）。類風濕性關節炎病人服藥遵從行為與其相關因素探討。長庚護理，23（3），282－298。&lt;br/&gt;吳佳蓉、陳清惠與葉忍莉（民91）。老年患者服藥行為影響因素的探討。長庚護理雜誌，13（2），166－172。&lt;br/&gt;周昌德（民95）。關節痛與腰背痛-如何早期發現僵直性脊椎炎及乾癬關節炎。台北市：健康文化。&lt;br/&gt;周昌德（民101）。僵直性脊椎炎-臨床表徵、診斷及治療。風濕病學。台北市：合記圖書出版社。&lt;br/&gt;陳俊雄、廖顯宗、梁統華與周昌德（民97）。僵直性脊椎炎－早期認知早期治療。內科學誌，19（6），481－490。&lt;br/&gt;施維怡與詹欣隆（民106）。僵直性脊椎炎及軸心型脊椎關節炎診斷之進展。台北市醫師公會會刊，61（7），20－24。&lt;br/&gt; &lt;br/&gt;英文:&lt;br/&gt;&lt;br/&gt;Andrade, S. E., Kahler, K. H., Frech, F., &amp;amp; Chan, K. A. (2006). Methods for evaluation of medication adherence and persistence using automated databases. Pharmacoepidemiology and Drug Safety, 15(8):565–574.&lt;br/&gt;Aydin, S. Z., Can, M., Atagunduz, P., &amp;amp; Direskeneli, H. (2010). Active disease requiring TNF-alpha-antagonist therapy can be well discriminated with different ASDAS sets: a prospective, follow-up of disease activity assessment in ankylosing spondylitis. Clinical and Experimental Rheumatology, 28(5), 752–755.&lt;br/&gt;Baraliakos, X., Listing, J., Rudwaleit, M., Sieper, J., &amp;amp; Braunl, J. (2009). Development of a radiographic scoring tool for ankylosing spondylitis only based on bone formation: addition of the thoracic spine improves sensitivity to change. Arthritis Care &amp;amp; Research, 61(6), 764–771.&lt;br/&gt;Braun, J., &amp;amp; Sieper, J. (2007). Ankylosing spondylitis. Lancet, 369(9570), 1379–1390.&lt;br/&gt;Brionez, T. F., &amp;amp; Reveille, J. D. (2008). The contribution of genes outside the major histocompatibility complex to susceptibility to ankylosing spondylitis. Current Opinion in Rheumatology, 20(4):384–391.&lt;br/&gt;Chang, C. T., Hsieh, M. Y., &amp;amp; Kuo, C. F. (2017). Trend of epidemiology of ankylosing spondylitis between 2006 and 2015 in Taiwan: a 10 years nationwide population study. Formosan Journal of Rheumatology, 31(2), 1–9.&lt;br/&gt;Chen, J. A., Hou, T. Y., Liu, F. C., Chen, C. H., Lai, J. H., Chang, D. M., &amp;amp; Kuo,S. Y. (2007). The prevalence of HLA-B27 subtypes in AS patients. Formosan Journal of Rheumatology, 21(1), 52–56.&lt;br/&gt;Cramer, J. A., Roy, A., Burrell, A., Fairchild, C. J., Fuldeore, M. J., Ollendorf, D. A., &amp;amp; Wong, P. K. (2008). Medication compliance and persistence: terminology and definitions. Value in Health, 11(1), 44–47.&lt;br/&gt;Dillon, C. F., &amp;amp; Hirsch, R. (2011). The United States national health and nutrition examination survey and the epidemiology of ankylosing spondylitis. American Journal of the Medical Sciences, 341(4), 281–283.&lt;br/&gt;Doward, L., Spoorenberg, A., Cook, S. A., Whalley, D., Helliwell, P. S., Kay, L. J., ... &amp;amp; Chamberlain, M. A. (2003). Development of the ASQoL: a quality of life instrument specific to ankylosing spondylitis. Annals of the Rheumatic Diseases, 62(1), 20–26.&lt;br/&gt;Garrett, S., Jenkinson, T., Kennedy, L. G., Whitelock, H., Gaisford, P., &amp;amp; Calin, A. (1994). A new approach to defining disease status in ankylosing spondylitis: the Bath Ankylosing Spondylitis Disease Activity Index. Journal of Rheumatology, 21(12), 2286–2291.&lt;br/&gt;Goh, L., &amp;amp; Samanta, A. (2012). Update on biologic therapies in ankylosing spondylitis: a literature review. International Journal of Rheumatic Diseases, 15(5), 445–454.&lt;br/&gt;Khan, M. A. (2002). Update on spondyloarthropathies. Annals of Internal Medicine, 136(12), 896–907.&lt;br/&gt;Lukas, C., Landewe, R., Sieper, J., Dougados, M., Davis, J., Braun, J., ... &amp;amp; Van der Heijde, D. (2008). Development of an ASAS-endorsed disease activity score (ASDAS) in patients with ankylosing spondylitis. Annals of the Rheumatic Diseases, 68(1), 18–24.&lt;br/&gt;Machado, P. M., Landewe, R. B., &amp;amp; van der HEIJDE, D. M. (2011). Endorsement of definitions of disease activity states and improvement scores for the Ankylosing Spondylitis Disease Activity Score: results from OMERACT 10. Journal of Rheumatology, 38(7), 1502–1506.&lt;br/&gt;Machado, P., Landewé, R., Lie, E., Kvien, T. K., Braun, J., Baker, D., ... &amp;amp; Assessment of SpondyloArthritis international Society. (2010). Ankylosing Spondylitis Disease Activity Score (ASDAS): defining cut-off values for disease activity states and improvement scores. Annals of the Rheumatic Diseases, 70(1), 47–53.&lt;br/&gt;Reveille, J.D. (2011). Epidemiology of spondyloarthritis in North America. American Journal of the Medical Sciences, 341(4), 284–286.&lt;br/&gt;Van Der Heijde, D., Braun, J., Dougados, M., Sieper, J., Pedersen, R., Szumski, A., &amp;amp; Koenig, A. S. (2012). Sensitivity and discriminatory ability of the Ankylosing Spondylitis Disease Activity Score in patients treated with etanercept or sulphasalazine in the ASCEND trial. Rheumatology, 51(10), 1894–1905.&lt;br/&gt;Wanders, A., Heijde, D. V. D., Landewé, R., Béhier, J. M., Calin, A., Olivieri, I., ... &amp;amp; Dougados, M. (2005). Nonsteroidal antiinflammatory drugs reduce radiographic progression in patients with ankylosing spondylitis: a randomized clinical trial. Arthritis &amp;amp; Rheumatism, 52(6), 1756–1765.&lt;br/&gt;Xu, M., Lin, Z., Deng, X., Li, L., Wei, Y., Liao, Z., ... &amp;amp; Lin, Q. (2011). The Ankylosing Spondylitis Disease Activity Score is a highly discriminatory measure of disease activity and efficacy following tumour necrosis factor-α inhibitor therapies in ankylosing spondylitis and undifferentiated spondyloarthropathies in China. Rheumatology, 50(8), 1466–1472.&lt;br/&gt;Yeh, F. C., Chen, H. C., Hou, T. Y., Liu, F. C., Kuo, S. Y., Chu, S. J., ... &amp;amp; Chen, C. H. (2014). Diagnostic validity of computed tomography for HLA-B27 negative ankylosing spondylitis: A retrospective study of 209 patients. Formosan Journal of Rheumatology, 28(1), 60–66.&lt;br/&gt;Zhao, L. K., Liao, Z. T., Li, C. H., Li, T. W., Wu, J., Lin, Q., ... &amp;amp; Gu, J. R. (2007). Evaluation of quality of life using ASQoL questionnaire in patients with ankylosing spondylitis in a Chinese population. Rheumatology International, 27(7), 605–611.&lt;br/&gt;&lt;br/&gt; &lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
+      <c r="Z9" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/6r6c3j</t>
         </is>
@@ -1729,35 +1715,34 @@
           <t>Travel time prediction、model selection、SVR</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>點閱:112</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>點閱:112</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
         <is>
           <t xml:space="preserve">
 近年來，旅行時間預測一直是智慧交通系統中一個重要的議題，特別是在處理擁堵問題上，旅行時間預測更是扮演重要的角色。根據2017年ACM KDDCUP的聲明，高速公路尖峰時段的擁堵問題可能會壓垮相關交通管理部門，因為正如我們所知，擁堵會造成經濟損失。如果有一個準確的旅行時間預測模型來預測旅行時間，便可以幫助旅行者做出關於何時旅行以及旅行路線的決策，從而避免擁堵所造成的經濟損失和浪費旅行者的時間。本論文中，我們採用傳統的流程來預測旅行時間，找出重要特徵，並比較了四種傳統模型在旅行時間預測中的準確性。實驗結果表明SVR模型具有更好的總體準確性，因此我們選擇它作為我們的基線模型。在旅行時間預測所使用的特徵中，我們猜測降雨量和當前的交通狀況特徵可能會對旅行時間產生很大影響。我們提出了雙特徵方法，以不同於傳統方式的方式處理降雨特徵和當前交通狀況特徵，從而提高SVR模型的準確性。我們設計了一系列的實驗來證明雙特徵方法是否能有效提升SVR模型的準確性，結果表明，我們提出的雙特徵方法可以提高SVR模型的準確性，符合我們的預期。</t>
         </is>
       </c>
-      <c r="Z10" t="inlineStr">
+      <c r="Y10" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 Altman, N. S. (1992). An introduction to kernel and nearest-neighbor nonparametric        regression. The American Statistician, 46(3), 175-185.&lt;br/&gt;Fei, X., Lu, C. C., &amp;amp; Liu, K. (2011). A bayesian dynamic linear model approach for real-time short-term freeway travel time prediction. Transportation Research Part C: Emerging Technologies, 19(6), 1306-1318.&lt;br/&gt;Friedman, J. H. (2001). Greedy function approximation: a gradient boosting machine. Annals of statistics, 1189-1232. ISO 690&lt;br/&gt;Friedman, J. H. (2002). Stochastic gradient boosting. Computational Statistics &amp;amp; Data Analysis, 38(4), 367-378.&lt;br/&gt;Innamaa, S. (2005). Short-term prediction of travel time using neural networks on an interurban highway. Transportation, 32(6), 649-669.&lt;br/&gt;International Bridge, Tunnel and Turnpike Association, (2016). 2016 National Toll Technology Survey Final.&lt;br/&gt;Li, C. S., &amp;amp; Chen, M. C. (2013). Identifying important variables for predicting travel time of freeway with non-recurrent congestion with neural networks. Neural Computing and Applications, 23(6), 1611-1629.&lt;br/&gt;Li, X., &amp;amp; Bai, R. (2016, December). Freight Vehicle Travel Time Prediction Using Gradient Boosting Regression Tree. In Machine Learning and Applications (ICMLA), 2016 15th IEEE International Conference on (pp. 1010-1015). IEEE. ISO 690&lt;br/&gt;Myung, J., Kim, D. K., Kho, S. Y., &amp;amp; Park, C. H. (2011). Travel time prediction using k nearest neighbor method with combined data from vehicle detector system and automatic toll collection system. Transportation Research Record: Journal of the Transportation Research Board, (2256), 51-59.&lt;br/&gt;Pedregosa, F., Varoquaux, G., Gramfort, A., Michel, V., Thirion, B., Grisel, O., ... &amp;amp; Vanderplas, J. (2011). Scikit-learn: Machine learning in Python. Journal of Machine Learning Research, 12(Oct), 2825-2830.&lt;br/&gt;Qiao, W., Haghani, A., &amp;amp; Hamedi, M. (2012). Short-term travel time prediction considering the effects of weather. Transportation Research Record: Journal of the Transportation Research Board, (2308), 61-72.&lt;br/&gt;Schapire, R. E. (1990). The strength of weak learnability. Machine learning, 5(2), 197-227.&lt;br/&gt;Schrank, D., Eisele, B., Lomax, T., &amp;amp; Bak, J. (2015). 2015 urban mobility scorecard. ISO 690&lt;br/&gt;van Hinsbergen, C. I., Van Lint, J. W. C., &amp;amp; Van Zuylen, H. J. (2009). Bayesian committee of neural networks to predict travel times with confidence intervals. Transportation Research Part C: Emerging Technologies, 17(5), 498-509.&lt;br/&gt;Vlahogianni, E. I., Karlaftis, M. G., &amp;amp; Golias, J. C. (2014). Short-term traffic forecasting: Where we are and where we’re going. Transportation Research Part C: Emerging Technologies, 43, 3-19.&lt;br/&gt;Wu, C. H., Ho, J. M., &amp;amp; Lee, D. T. (2004). Travel-time prediction with support vector regression. IEEE transactions on intelligent transportation systems, 5(4), 276-281.&lt;br/&gt;Zhang, Y., &amp;amp; Haghani, A. (2015). A gradient boosting method to improve travel time prediction. Transportation Research Part C: Emerging Technologies, 58, 308-324.&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA10" t="inlineStr">
+      <c r="Z10" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/m6464w</t>
         </is>
@@ -1862,35 +1847,34 @@
           <t>text analysis、knowledge management、nursing home、nursing home accreditation</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>點閱:116</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>點閱:116</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
         <is>
           <t xml:space="preserve">
 本研究主要探討如何應用知識管理建置護理之家評鑑系統。目前長期照顧機構的評鑑準備工作主要仍仰賴紙本資料，可能會有資料重複填寫、遺失或缺漏、需要大量空間保存等問題，此外長照機構內的服務提供者多半為中齡者，對於新科技的應用常抱持著反對或消極的態度，設計一個簡單且實用的評鑑系統，提高評鑑準備人員使用的意願並且改善評鑑準備時需花費的大量物力、人力與時間，有其必要性。於需求分析階段，以逐步文本分析結合知識管理的知識加值概念，將護理之家評鑑條文文本進行拆解，從中萃取有重要意義的字詞進行編碼及詮釋，並將其應用於護理之家評鑑系統中，讓使用者可以快速從知識交換平台找到該項條文需要的文件。於介面設計階段，以圖形化使用者介面為設計原則，並適當加入圖像及顏色搭配，避免都是文字或圖像會不容易辨別或同一介面顏色太多讓使用者眼花撩亂。期望可以讓護理之家中的評鑑準備人員容易地學習及操作系統。滿意度整體評估結果顯示多數的使用者可以接受及認同本研究設計之護理之家評鑑系統，不過在系統與資訊品質、知覺易用二個構面上仍有需改善之地方，即系統的操作容易性、圖示直覺性對於使用者而言仍不夠符合其需求。</t>
         </is>
       </c>
-      <c r="Z11" t="inlineStr">
+      <c r="Y11" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 英文文獻&lt;br/&gt;Berger, A. A. （1995）. Cultural criticism: A primer of key concepts （Vol. 4）. Sage Publications.&lt;br/&gt;Connell, J. L., &amp;amp; Shafer, L. (1989). Structured rapid prototyping: an evolutionary approach to software development. Yourdon Press.&lt;br/&gt;Davis, F. D., Bagozzi, R. P., &amp;amp; Warshaw, P. R. （1989）. User acceptance of computer technology: a comparison of two theoretical models. Management science, 35（8）, 982-1003.&lt;br/&gt;DeLone, W. H., &amp;amp; McLean, E. R. （1992）. Information systems success: The quest for the dependent variable. Information systems research, 3（1）, 60-95.&lt;br/&gt;Fairclough, N. &amp;amp; Wodak, R. （1995）. Critical discourse analysis （pp.1995-1995）. na.&lt;br/&gt;Nonaka, I., &amp;amp; Takeuchi, H. （1995）. The knowledge-creating company: How Japanese companies create the dynamics of innovation. Oxford university press.&lt;br/&gt;Schleiermacher, F. （1809）. General Hermeneutics. Schleiermacher: Hermeneutics and criticism, 227-268.&lt;br/&gt;Stewart, T., &amp;amp; Ruckdeschel, C. （1998）. Intellectual capital: The new wealth of organizations.&lt;br/&gt;Tan, F. B., Tung, L. L., &amp;amp; Xu, Y. （2009）. A study of web-designer's criteria for effective business-to-consumer （b2c） websites using the repertory grid technique. Journal of Electronic Commerce Research, 10（3）, 155.&lt;br/&gt;Warnke, G. （1987）. Gadamer: Hermeneutics, tradition, and reason （Vol. 1）. Stanford University Press.&lt;br/&gt;中文文獻&lt;br/&gt;iGms百旭科技（民106）。產品介紹-評鑑管理系統（HEV）。民106年11月29日取自&lt;br/&gt;http://www.igms.com.tw/Site/Product/default.aspx?id=plan&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006130199" target="_blank"&gt;王惠玄、林俊逸、邱炯訓（民93）。醫院評鑑網路申報系統建置。中山管理評論， 12（6），頁 141-163。&lt;/a&gt;&lt;br/&gt;汎宇電商股份有限公司（民106）。產品服務：代理服務-GIS長期照護系統。民106年11月20日取自 http://uecdemo.byethost4.com/?p=168&amp;amp;i=1&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006907405" target="_blank"&gt;吳肖琪（民106）。我國長照政策之新契機。長期照護雜誌，21（1），頁 1-7。&lt;/a&gt;&lt;br/&gt;吳杰亮（民104年6月）。如何利用資訊設計輔助評鑑。「104年度醫院評鑑學術研討會」發表之論文，國泰人壽大樓。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006536276" target="_blank"&gt;李忠穎（民98）。建置機構式長期照護資訊系統-以某長期照護中心為例。安泰醫護雜誌， 15（1），頁 53-68。&lt;/a&gt;&lt;br/&gt;易透網科技開發股份有限公司（民106）。程式設計-醫院評鑑系統。民106年11月29日取自http://www.etan.com.tw/etan2010/programing11.php&lt;br/&gt;林宏榮（民103）。機構評鑑、認證及訪查。新北市：財團法人醫院評鑑暨醫療品質策進會。&lt;br/&gt;林東清（民91）。資訊管理--e化企業的核心競爭能力。臺北：智勝。&lt;br/&gt;林芳玫（民85）。女性與媒體再現。臺北：巨流。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006603717" target="_blank"&gt;林麗嬋、吳婉翎、翟文英（民99）。住民照顧衝擊:長期照護機構評鑑決策模式發展基礎。長期照護雜誌，14（2），頁 125-135。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005705366" target="_blank"&gt;夏春祥（民86）。文本分析與傳播研究。新聞學研究， 54，頁 141-166。&lt;/a&gt;&lt;br/&gt;徐國峰（民94）。龍魂不滅—傳播儀式中的社群記憶。國立政治大學廣播電視學研究所。&lt;br/&gt;悅康健康管理顧問科技股份有限公司（民106）。Product-AM醫院評鑑系統。民106年11月29日取自http://www.catchyourhealth.com.tw/zh-TW/product_AM.html&lt;br/&gt;高雄醫學大學附設中和紀念醫院（民106）。醫品室：業務職掌-相關連結。民106年11月29日取自http://www.kmuh.org.tw/wwwwAdministration/MedicalQuality/works_6.html&lt;br/&gt;健仁醫院（民94）。地區醫院新制醫院評鑑網站資訊系統之開發與應用。民106年11月29日取自http://www.areahp.org.tw/upload/event_source/94ANS3M2.ppt&lt;br/&gt;張皓怡（民104）。以 Web APP 建置長期照顧資訊系統創新之研究。國立臺北護理健康大學資訊管理研究所。&lt;br/&gt;張嘉秀、李世代（民96）。長期照護資訊發展面面觀。長期照護雜誌，11（4），頁 331-344。&lt;br/&gt;許雅華（民106）。影響台灣長期照護機構資訊化相關因素及需求探討。亞洲大學健康產業管理學系。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0004804480" target="_blank"&gt;郭麗敏、黃子庭（民93）。照顧一位新遷居至護理之家的老年住民之護理經驗。護理雜誌， 51（3），頁 94-99。&lt;/a&gt;&lt;br/&gt;陳正榮（民106年3月31日）。醫院評鑑經驗分享-三軍總醫院經驗。「106年度《醫院評鑑分享交流學術研討會》」發表之論文，臺中榮民總醫院研究大樓。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006870649" target="_blank"&gt;陳玫如、陳泰源（民105）。長期照顧服務法對護理之家經營策略之研究。全球管理與經濟，12(1)，53-70.&lt;/a&gt;&lt;br/&gt;陳怡秀（民106）。探討長期照護資訊系統使用者滿意度之研究。南華大學資訊管理學系。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006106185" target="_blank"&gt;傅家芸、呂麗戎、張怡秋（民96）。應用院內網路系統因應新制醫院評鑑—以南部某醫院為例。醫療資訊雜誌， 16（4），頁 83-92。&lt;/a&gt;&lt;br/&gt;博鈞科技股份有限公司（民106）。產品與服務：ECare長期照護機構管理系統-系統架構。民106年11月20日取自 http://www.mobisnet.com.tw/core/main/inpage.php?pageId=33&lt;br/&gt;黃莉庭（民104）。原質化介面設計風格導入台鐵網頁設計。國立臺灣師範大學設計學系。&lt;br/&gt;黃裔貽（民106年3月31日）。亞東醫院評鑑準備經驗分享。「106年度《醫院評鑑分享交流學術研討會》」發表之論文，臺中榮民總醫院研究大樓。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0004720749" target="_blank"&gt;黃興進（民91）。醫療資訊管理系統研究議題之探討。資訊管理學報， 9（S），頁 101-116。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006642192" target="_blank"&gt;葉佳承、楊文金、廖斌吟、黃柏森 （民100）。 兩篇七年級「能量塔」文本之比較分析。教育科學研究期刊， 56（2），頁 175-206。&lt;/a&gt;&lt;br/&gt;構思數位策略股份有限公司（民106）。 服務與方案：長期照護機構e化服務-照護專業管理系統。取自 http://www.gosite.com.tw/solutions/carepro/homecare.html&lt;br/&gt;趙大羽、關東升（民103）。互動設計的藝術-iOS7/8擬物化到扁平化革命。臺北：佳魁資訊。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006682983" target="_blank"&gt;蔡淑鳳、林育秀、梁亞文（民101）。影響護理之家評鑑結果之因素研究：以2009年台灣首次全國護理之家評鑑為例。臺灣公共衛生雜誌， 31（2），頁 119-132。 doi: doi:10.6288/TJPH2012-31-02-03&lt;/a&gt;&lt;br/&gt;蔡芳文、林巧韻（民102）。長期照顧服務智慧化與科技化-以雙連安養中心為例。&lt;br/&gt;衛生福利部（民104）。長期照顧服務量能提升計畫（104~107年）。&lt;br/&gt;衛生福利部（民105a）。長期照顧十年計畫2.0（106~115年）。&lt;br/&gt;衛生福利部（民105b）。長照保險制度規劃。&lt;br/&gt;衛生福利部（民106a）。106年度一般護理之家評鑑基準。&lt;br/&gt;衛生福利部（民106b，民105年9月）。長照服務資源地理地圖。取自 http://ltcgis.mohw.gov.tw/Select/QueryResource.aspx&lt;br/&gt;衛生福利部（民106b，民106年11月7日）。 長照政策專區。長照服務法-子法。取自 http://topics.mohw.gov.tw/LTC/cp-92-29914-201.html&lt;br/&gt;衛生福利部統計處（民106，民107年1月16日）。衛生福利統計專區。長期照顧統計。取自https://dep.mohw.gov.tw/DOS/lp-3550-113.html&lt;br/&gt;鄭玉珍（民97）。區域級以上（含）醫院採用資訊科技因應新制醫院評鑑之因素。國立中正大學會計與資訊科技所。&lt;br/&gt;叡揚資訊股份有限公司（民106）。產品與服務-醫院評鑑管理系統。民106年11月29日取自&lt;br/&gt;http://www.gss.com.tw/index.php/product-and-service/hospital-evaluation&lt;br/&gt;諾亞克科技股份有限公司（民106）。產品與服務-長期照護護理系統。取自 https://www.u-ark.com.tw/product-??????.htm&lt;br/&gt;蔣政廷。透由資訊系統整合醫院評鑑作業-以台灣社區醫院協會評鑑網路版及單機版為例。民106年11月29日取自http://www.areahp.org.tw/upload/project/txt/980413.pdf&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
+      <c r="Z11" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/hp79tn</t>
         </is>
@@ -1995,35 +1979,34 @@
           <t>Sarcopenia、Functional fitness test、Cut-off point data</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>點閱:348</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>點閱:348</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
         <is>
           <t xml:space="preserve">
 在生命步入老化的過程中會引起許多生理功能的衰退，隨著年齡的增長，肌肉質量的減少會加速，這一生理現象就是所謂的肌少症。肌少症並不是一種疾病，而是描述一種綜合性的生理特徵，由於成因不明顯且無立即性的危險，因此常被國人所忽略。肌少症不只影響生理層面，還會增加老年人跌倒、認知功能障礙與失能等風險。在文獻中顯示，亞洲地區肌少症好發率相關的調查差異極大，除了採樣地區與族群不同，更缺乏統一的評估指標，目前台灣對於肌少症切點數據的研究仍然沒有共識，台灣應建立專屬的檢測標準。現今篩檢肌少症最準確的檢查是進行肌肉質量的量測，但是其高昂的費用與時效性，導致難以應用於偏遠城鄉或社區進行大量篩檢。在台灣，社區高齡體適能檢測是經濟且有效的預防醫療措施，並行之有年。因此本研究目的有二，首先以功能性體適能檢測與肌少症相關性進行研究，探討利用功能性體適能檢測肌少症之方法與流程。其二是利用資料學習方法建置篩檢肌少症之系統，透過不斷更新切點數據來達到更準確的篩檢，並能有效在社區進行施測，建立標準的參考數據。</t>
         </is>
       </c>
-      <c r="Z12" t="inlineStr">
+      <c r="Y12" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 【英文文獻】&lt;br/&gt;Abizanda, P., Navarro, J. L., García-Tomás, M. I., López-Jiménez, E., Martínez-Sánchez, E., &amp;amp; Paterna, G. (2012). Validity and Usefulness of Hand-Held Dynamometry for Measuring Muscle Strength in Community-Dwelling Older Persons. Archives of gerontology and geriatrics, 54(1), 21-27.&lt;br/&gt;Arnold, C. M., Warkentin, K. D., Chilibeck, P. D., &amp;amp; Magnus, C. R. (2010). The Reliability and Validity of Handheld Dynamometry for the Measurement of Lower-Extremity Muscle Strength in Older Adults. The Journal of Strength &amp;amp; Conditioning Research, 24(3), 815-824.&lt;br/&gt;Baumgartner, R. N., Koehler, K. M., Gallagher, D., Romero, L., Heymsfield, S. B., Ross, R. R., ... &amp;amp; Lindeman, R. D. (1998). Epidemiology of Sarcopenia Among the Elderly in New Mexico. American journal of epidemiology, 147(8), 755-763.&lt;br/&gt;Cesari, M., Landi, F., Vellas, B., Bernabei, R., &amp;amp; Marzetti, E. (2016). Sarcopenia and Physical Frailty: two sides of the same coin. Pathophysiological Mechanisms of Sarcopenia in Aging and in Muscular Dystrophy: A Translational Approach.&lt;br/&gt;Chang, C.-I., Chen, C.-Y., Huang, K.-C., Wu, C.-H., Hsiung, C., &amp;amp; Hsu, C.-C. (2013). Comparison of Three BIA Muscle Indices for Sarcopenia Screening in Old Adults. European Geriatric Medicine, 4(3), 145-149.&lt;br/&gt;Chen, L. K., Liu, L. K., Woo, J., Assantachai, P., Auyeung, T. W., Bahyah, K. S., ... &amp;amp; Lee, J. S. (2014). Sarcopenia in Asia: Consensus Report of the Asian Working Group for Sarcopenia. Journal of the American Medical Directors Association, 15(2), 95-101.&lt;br/&gt;Chien, M.-Y., Kuo, H.-K., &amp;amp; Wu, Y.-T. (2010). Sarcopenia, Cardiopulmonary Fitness, and Physical Disability in Community-Dwelling Elderly People. Physical therapy, 90(9), 1277-1287.&lt;br/&gt;Cruz-Jentoft, A. J., Baeyens, J. P., Bauer, J. M., Boirie, Y., Cederholm, T., Landi, F., et al. (2010). Sarcopenia: European Consensus on Definition and Diagnosis Report of the European Working Group on Sarcopenia in Older People. Age and ageing, afq034.&lt;br/&gt;Fried, L. P., Tangen, C. M., Walston, J., Newman, A. B., Hirsch, C., Gottdiener, J., et al. (2001). Frailty in Older Adults Evidence for a Phenotype. The Journals of Gerontology Series A: Biological Sciences and Medical Sciences, 56(3), M146-M157.&lt;br/&gt;Goodpaster, B. H., Park, S. W., Harris, T. B., Kritchevsky, S. B., Nevitt, M., Schwartz, A. V., et al. (2006). The Loss of Skeletal Muscle Strength, Mass, and Quality in Older Adults: the Health, Aging and Body Composition Study. The Journals of Gerontology Series A: Biological Sciences and Medical Sciences, 61(10), 1059-1064.&lt;br/&gt;Iannuzzi-Sucich, M., Prestwood, K. M., &amp;amp; Kenny, A. M. (2002). Prevalence of Sarcopenia and Predictors of Skeletal Muscle Mass in Healthy, Older Men and Women. The Journals of Gerontology Series A: Biological Sciences and Medical Sciences, 57(12), M772-M777.&lt;br/&gt;Janssen, I., Heymsfield, S. B., &amp;amp; Ross, R. (2002). Low Relative Skeletal Muscle Mass (Sarcopenia) in Older Persons is Associated with Functional Impairment and Physical Disability. Journal of the American Geriatrics Society, 50(5), 889-896.&lt;br/&gt;Jones, C. J., &amp;amp; Rikli, R. E. (2002). Measuring Functional. The Journal on active aging, 1, 24-30.&lt;br/&gt;Kubicki, A. (2014). Functional Assessment in Older Adults: Should We Use Timed Up and Go or Gait Speed Test? Neuroscience letters, 577, 89-94.&lt;br/&gt;Mijnarends, D. M., Meijers, J. M., Halfens, R. J., ter Borg, S., Luiking, Y. C., Verlaan, S., et al. (2013). Validity and Reliability of Tools to Measure Muscle Mass, Strength, and Physical Performance in Community-Dwelling Older People: a Systematic Review. Journal of the American Medical Directors Association, 14(3), 170-178.&lt;br/&gt;Rikli, R. E., &amp;amp; Jones, C. J. (1999). Functional Fitness Normative Scores for Community-Residing Older Adults, Ages 60-94. Journal of Aging and Physical Activity, 7, 162-181.&lt;br/&gt;Rikli, R. E., &amp;amp; Jones, C. J. (2013). Development and Validation of Criterion-Referenced Clinically Relevant Fitness Standards for Maintaining Physical Independence in Later Years. The Gerontologist, 53(2), 255-267.&lt;br/&gt;Rose, D. J. (2002). Promoting Functional Independence Among" At Risk" and Physically Frail Older Adults Through Community-Based Fall-Risk-Rreduction Programs. Journal of Aging and Physical Activity, 10(2), 207-225.&lt;br/&gt;Roubenoff, R. (2003). Sarcopenia: Effects on Body Composition and Function. The Journals of Gerontology Series A: Biological Sciences and Medical Sciences, 58(11), M1012-M1017.&lt;br/&gt;Schrager, M. A., Metter, E. J., Simonsick, E., Ble, A., Bandinelli, S., Lauretani, F., et al. (2007). Sarcopenic Obesity and Inflammation in the InCHIANTI Study. Journal of Applied Physiology, 102(3), 919-925.&lt;br/&gt;Spirduso, W. W. (1995). Physical Functioning of the Old and Oldest-Old. Physical dimensions of aging. Champaign, IL: Human Kinetics, 329-358.&lt;br/&gt;Stenholm, S., Harris, T. B., Rantanen, T., Visser, M., Kritchevsky, S. B., &amp;amp; Ferrucci, L. (2008). Sarcopenic Obesity-Definition, Etiology and Consequences. Current opinion in clinical nutrition and metabolic care, 11(6), 693.&lt;br/&gt;Takeshima, N., Rogers, N. L., Rogers, M. E., Islam, M. M., Koizumi, D., &amp;amp; Lee, S. (2007). Functional Fitness Gain Varies in Older Adults Depending on Exercise Mode. Medicine and science in sports and exercise, 39(11), 2036.&lt;br/&gt;&lt;br/&gt;【中文文獻】&lt;br/&gt;王秀華與李淑芳(2009)。老年人功能性體適能之運動處方。大專體育，(101)， 164-171。&lt;br/&gt;王秀華與李淑芳(2011)。不同運動階段老年婦女其功能性體適能與健康生活品質之研究。體育學報，44(3)，333-350。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006812958" target="_blank"&gt;田玉笛、王秀華與錢桂玉(2015)。以社區應用為導向之中老年人行動能力評估。中華體育季刊，29(1)，29-36。&lt;/a&gt;&lt;br/&gt;江瑞坤、鄭宇翔、陳欣欣、陳淑娟與蔡坤維(2006)。雲嘉南老人跌倒之研究。台灣老年醫學雜誌，1(3)，174-181。&lt;br/&gt;吳易謙、熊昭、陳慶餘、吳名祥與許志成(2014)。台灣社區老人肌少症流行病學初探。臺灣醫學，18(3)，290-302。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006784156" target="_blank"&gt;吳雅汝、周怡君與詹鼎正(2014)。文獻回顧-肌少症與衰弱症。內科學誌，25(3)，131-136。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006817137" target="_blank"&gt;吳蔓君(2015)。肌少症簡介。家庭醫學與基層醫療，30(4)，103-107。&lt;/a&gt;&lt;br/&gt;李佳倫與鄭景峰(2010)。臺灣老年人身體活動量與功能性體適能的關係。大專體育學刊，12(4)，79-89。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006838638" target="_blank"&gt;李幸穎、孫嘉宏與林陳涌(2015)。多面向巡迴訓練對城鄉社區老人身體功能與平衡能力之影響。物理治療，40(2)，53-65。&lt;/a&gt;&lt;br/&gt;侯孟次、吳佩穎、林怡貝、張尹凡、陳全裕、官大紳等人(2011)。偏遠社區老年男性體適能常模與現況分析。台灣老年醫學暨老年學雜誌，6(3)，190-202。&lt;br/&gt;高鈺彥(2009)。健走與太極拳運動對中老年婦女功能性體適能及心率變異性影響之比較研究。臺灣師範大學體育學系學位論文，1-59。&lt;br/&gt;張珮慈與傅麗蘭(2016)。亞洲肌少症之評估指標比較與盛行率介紹。臺灣體育學術研究，(60)，145-159。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006760642" target="_blank"&gt;張淑芳(2014)。老年肌少症之診斷與治療。護理雜誌，61(2)，101-105。&lt;/a&gt;&lt;br/&gt;陳怡如(2006)。台北市老人身體活動，功能性體適能與跌倒之模式分析。臺灣大學護理學研究所學位論文，1-172。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006838934" target="_blank"&gt;陳慶餘(2015)。臺灣年老衰弱症的研究與應用。長期照護雜誌，19(2)，137-148。&lt;/a&gt;&lt;br/&gt;傅麗蘭與楊政峰(1999)。獨居老人跌倒情形，步態，居家環境及身體功能評估。 中華民國物理治療學會雜誌，24(2)，53-62。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005799099" target="_blank"&gt;黃泰諭、張哲榕、林曼蕙與方進隆(2005)。十週水中有氧訓練對女性老年人功能性體適能之影響。運動生理暨體能學報，(3)，121-129。&lt;/a&gt;&lt;br/&gt;黃偉智(2008)。臺東縣退休公教人員健康促進生活型態與功能性體適能之研究。臺東大學進修部運動休閒管理碩學位論文，1-121。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005885520" target="_blank"&gt;楊惠如、呂桂雲、陳宇嘉與張永源。(2006)。社區獨居老人健康狀況與長期照護需求研究，實證護理，2(3)，229-240。&lt;/a&gt;&lt;br/&gt;歐恬維(2010)。不同身體活動量老年女性體適能與心智功能之比較研究。臺灣師範大學體育學系學位論文，1-76。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006670287" target="_blank"&gt;蔡存維、郭彥宇與蔡櫻蘭(2011)。團體伸展訓練課程對長期照護機構高齡者功能性體適能的影響。大專體育學刊，13(4)，445-452。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006799398" target="_blank"&gt;蔡英美、郭慈安與王俊明(2012)。老年人生活型態、運動參與程度與功能性體適能之研究。運動與健康研究，2(1)，25-49。&lt;/a&gt;&lt;br/&gt;謝珮琳(2012)。年長者功能性體適能常模與運動行為及自覺健康之關係。成功大學體育健康與休閒研究所學位論文，1-149。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006899168" target="_blank"&gt;韓德生(2016)。肌少症的評估與診斷。長期照護雜誌，20(2)，115-124。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006813072" target="_blank"&gt;嚴嘉楓、紀彣宙與周正修(2015)。肌少症之流行病學及健康促進介入之探討。身心障礙研究季刊，13(1)，9-25。&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;【網站資料】&lt;br/&gt;中華民國人口推估(2016)。國家發展委員會。取自：&lt;br/&gt;http://www.ndc.gov.tw/Content_List.aspx?n=84223C65B6F94D72&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22105NTNU5567001%22.&amp;amp;searchmode=basic" target="_blank"&gt;何信弘(2016)。驗證社區高齡者功能性體適能快速評估與多元性運動介入效益之研究(博士論文)。取自：http://handle.ncl.edu.tw/11296/ndltd/52038365857647948953&lt;/a&gt;&lt;br/&gt;吳明宜(2010)。常用職評工具之地域性常模建立。取自：file:///C:/Users/4fair/Downloads/%E5%B8%B8%E6%A8%A1%E5%B7%A5%E5%85%B7%E6%88%90%E6%9E%9C991129.pdf&lt;br/&gt;吳明城與詹正豐(2015)。104年度臺灣年長者功能性體適能現況評估研究。取自：http://www.sa.gov.tw/wSite/public/Attachment/f1474259369474.pdf&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22098NCPE5419026%22.&amp;amp;searchmode=basic" target="_blank"&gt;李聿(2010)。瑜珈提斯對中高及高齡者平衡能力與功能性體適能之影響(碩士論文)。取自：&lt;/a&gt;&lt;br/&gt;http://handle.ncl.edu.tw/11296/ndltd/44352525921461506115&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22097NTCP5567010%22.&amp;amp;searchmode=basic" target="_blank"&gt;周嘉琪(2009)。以健身運動與自尊模式為基礎探討功能性體適能運動計劃對安養護機構老年人自尊的影響(博士論文)。取自：http://handle.ncl.edu.tw/11296/ndltd/53698986572910346156&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22094NPTTC567011%22.&amp;amp;searchmode=basic" target="_blank"&gt;林炎岐(2006)。國小男童身體柔軟度、運動表現與生活型態之相關研究(碩士論文)。取自：&lt;/a&gt;&lt;br/&gt;http://handle.ncl.edu.tw/11296/ndltd/09562296488770202886&lt;br/&gt;陳晶瑩(2013)。老年人預防保健分類簡介。臺大醫院電子報。2013年3月64期，取自：&lt;br/&gt;http://epaper.ntuh.gov.tw/health/201303/special_1_1.html&lt;br/&gt;整合分析II：診斷檢驗(2010)。中國醫藥大學。取自：http://biostatdept.cmu.edu.tw/doc/epaper_b/26.pdf&lt;br/&gt;體位測量模型估算老人大腿肌肉量與身體活動功能之相關性探討(2010)。國家衛生研究院電子報。2010年9月372期，取自：http://enews.nhri.org.tw/enews_list_new2_more.php?volume_indx=372&amp;amp;showx=showarticle&amp;amp;article_indx=8006&lt;br/&gt;體適能科技檢測研究案(2016)。臺大物理治療學系。取自：http://www.sa.gov.tw/wSite/public/Attachment/f1483089879824.pdf&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA12" t="inlineStr">
+      <c r="Z12" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/usj65z</t>
         </is>
@@ -2128,35 +2111,34 @@
           <t>Doctor- Patient Communication、Visualization Medical、3D Modeling、Communication Visualize、Medical Visualization</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>點閱:305</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>點閱:305</t>
+          <t>23</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
         <is>
           <t xml:space="preserve">
 　　隨著科技的發達，許多醫療器材跟著數位化，電子病歷與醫療資訊系統的出現，不僅有效降低醫療失誤，也大大提升了醫療品質及效率。如今，「以病人為中心」的醫療概念出現，為了加強病人對自己身體健康之重視，對於人體的基本狀況、疾病的基本觀念（包括如何預防與治療）是必須的。因此，本研究提出了以3D人體模型頁面，與醫師之醫囑系統做連結，使醫師在看診的過程中，可連結至頁面，將3D人體模型與疾病基本觀念，作為醫病溝通之輔助工具，以近年較常見之腸胃相關疾病作為案例使用，期望能透過此系統，有效提升醫師與病人之間的溝通效果。　　本研究以專家訪談與病人滿意度問卷作為系統之評估，訪談對象為3位具有20年以上腸胃看診經歷的腸胃科醫師，病人滿意度問卷總共蒐集了70份有效問卷，並以統計軟體SPSS22.0進行資料分析，再與醫師之訪談內容，做一研究統整。研究結果顯示，視覺化之醫病溝通，有效提升病人對於看診時的滿意度，且針對系統內容，病人更願意瞭解與疾病相關之基本觀念，本研究之研究成果，提供醫病雙方一個更方便且更有效的溝通輔助工具。</t>
         </is>
       </c>
-      <c r="Z13" t="inlineStr">
+      <c r="Y13" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 英文文獻&lt;br/&gt;1.Agus, M., Bettio, F., Gobbetti, E., &amp;amp; Pintore, G. (2007, February). Medical Visualization with New Generation Spatial 3D Displays. In Eurographics Italian Chapter Conference (pp. 161-166).&lt;br/&gt;2.Alejski, A., Chen, Y., &amp;amp; Rutt, B. K. (2002). Ultra-high-resolution imaging with a clinical MRI. IEEE instrumentation &amp;amp; measurement magazine, 5(2), 18-23.&lt;br/&gt;3.Alsos, O. A., Das, A., &amp;amp; Svanæs, D. (2012). Mobile health IT: The effect of user interface and form factor on doctor–patient communication. International Journal of Medical Informatics, 81(1), 12-28.&lt;br/&gt;4.Anderson, P., Chapman, P., Ma, M., &amp;amp; Rea, P. (2013). Real-time medical visualization of human head and neck anatomy and its applications for dental training and simulation. Current Medical Imaging Reviews, 9(4), 298-308.&lt;br/&gt;5.Angus, D., Watson, B., Smith, A., Gallois, C., &amp;amp; Wiles, J. (2012). Visualising conversation structure across time: Insights into effective doctor-patient consultations. PloS one, 7(6), e38014.&lt;br/&gt;6.Aronsson, K., &amp;amp; Rundström, B. (1988). Child discourse and parental control in pediatric consultations. Text-Interdisciplinary Journal for the Study of Discourse, 8(3), 159-190.&lt;br/&gt;7.Asan, O., Young, H. N., Chewning, B., &amp;amp; Montague, E. (2015). How physician electronic health record screen sharing affects patient and doctor non-verbal communication in primary care. Patient Education and Counseling, 98(3), 310-316.&lt;br/&gt;8.Baker, C., Blackwood, J., Hartless, C., Pirro, J., &amp;amp; Flower, A. A. (2017, April). Healthcare analytics and visualization using SEMantic Open Source Software (SEMOSS). In Systems and Information Engineering Design Symposium (SIEDS), 2017 (pp. 144-149). IEEE.&lt;br/&gt;9.Beisecker, A. E., &amp;amp; Beisecker, T. D. (1990). Patient information-seeking behaviors when communicating with doctors. Medical Care, 28(1), 19-28.&lt;br/&gt;10.Bensing, J. (1991). Doctor-patient communication and the quality of care. Social science &amp;amp; Medicine, 32(11), 1301-1310.&lt;br/&gt;11.Beveridge, E., Ma, M., Rea, P., Bale, K., &amp;amp; Anderson, P. (2013, January). 3D visualisation for education, diagnosis and treatment of lliotibial band syndrome. In Computer Medical Applications (ICCMA), 2013 International Conference on (pp. 1-6). IEEE.&lt;br/&gt;12.Bognár, A., Barach, P., Johnson, J. K., Duncan, R. C., Birnbach, D., Woods, D., ... &amp;amp; Bacha, E. A. (2008). Errors and the burden of errors: attitudes, perceptions, and the culture of safety in pediatric cardiac surgical teams. The Annals of Thoracic Surgery, 85(4), 1374-1381.&lt;br/&gt;13.Boothe, C., Strawderman, L., &amp;amp; Hosea, E. (2013). The effects of prototype medium on usability testing. Applied ergonomics, 44(6), 1033-1038.&lt;br/&gt;14.Brouse, C., Dumont, G., Yang, P., Lim, J., &amp;amp; Ansermino, J. M. (2007, August). iAssist: a software framework for intelligent patient monitoring. In Engineering in Medicine and Biology Society, 2007. EMBS 2007. 29th Annual International Conference of the IEEE (pp. 3790-3793). IEEE.&lt;br/&gt;15.Bruner, J. S. (1974). From communication to language—A psychological perspective. Cognition, 3(3), 255-287.&lt;br/&gt;16.Castejón, J., López-Roig, S., Pastor, M. A., Pico, C., Reig, M. T., Rodriguez-Marin, J., &amp;amp; Terol, C. (1993). Cancer patients: health information and quality of life. In the 7th Conference of the European Health Psychology Society.&lt;br/&gt;17.Cenydd, L., John, N., Bloj, M., Walter, A., &amp;amp; Phillips, N. (2012). Visualizing the surface of a living human brain. IEEE computer graphics and applications, 32(2), 55-65.&lt;br/&gt;18.Champney, L. (1995). Introduction to quantitative political science. Longman Publishing Group.&lt;br/&gt;19.Chang, M. C., Trinh, N. H., Fleming, B. C., &amp;amp; Kimia, B. B. (2010, March). Reliable fusion of knee bone laser scans to establish ground truth for cartilage thickness measurement. In Medical Imaging: Image Processing (p. 76232M).&lt;br/&gt;20.Chittaro, L. (2001). Information visualization and its application to medicine. Artificial Intelligence in Medicine, 22(2), 81-88.&lt;br/&gt;21.Ciuciu, I., &amp;amp; Debruyne, C. (2012, September). Assessing the user satisfaction with an ontology engineering tool based on social processes. In OTM Confederated International Conferences" On the Move to Meaningful Internet Systems" (pp. 242-251). Springer Berlin Heidelberg.&lt;br/&gt;22.DeLone, W. H., &amp;amp; McLean, E. R. (1992). Information systems success: The quest for the dependent variable. Information systems research, 3(1), 60-95.&lt;br/&gt;23.DeLone, W. H., &amp;amp; McLean, E. R. (2002, January). Information systems success revisited. In System Sciences, 2002. HICSS. Proceedings of the 35th Annual Hawaii International Conference on (pp. 2966-2976). IEEE.&lt;br/&gt;24.Delone, W. H., &amp;amp; McLean, E. R. (2003). The DeLone and McLean model of information systems success: a ten-year update. Journal of management information systems, 19(4), 9-30.&lt;br/&gt;25.Desjarlais-deKlerk, K., &amp;amp; Wallace, J. E. (2013). Instrumental and socioemotional communications in doctor-patient interactions in urban and rural clinics. BMC Health Services Research, 13(1), 1.&lt;br/&gt;26.Eveleigh, R. M., Muskens, E., van Ravesteijn, H., van Dijk, I., van Rijswijk, E., &amp;amp; Lucassen, P. (2012). An overview of 19 instruments assessing the doctor-patient relationship: different models or concepts are used. Journal of Clinical Epidemiology, 65(1), 10-15.&lt;br/&gt;27.Frey, C. (2009). Why communicate visually?. The mindmapping software blog. Retrieved from http://mindmappingsoftwareblog.com/why-communicate-visually/&lt;br/&gt;28.Fruhling, A., &amp;amp; Lee, S. (2005). Assessing the reliability, validity and adaptability of PSSUQ. AMCIS 2005 Proceedings, 378.&lt;br/&gt;29.Gopinath, B., Radhakrishnan, K., Sarma, P. S., Jayachandran, D., &amp;amp; Alexander, A. (2000). A questionnaire survey about doctor–patient communication, compliance and locus of control among South Indian people with epilepsy. Epilepsy Research, 39(1), 73-82.&lt;br/&gt;30.Hakone, A., Harrison, L., Ottley, A., Winters, N., Gutheil, C., Han, P. K., &amp;amp; Chang, R. (2017). PROACT: Iterative Design of a Patient-Centered Visualization for Effective Prostate Cancer Health Risk Communication. IEEE transactions on visualization and computer graphics, 23(1), 601-610.&lt;br/&gt;31.Institute of Medicine (US). Committee on Quality of Health Care in America. (2001). Crossing the Quality Chasm: A new health system for the 21st century. National Academy Press.&lt;br/&gt;32.Jung, W. M., Lee, T., Lee, I. S., Kim, S., Jang, H., Kim, S. Y., ... &amp;amp; Chae, Y. (2015). Spatial patterns of the indications of acupoints using data mining in classic medical text: a possible visualization of the meridian system. Evidence-Based Complementary and Alternative Medicine, 2015.&lt;br/&gt;33.Kale, E. H., Mumcuoglu, E. U., &amp;amp; Hamcan, S. (2012). Automatic segmentation of human facial tissue by MRI–CT fusion: A feasibility study. Computer methods and programs in biomedicine, 108(3), 1106-1120.&lt;br/&gt;34.Kaspar, M., Parsad, N. M., &amp;amp; Silverstein, J. C. (2013). An optimized web-based approach for collaborative stereoscopic medical visualization. Journal of the American Medical Informatics Association, 20(3), 535-543.&lt;br/&gt;35.Kleinman, A. (1980). Patients and healers in the context of culture: An Exploration of the Borderland between Anthropology, Medicine, and Psychiatry. Vol. 3. Univ of California Press.&lt;br/&gt;36.Kurillo, G., &amp;amp; Bajcsy, R. (2013). 3D teleimmersion for collaboration and interaction of geographically distributed users. Virtual Reality, 1-15.&lt;br/&gt;37.Lazare, A., Putnam, S. M., &amp;amp; Lipkin Jr, M. (1995). Three functions of the medical interview. In The medical interview (pp. 3-19). Springer New York. Lewis, J. R. (2002). Psychometric Evaluation of the PSSUQ Using Data from Five Years of Usability Studies. International Journal of Human-Computer Interaction, 14(3&amp;amp;4), 463-488.&lt;br/&gt;38.Lewis, J. R. (2002). Psychometric evaluation of the PSSUQ using data from five years of usability studies. International Journal of Human-Computer Interaction, 14(3-4), 463-488.&lt;br/&gt;39.Liang, Y. Z., Fang, B., Wang, Y., Wu, L., &amp;amp; Chen, P. (2011, July). Design of an interactive 3D medical visualization system. In 2011 International Conference on Wavelet Analysis and Pattern Recognition (pp. 60-64). IEEE.&lt;br/&gt;40.Light, J. (1988). Interaction involving individuals using augmentative and alternative communication systems: State of the art and future directions. Augmentative and Alternative Communication, 4(2), 66-82.&lt;br/&gt;41.Lin, H. F. (2007). Measuring online learning systems success: Applying the updated DeLone and McLean model. Cyberpsychology &amp;amp; behavior, 10(6), 817-820.&lt;br/&gt;42.Lin, L., Chen, S., Shao, Y., &amp;amp; Gu, Z. (2013). Plane-based sampling for ray casting algorithm in sequential medical images. Computational and mathematical methods in medicine, 2013.&lt;br/&gt;43.Lipp, M. J., Riolo, C., Riolo, M., Farkas, J., Liu, T., &amp;amp; Cisneros, G. J. (2016, April). Showing you care: An empathetic approach to doctor–patient communication. In Seminars in Orthodontics. WB Saunders.&lt;br/&gt;44.Livatino, S., De Paolis, L. T., D'Agostino, M., Zocco, A., Agrimi, A., De Santis, A., ... &amp;amp; Lapresa, M. (2015). Stereoscopic visualization and 3-D technologies in medical endoscopic teleoperation. IEEE Transactions on Industrial Electronics, 62(1), 525-535.&lt;br/&gt;45.Lundstrom, C., Rydell, T., Forsell, C., Persson, A., &amp;amp; Ynnerman, A. (2011). Multi-touch table system for medical visualization: Application to orthopedic surgery planning. IEEE Transactions on Visualization and Computer Graphics, 17(12), 1775-1784.&lt;br/&gt;46.Mahmoudi, S. E., Akhondi-Asl, A., Rahmani, R., Faghih-Roohi, S., Taimouri, V., Sabouri, A., &amp;amp; Soltanian-Zadeh, H. (2010). Web-based interactive 2D/3D medical image processing and visualization software. computer methods and programs in biomedicine, 98(2), 172-182.&lt;br/&gt;47.Marcus, S. H., &amp;amp; Tuchfeld, B. S. (1993). Sharing information, sharing responsibility: helping health care consumers make informed decisions. In Proceedings of the Annual Symposium on Computer Application in Medical Care (p. 3). American Medical Informatics Association.&lt;br/&gt;48.Maupu, D., Van Horn, M. H., Weeks, S., &amp;amp; Bullitt, E. (2005). 3D stereo interactive medical visualization. IEEE Computer Graphics and Applications, 25(5), 67-71.&lt;br/&gt;49.McAuliffe, M. J., Lalonde, F. M., McGarry, D., Gandler, W., Csaky, K., &amp;amp; Trus, B. L. (2001). Medical image processing, analysis and visualization in clinical research. In Computer-Based Medical Systems, 2001. CBMS 2001. Proceedings. 14th IEEE Symposium on (pp. 381-386). IEEE.&lt;br/&gt;50.McCandless, D. (2010). The beauty of data visualization. TED website, http://bit. ly/sHXvKc.&lt;br/&gt;51.Meiselwitz, G., &amp;amp; Sadera, W. (2008). Investigating the connection between usability and learning outcomes in online learning environments. Journal of Online Learning and Teaching, 4(2), 9.&lt;br/&gt;52.Ong, L. M., De Haes, J. C., Hoos, A. M., &amp;amp; Lammes, F. B. (1995). Doctor-patient communication: a review of the literature. Social Science &amp;amp; Medicine, 40(7), 903-918.&lt;br/&gt;53.Patel, R. A., Hartzler, A., Pratt, W., Back, A., Czerwinski, M., &amp;amp; Roseway, A. (2013, May). Visual feedback on nonverbal communication: a design exploration with healthcare professionals. In 2013 7th International Conference on Pervasive Computing Technologies for Healthcare and Workshops (pp. 105-112). IEEE.&lt;br/&gt;54.Paternotte, E., van Dulmen, S., van der Lee, N., Scherpbier, A. J., &amp;amp; Scheele, F. (2015). Factors influencing intercultural doctor–patient communication: A realist review. Patient Education and Counseling, 98(4), 420-445.&lt;br/&gt;55.Petter, S., &amp;amp; McLean, E. R. (2009). A meta-analytic assessment of the DeLone and McLean IS success model: An examination of IS success at the individual level. Information &amp;amp; Management, 46(3), 159-166.&lt;br/&gt;56.Robinson, J. D., &amp;amp; Heritage, J. (2005). The structure of patients’ presenting concerns: the completion relevance of current symptoms. Social Science &amp;amp; Medicine, 61(2), 481-493.&lt;br/&gt;57.Rohrer, M. (1997). Seeing is believing: The importance of Visualization in Manufacturing Simulation. IIE Solutions, 29(5), 24-28.&lt;br/&gt;58.Roter, D. L., Hall, J. A., &amp;amp; Katz, N. R. (1987). Relations between physicians' behaviors and analogue patients' satisfaction, recall, and impressions. Medical Care, 437-451.&lt;br/&gt;59.Santhanam, A. P., Imielinska, C., Davenport, P., Kupelian, P., &amp;amp; Rolland, J. P. (2008). Modeling real-time 3-D lung deformations for medical visualization. IEEE Transactions on Information Technology in Biomedicine, 12(2), 257-270.&lt;br/&gt;60.Santhanam, A., Fidopiastis, C., Hamza-Lup, F., Rolland, J. P., &amp;amp; Imielinska, C. (2004). Physically-based deformation of high-resolution 3D lung models for augmented reality based medical visualization. MICCAI AMI-ARCS, 21-32.&lt;br/&gt;61.Satoh, T., Omi, M., Ohsako, C., Katsumata, A., Yoshimoto, Y., Tsuchimoto, S., ... &amp;amp; Date, I. (2005). Visualization of aneurysmal contours and perianeurysmal environment with conventional and transparent 3D MR cisternography. American journal of neuroradiology, 26(2), 313-318.&lt;br/&gt;62.Schendel, S. A., &amp;amp; Lane, C. (2009, March). 3D orthognathic surgery simulation using image fusion. In Seminars in Orthodontics (Vol. 15, No. 1, pp. 48-56). WB Saunders.&lt;br/&gt;63.Shaller, D. V., Sharpe, R. S., &amp;amp; Rubin, R. D. (1998). A national action plan to meet health care quality information needs in the age of managed care. Jama, 279(16), 1254-1258.&lt;br/&gt;64.Stellamanns, J., Ruetters, D., Dahal, K., Schillmoeller, Z., &amp;amp; Huebner, J. (2017). Visualizing risks in cancer communication: A systematic review of computer-supported visual aids. Patient Education and Counseling.&lt;br/&gt;65.Stewart, M. A. (1995). Effective physician-patient communication and health outcomes: a review. CMAJ: Canadian Medical Association Journal, 152(9), 1423.&lt;br/&gt;66.Tatarchuk, N., Shopf, J., &amp;amp; DeCoro, C. (2008). Advanced interactive medical visualization on the GPU. Journal of Parallel and Distributed Computing, 68(10), 1319-1328.&lt;br/&gt;67.Thayaparan, A. J., &amp;amp; Mahdi, E. J. (2013). The Patient Satisfaction Questionnaire Short Form (PSQ-18) as an adaptable, reliable, and validated tool for use in various settings. Medical education online, 18.&lt;br/&gt;68.Van der Feltz-Cornelis, C. M., Van Oppen, P., Van Marwijk, H. W., De Beurs, E., &amp;amp; Van Dyck, R. (2004). A patient-doctor relationship questionnaire (PDRQ-9) in primary care: development and psychometric evaluation. General hospital psychiatry, 26(2), 115-120.&lt;br/&gt;69.Wang, Y. S., &amp;amp; Liao, Y. W. (2008). Assessing eGovernment systems success: A validation of the DeLone and McLean model of information systems success. Government Information Quarterly, 25(4), 717-733.&lt;br/&gt;70.Wright, E. B., Holcombe, C., &amp;amp; Salmon, P. (2004). Doctors' communication of trust, care, and respect in breast cancer: qualitative study. Bmj, 328(7444), 864.&lt;br/&gt;71.Yong, H. W., Bade, A., &amp;amp; Muniandy, R. K. (2015). 3D Reconstruction of Breast cancer from mammograms using volume rendering techniques. Journal Teknologi, 75(2).&lt;br/&gt;&lt;br/&gt;中文文獻&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005909204" target="_blank"&gt;1.丁俐月（民95）。溝通分析理論在醫病關係上的應用。諮商與輔導，249， 36-42。&lt;/a&gt;&lt;br/&gt;2.白信德（民101）。認識”急性闌尾炎”。博仁綜合醫院醫訊，1。取自http://www.pojengh.com.tw/download/PDF/%E5%8D%9A%E4%BB%81%E9%86%AB%E8%A8%8APDF%E6%AA%94/101/6%E6%9C%88%E8%99%9F%E5%8D%9A%E4%BB%81-1.pdf&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22103CGU05392005%22.&amp;amp;searchmode=basic" target="_blank"&gt;3.白昱祥（民104）。基於網頁瀏覽器與WebGL技術之三維醫學影像顯示平台。長庚大學資訊工程學系碩士論文，1-80。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22093NTHU5031092%22.&amp;amp;searchmode=basic" target="_blank"&gt;4.白珊慈（民93）。提升知識再利用效能之知識視覺化技術：以空間知識為例。國立清華大學工業工程與工程管理學系碩士論文，1-180。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22103CCU00392116%22.&amp;amp;searchmode=basic" target="_blank"&gt;5.何雨龍（民105）。研製可顯示深部電極之腦部三維重建系統。國立中正大學資訊工程研究所碩士論文，1-74。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22102NTUS5222018%22.&amp;amp;searchmode=basic" target="_blank"&gt;6.宜安（民103）。3dsmax在建築設計實踐上的應用。國立臺灣科技大學建築系碩士論文，1-61。&lt;/a&gt;&lt;br/&gt;7.尚祚恒（民101）。醫學視覺化資訊設計之探討。設計教育學報，3(3)，1-10。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22101CCU00396044%22.&amp;amp;searchmode=basic" target="_blank"&gt;8.林志明（民102）。使用3D人體模擬系統在醫學美容上的效益評。國立中正大學資訊管理研究所碩士論文，1-37。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22104NCTU5222009%22.&amp;amp;searchmode=basic" target="_blank"&gt;9.林育如（民105）。環境色票的工具流程開發與視覺化。國立交通大學建築研究所碩士論文，1-57。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005609593" target="_blank"&gt;10.林幸玟、李宇芬（民88）。醫病溝通。基層醫學，14(5)，87-88。&lt;/a&gt;&lt;br/&gt;11.林芳如（民94）。小兒科醫師與病人家屬之語言與非語言溝通互動分析：以北縣某區域醫院一位小兒科醫師為例。臺北醫學大學醫學人文研究所學位論文，1-71。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005545718" target="_blank"&gt;12.林綺雲（民86）。醫生與病人的對話: 談醫病溝通差距的影響與因應。諮商與輔導月刊，142，21-23。&lt;/a&gt;&lt;br/&gt;13.林錦春（民98）。小兒腹部急症--腸套疊。高雄醫學大學附設中和紀念醫院小港院區醫療資訊月刊，29(2)。&lt;br/&gt;14.俞宏峰、陳為、陳偉鋒（民103），資料視覺化基礎，資料視覺化。台北市：佳魁資訊股份有限公司，4-19。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006107195" target="_blank"&gt;15.柯巧俐、鄭詩宗（民96）。臺灣的醫病溝通現況與患者的語言人權。臺灣醫界，50(9)，37-39。&lt;/a&gt;&lt;br/&gt;16.洪玉芳（民101）。醫病溝通中以病人誘發、醫師自我修復為主之言談修復機制：以台灣某教學醫院為例。國立成功大學外國語文學系學位論文，1-104。&lt;br/&gt;17.夏菁、陳為、郭方舟（民103），時變資料視覺化，資料視覺化。台北市：佳魁資訊股份有限公司，8-2~8-11。&lt;br/&gt;18.高維禮（民101）。3D空間渲染圖建構流程研究-以室內設計為例。大同大學工業設計學系(所)，1-111。&lt;br/&gt;19.國家實驗研究院（民98）。病情看得見，醫病關係更貼心【3D醫療影像處理軟體MiiL】。國家實驗研究院電子報，第4期。取自http://www.narlabs.org.tw/tw/epaper/section_3/information.php?SECTION_3_ID=25#&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22087NCKU0442128%22.&amp;amp;searchmode=basic" target="_blank"&gt;20.張財榮（民88）。使用VRML軟體元件之3D醫學影像模型重構技術的研究與應用。國立成功大學電機工程學系碩士論文，1-131。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006013987" target="_blank"&gt;21.張曉卉（民96）。創造醫療價值，從「以病人為中心」做起。康健雜誌105期。取自http://www.commonhealth.com.tw/article/article.action?nid=63426&amp;amp;fullpage=true&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005570242" target="_blank"&gt;22.張櫻淳、黃文鴻、蘇喜（民87）。醫院形象定位之研究-以台北市六家醫學中心的家醫科就診民衆為例。中華公共衛生雜誌，17(2)，111-124。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22096ISU05121118%22.&amp;amp;searchmode=basic" target="_blank"&gt;23.曹耿寧（民97）。健康內控、醫病溝通與醫病關係之研究-外向性之調節效果。義守大學管理研究所碩士論文，1-85。&lt;/a&gt;&lt;br/&gt;24.郭文浩（民99）。醫療影像開發工具ITA建立影像處理系統。嘉南藥理科技大學醫務管理研究所碩士論文，1-107。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22104NCTU5222006%22.&amp;amp;searchmode=basic" target="_blank"&gt;25.陳仡竫（民105）。電影劇本架構模型視覺化。國立交通大學建築研究所碩士論文，1-78。&lt;/a&gt;&lt;br/&gt;26.陳育良（民96）。以視覺化技術為基礎之時間知識表達模式。國立清華大學工業工程與工程管理學系學位論文，1-194。&lt;br/&gt;27.陳為（民103），資料視覺化簡介，資料視覺化。台北市：佳魁資訊股份有限公司，1-3~1-8。&lt;br/&gt;28.陳鈞凱(民106)年。最新十大癌症排行 腸癌第9度奪冠。今日新聞NOWNews。民106年5月4日，取自https://tw.news.yahoo.com/%E6%9C%80%E6%96%B0%E5%8D%81%E5%A4%A7%E7%99%8C%E7%97%87%E6%8E%92%E8%A1%8C-%E8%85%B8%E7%99%8C%E7%AC%AC9%E5%BA%A6%E5%A5%AA%E5%86%A0-025012824.html&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22104NTNU5447004%22.&amp;amp;searchmode=basic" target="_blank"&gt;29.陳德雯（民105）。兩性醫病溝通於線上醫療諮詢之初探。國立臺灣師範大學圖書資訊學研究所碩士論文，1-137。&lt;/a&gt;&lt;br/&gt;30.馮筠、崔磊、賀小佈、孫霞、康寶生（民105）。從二維到三維：醫學影像分析及器官三維重建，大陸：科學出版社。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22094ISU05114007%22.&amp;amp;searchmode=basic" target="_blank"&gt;31.黃志華（民95）。三維頭部資料之分割融合與立體呈現。義守大學生物醫學工程學系碩士論文，1-93。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22088CCU00121012%22.&amp;amp;searchmode=basic" target="_blank"&gt;32.黃秀雅（民89）。醫病溝通中第三者角色、影響與因應之分析。國立中正大學企業管理研究所碩士論文，未出版，嘉義，1-130。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22089DYU00030004%22.&amp;amp;searchmode=basic" target="_blank"&gt;33.黃信憲（民90）。影像之分割重建與立體視覺化-以磁振肝門靜脈影像處理為案例。大葉大學工業工程研究所碩士論文，1-120。&lt;/a&gt;&lt;br/&gt;34.楊正仁（民90）。資訊視覺化呈現之發展與挑戰。元智大學資訊工程學系碩士論文。數位典藏與數位學習聯合目錄，291-305。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22098CCU05777051%22.&amp;amp;searchmode=basic" target="_blank"&gt;35.葉世一（民99）。齒顎矯正電腦輔助教學系統。國立中正大學資訊管理所暨醫療資訊管理所碩士論文，1-68。&lt;/a&gt;&lt;br/&gt;36.葉永文（民101）。醫病關係：一種信任問題的考察。《台灣醫學人文學刊》，第十三卷，第一、二期，77-104。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22100CJU00528022%22.&amp;amp;searchmode=basic" target="_blank"&gt;37.鄒筠緹（民101）。以計劃行為理論探討影響醫學生進行醫病溝通之要素。長榮大學醫務管理學系碩士班碩士論文，1-127。&lt;/a&gt;&lt;br/&gt;38.廖垣達（民98）。醫病視覺化輔助溝通系統之研究。立德大學資訊傳播研究所學位論文，1-73。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22098CHPI5112002%22.&amp;amp;searchmode=basic" target="_blank"&gt;39.廖紹宇（民99）。使用CUDA實作立體影像渲染於醫學影像。中華大學生物資訊學系碩士論文，1-45。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22104NKIT5396028%22.&amp;amp;searchmode=basic" target="_blank"&gt;40.廖紹甫（民104）。探索醫病溝通流程輔助支援系統之效益。國立高雄第一科技大學資訊管理研究所碩士論文，1-66。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22099NCIT5428023%22.&amp;amp;searchmode=basic" target="_blank"&gt;41.劉家慶（民100）。3D 賽車遊戲設計與製作。國立勤益科技大學電子工程系碩士論文，1-56。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0004707955" target="_blank"&gt;42.蔡美慧、盧豐華（民90）。適當的回應病人：從言談技巧改善醫病關係。醫學教育，5(3)，245-252。&lt;/a&gt;&lt;br/&gt;43.蔡英傑（民95）。你不能沒腸識：頑固教授的24個腸道保健秘訣。台灣：如何出版社。&lt;br/&gt;44.衛生服利部（民105）。病毒性腸胃炎。衛生福利部疾病管制署。取自http://www.cdc.gov.tw/diseaseinfo.aspx?treeid=82ce806a312cefec&amp;amp;nowtreeid=f0fd5a55bbb6c41a&amp;amp;tid=9FA12F779BF31729&lt;br/&gt;45.衛生福利部國民健康署（民105）。103年癌症登記報告。取自http://www.hpa.gov.tw/Pages/TopicList.aspx?nodeid=269&amp;amp;idx=0&lt;br/&gt;46.衛福部癌症防治組（民105）。衛生福利部公布102年癌症發生資料 大腸癌持續居冠 50-74歲篩檢每21人就有1人發現病變，籲國人快篩檢!。衛生福利部國民健康署。取自http://www.hpa.gov.tw/Bhpnet/Web/News/News.aspx?No=201604150001&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22078NTU02208013%22.&amp;amp;searchmode=basic" target="_blank"&gt;47.鄭麗寶（民79）。醫療過程中人際互動的社會學分析。國立台灣大學社會學研究所碩士論文，1-113。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22090NCU05489085%22.&amp;amp;searchmode=basic" target="_blank"&gt;48.謝爵隆（民91）。虛擬人體大體解剖教學系統之研究。國立中央大學機械工程研究所碩士論文，1-98。&lt;/a&gt;&lt;br/&gt;49.醫護管理處-品質管理股（民105）。醫療爭議調處 促進溝通平台 臺北市政府衛生局創造醫病雙贏。臺北市政府衛生局。取自http://health.gov.taipei/Default.aspx?tabid=36&amp;amp;mid=442&amp;amp;itemid=37696&lt;br/&gt;50.顏淑芬（民89）。淺談胃炎及其保健之道。高雄榮總醫院醫訊文章，3(10)。取自http://cms03p.vghks.gov.tw/periodical/asp/article.asp?per_no=031013&lt;br/&gt;51.羅賴鈞（民98）。醫學影像之三維顯示與骨組織三角網格重建技術探討。國立中央大學機械工程研究所碩士論文，1-157。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006527997" target="_blank"&gt;52.蘇豐裕、王嘉男、林谷鴻（民97）。ERP 系統使用者滿意度之研究-以 F 公司爲例。工程科技與教育學刊，5(3)，497-520。&lt;/a&gt;&lt;br/&gt;53.鐘國彪（民77）。公保門診醫師與病人互動之研究：病人滿意度和遵醫囑服藥情形的探討。陽明大學公共衛生研究所碩士論文，1-246。&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA13" t="inlineStr">
+      <c r="Z13" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/74kg29</t>
         </is>
@@ -2261,35 +2243,34 @@
           <t>Smart Parking、Mobile Device、Action Research、Interaction Design、Mobile Application Design</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>點閱:478</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>點閱:478</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 現今由於交通工具的成長十分之快速，相對的造成停車場一地難尋，因此停 車的需求十分的迫切。雖然有許多的智慧停車 APP 如雨後春筍般出來，但是市 面上有許多 APP 因為設計不佳的關係導致了 APP 與使用者的互動性不良。本研 究透過行動研究來讓智慧停車 APP 開發者了解如何使用互動性的設計準則以及 市面上的 APP，來開發出一個讓使用者與 APP 之間有著更高互動性的智慧停車 APP，研究中透過與使用者的訪談以及評量等方式來進行系統評量。本研究發現 螢幕大小、畫面配色、即時訊息以及資訊提供等方面在物聯網應用時，會影響到 使用者對於 APP 的互動性，希望除透過本研究的結果來提升 APP 的設計品質外， 也能夠增加未來 APP 與使用者的互動性。</t>
         </is>
       </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>&lt;div style="padding:10px;text-align:left;"&gt;
+中文文獻&lt;br/&gt;小松原明哲(1992)。對話型認知人間工學設計。東京:技報堂出版。 王石番(1989)。傳播內容分析法-理論與實證。台北:幼獅文化。 王琮惠(2007)。質性研究的信度與效度。&lt;br/&gt;黃光玉、劉念夏、陳清文(譯)(2004)。媒介與傳播研究方法:質化與量化途徑。 台北:風雲論壇。(原著:Arthur Asa Berger, Media and Communication Research Methods)&lt;br/&gt;陳建雄(譯) (2006)。互動設計:跨越人-電腦互動。台北:全華。(原著:Jennifer Preece, Yvonne Rogers, Helen Sharp)&lt;br/&gt;賴錦慧(譯)(2010)。人機介面設計第五版。台北:東華出版社。(原著 Shneiderman &amp;amp; Plaisant(2009)&lt;br/&gt;&lt;br/&gt;英文文獻&lt;br/&gt;Abolfazli, S., Sanaei, Z., Gani, A., Xia, F., &amp;amp; Yang, L. T. (2014). Rich mobile applications: genesis, taxonomy, and open issues. Journal of Network and Computer Applications, 40, 345-362.&lt;br/&gt;Adams, F. M. and Osgood, C. E., 1973, “A cross-cultural study of the affective meanings of color.” Journal of Cross-Cultural Psychology, 4(2), 135-156.&lt;br/&gt;Alba, J., Lynch, J., Weitz, B., Janiszewski, C., Lutz, R., Sawyer, A. and Wood, S. (1997). Interactive home shopping: consumer, retailer, and manufacturer incentives to participate in electronic marketplaces. Journal of Marketing, 61(3), 38-53.&lt;br/&gt;Allam, S., Flowerday, S. V., &amp;amp; Flowerday, E. (2014). Smartphone information security awareness: A victim of operational pressures. Computers &amp;amp; Security, 42, 56–65.&lt;br/&gt;Altrichter, H., Posch, P., &amp;amp; Somekh, B. (1993). Teachers investigate their work: An introduction to the methods of action research. Psychology Press.&lt;br/&gt;Arnott, R., &amp;amp; Inci, E. (2006). An integrated model of downtown parking and traffic congestion. Journal of Urban Economics, 60(3), 418-442.&lt;br/&gt;Balasubramanian, S., Peterson, R. A., &amp;amp; Jarvenpaa, S. L. (2002). Exploring the implica- tions of m-commerce for markets and marketing. Journal of the Academy of Marketing Science, 30(4), 348–361.&lt;br/&gt;Ballagas, R., Borchers, J., Rohs, M., &amp;amp; Sheridan, J. G. (2006). The smart phone: a ubiquitous input device. IEEE Pervasive Computing, 5(1), 70-77.&lt;br/&gt;Bangor, A. (2009) Determining what individual SUS scores mean: Adding an adjective rating scale.Journal of Usability Studies, 114-123&lt;br/&gt;Barnes, S. J. (2002). Wireless digital advertising: nature and implications. International Journal of Advertising, 21(3), 399-420.&lt;br/&gt;Baskerville, R., &amp;amp; Myers, M. D. (2004). Special issue on action research in information systems: Making IS research relevant to practice: Foreword. MIS Quarterly, 28(3), 329-335.&lt;br/&gt;Bauer, H. H., Reichardt, T., Barnes, S. J., &amp;amp; Neumann, M. M. (2005). Driving consumer acceptance of mobile marketing: A theoretical framework and empirical study. Journal of electronic commerce research, 6(3), 181.&lt;br/&gt;Bezjian-Avery, A., Calder, B., &amp;amp; Iacobucci, D. (1998). New media interactive advertising vs. traditional advertising. Journal of advertising research, 38, 23-32.&lt;br/&gt;Broekhuizen, T., &amp;amp; Hoffmann, A. (2012). Interactivity perceptions and online newspaper preference. Journal of Interactive Advertising, 12(2), 29-43.&lt;br/&gt;Brooke, J. (1986). System usability scale (SUS): a quick-and-dirty method of system evaluation user information. Reading, UK: Digital Equipment Co Ltd.&lt;br/&gt;Chang, Y. F., Chen, C. S., &amp;amp; Zhou, H. (2009). Smart phone for mobile commerce. Computer Standards &amp;amp; Interfaces, 31(4), 740-747.&lt;br/&gt;Chen, K., &amp;amp; Yen, D. C. (2004). Improving the quality of online presence through interactivity. Information &amp;amp; Management, 42(1), 217-226.&lt;br/&gt;Cheong, S. N., Ling, H. C., &amp;amp; Teh, P. L. (2014). Secure encrypted steganography graphical password scheme for near field communication smartphone access control system. Expert Systems with Applications, 41(7), 3561–3568.&lt;br/&gt;Cheung, S. Y., &amp;amp; Varaiya, P. P. (2007). Traffic surveillance by wireless sensor networks: Final report. California PATH Program, Institute of Transportation Studies, University of California at Berkeley.&lt;br/&gt;Chhablani, J., Kaja, S., &amp;amp; Shah, V. A. (2012). Smartphones in ophthalmology. Indian Journal of Ophthalmology, 60(2), 127–131.&lt;br/&gt;Chou, S. Y., Lin, S. W., &amp;amp; Li, C. C. (2008). Dynamic parking negotiation and guidance using an agent-based platform. Expert Systems with Applications, 35(3), 805-817.&lt;br/&gt;Chung, K. S., &amp;amp; Lee, J. E. (2012). Design and development of m-learning service based on 3G cellular phones. Journal of Information Process Systems, 8(3), 521–538.&lt;br/&gt;Cusumano, M. A. (2010). Platforms and services: Understanding the resurgence of Ap- ple. Communications of the ACM, 53(10), 22–24.&lt;br/&gt;Cyr, D., Head, M., &amp;amp; Ivanov, A. (2009). Perceived interactivity leading to e-loyalty: Development of a model for cognitive–affective user responses. International Journal of Human-computer studies, 67(10), 850-869.&lt;br/&gt;Davis, G. B. (2002). Anytime/anyplace computing and the future of knowledge work. Communications of the ACM, 45(12), 67-73.&lt;br/&gt;Day, G. S. (1998). Organizing for interactivity. Journal of Interactive Marketing, 12(1), 47-53.&lt;br/&gt;Deighton, J. (1996). The future of interactive marketing. Harvard Business Review, 74(6), 151-160.&lt;br/&gt;Dholakia, R. R., Zhao, M., Dholakia, N., &amp;amp; Fortin, D. (2000). Interactivity and revisits to websites: A theoretical framework. In American Marketing Association. Conference Proceedings 12, 108.&lt;br/&gt;Displays, V. (1983). Work, and Vision, National Research Council.&lt;br/&gt;Emmanouilidis, C., Koutsiamanis, R. A., &amp;amp; Tasidou, A. (2013). Mobile guides: Taxonomy of architectures, context awareness, technologies and applications. Journal of Network and Computer Applications, 36(1), 103-125.&lt;br/&gt;Fortin, D. R. (1997). The impact of interactivity on advertising effectiveness in the new media. Unpublished Dissertation.&lt;br/&gt;Fortin, D. R., &amp;amp; Dholakia, R. R. (2005). Interactivity and vividness effects on social presence and involvement with a web-based advertisement. Journal of business research, 58(3), 387-396.&lt;br/&gt;Fraternali, P., Rossi, G., &amp;amp; Sánchez-Figueroa, F. (2010). Rich internet applications. IEEE Internet Computing, 14(3), 9-12.&lt;br/&gt;Galitz, W. O. (2007). The essential guide to user interface design: An introduction to GUI design principles and techniques. Indianapolis, IN: Wiley&lt;br/&gt;Gao, Q., Rau, P. L. P., &amp;amp; Salvendy, G. (2009). Perception of interactivity: Affects of four key variables in mobile advertising. International Journal of Human- Computer Interaction, 25(6), 479-505.&lt;br/&gt;Ghose, S., &amp;amp; Dou, W. (1998). Interactive functions and their impacts on the appeal of Internet presence sites. Journal of Advertising research, 38, 29-44.&lt;br/&gt;Grade rankings of SUS scores from “Determining What Individual SUS Scores Mean: Adding an Adjective Rating Scale,” by A. Bangor, P.T. Kortum, and J.T. Miller, 2009, Journal of Usability Studies, 4(3), 114-123. Reprinted with permission.&lt;br/&gt;Grodi, R., Rawat, D. B., &amp;amp; Rios-Gutierrez, F. (2016). Smart parking: Parking occupancy monitoring and visualization system for smart cities. 1-5. IEEE.&lt;br/&gt;Ha, L., &amp;amp; James, E. L. (1998). Interactivity reexamined: A baseline analysis of early business web sites. Journal of Broadcasting &amp;amp; Electronic Media, 42(4), 457-474.&lt;br/&gt;Hair, J. F., Ringle, C. M., &amp;amp; Sarstedt, M. (2011). PLS-SEM: Indeed a silver bullet. Journal of Marketing theory and Practice, 19(2), 139-152.&lt;br/&gt;Hamka, F., Bouwman, H., de Reuver, M., &amp;amp; Kroesen, M. (2014). Mobile customer segmentation based on smartphone measurement. Telematics and Informatics, 31(2), 220–227.&lt;br/&gt;Hess, T., Fuller, M., &amp;amp; Campbell, D. (2009). Designing interfaces with social presence: Using vividness and extraversion to create social recommendation agents. Journal of the Association for Information Systems, 10(12), 889.&lt;br/&gt;Hodel, T. B., &amp;amp; Cong, S. (2003). Parking space optimization services, a uniformed web application architecture. In ITS World Congress Proceedings, 16-20.&lt;br/&gt;Hoffman, D. L., &amp;amp; Novak, T. P. (1996). Marketing in hypermedia computer-mediated environments: Conceptual foundations. The Journal of Marketing, 50-68.&lt;br/&gt;Hsu, J. S. C. (2014). Understanding the role of satisfaction in the formation of perceived switching value. Decision Support Systems, 59, 152–162.&lt;br/&gt;Hwang, R. J., Shiau, S. H., &amp;amp; Jan, D. F. (2007). A new mobile payment scheme for roaming services. Electronic Commerce Research and Applications, 6(2), 184-191.&lt;br/&gt;Idris, M. Y. I., Leng, Y. Y., Tamil, E. M., Noor, N. M., &amp;amp; Razak, Z. (2009). Саг park system: a review of smart parking system and its technology. Inf. Technol. J, 8(2), 101-113.&lt;br/&gt;Jensen, J. F. (1999). Interactivity'-Tracking a New Concept in Media and Communication Studies. Computer Media and Communication.&lt;br/&gt;Johnson, J. (2000). Gui bookers: Don’t and do’s for software developers and web designers. MA: Morgan Kaufmann.&lt;br/&gt;Kannan, P. K., Chang, A. M., &amp;amp; Whinston, A. B. (2001). Wireless commerce: marketing issues and possibilities. Proceedings of the 34th Annual Hawaii International Conference on IEEE.&lt;br/&gt;Kinney, J. A. S., Neri, D. F., Mercado, D. T., &amp;amp; Ryan, A. P. (1983). Visual Fatigue In Sonar Control Rooms Lighted By Red, White, Or Blue Illumination.&lt;br/&gt;Ko, E., Kim, E. Y., &amp;amp; Lee, E. K. (2009). Modeling consumer adoption of mobile shopping for fashion products in Korea. Psychology and Marketing, 26(7), 669- 687.&lt;br/&gt;Kwon, Y., Kang, K., &amp;amp; Bae, C. (2014). Unsupervised learning for human activity recognition using smartphone sensors. Expert Systems with Applications, 41(14), 6067–6074.&lt;br/&gt;Lee, C. H., Wen, M. G., Han, C. C., &amp;amp; Kou, D. C. (2005). An automatic monitoring approach for unsupervised parking lots in outdoors. IEEE. In Proceedings 39th Annual 2005 International Carnahan Conference on Security Technology, 271- 274.&lt;br/&gt;Lee, J. S., &amp;amp; Hoh, B. (2010). Sell your experiences: a market mechanism based incentive for participatory sensing. In Pervasive Computing and Communications (PerCom), 2010 IEEE International Conference, 60-68.&lt;br/&gt;Lee, S. J., Lee, W. N., Kim, H., &amp;amp; Stout, P. A. (2004). A comparison of objective characteristics and user perception of web sites. Journal of Interactive Advertising, 4(2), 61-75.&lt;br/&gt;Lewin, K. (1946). Action research and minority problems. Journal of social issues, 2(4), 34-46.&lt;br/&gt;Li, D., Serizawa, Y., &amp;amp; Kiuchi, M. (2002, October). Extension of client-server applications to the Internet. IEEE Region 10 Conference on Computers, Communications, Control and Power Engineering, 1,355-358.&lt;br/&gt;Lin, F., &amp;amp; Ye, W. (2009). Operating system battle in the ecosystem of smartphone industry. Paper presented at the International Symposium on Information Engineering and Electronic Commerce&lt;br/&gt;Lindgren, R., Henfridsson, O., &amp;amp; Schultze, U. (2004). Design principles for competence management systems: a synthesis of an action research study. MIS Quarterly, 435- 472&lt;br/&gt;Liu, Y., &amp;amp; Shrum, L. J. (2002). What is interactivity and is it always such a good thing? Implications of definition, person, and situation for the influence of interactivity on advertising effectiveness. Journal of Advertising, 31(4), 53-64.&lt;br/&gt;Liu, Y. (2003). Developing a scale to measure the interactivity of websites. Journal of advertising research, 43(02), 207-216.&lt;br/&gt;Malykhina, A. P. (2007). Neural mechanisms of pelvic organ cross-sensitization. Neuroscience, 149(3), 660-672.&lt;br/&gt;Mahnke, F. H., &amp;amp; Mahnke, R. H. (1987). Color and light in man-made environments. New York: Van Nostrand Reinhold.&lt;br/&gt;Masaki, I. (1998). Machine-vision systems for intelligent transportation systems. IEEE Intelligent systems, 13(6), 24-31.&lt;br/&gt;McGill, I., &amp;amp; Beaty, L. (1992). Action Learning: A Practioner’s Guide.&lt;br/&gt;Mckernan, J.(1991). Curriculum action research:A handbook of methods and&lt;br/&gt;resources for the reflective practitioner, NY:St. Martin’ s Press Inc.&lt;br/&gt;McMillan, S. J., &amp;amp; Hwang, J. S. (2002). Measures of perceived interactivity: An exploration of the role of direction of communication, user control, and time in shaping perceptions of interactivity. Journal of Advertising, 31(3), 29-42.&lt;br/&gt;McNiff, J. L. P. &amp;amp; Whitehead, J.(1996) You and your action research project. London: Toutledge.&lt;br/&gt;Mimbela, L. E. Y., &amp;amp; Klein, L. A. (2000). Summary of vehicle detection and surveillance technologies used in intelligent transportation systems.&lt;br/&gt;Monzon, A. (2015). Smart cities concept and challenges: Bases for the assessment of smart city projects. In International Conference on Smart Cities and Green ICT Systems,17-31. Springer International Publishing.&lt;br/&gt;Newhagen, J.E., J.W. Cordes, and M.R. Levy (1995). Nightly@nbc.com: Audience Scope and the Perception of Interactivity in Viewer Mail on the Internet. Journal of Communication 45(3), 164–75.&lt;br/&gt;Nielsen, J. (1993). Usability engineering. San Francisco, CA: Morgan Kaufmann Publishers Inc.&lt;br/&gt;Nielsen, J., &amp;amp; Loranger, H. (2006). Prioritizing web usability. Pearson Education. Norman, K. L. (1991). The psychology of menu selection: Designing cognitive control&lt;br/&gt;at the human computer interface. Intellect Books.&lt;br/&gt;Norman, D. A. (2013). The design of everyday things: Revised and expanded edition.&lt;br/&gt;Basic books.&lt;br/&gt;Norman, D. A. (1983). Some observations on mental models. Mental models, 7(112), 7-14.&lt;br/&gt;Norman, D. A. (1986). Cognitive engineering. User centered system design: New perspectives on human-computer interaction, 3161.&lt;br/&gt;Norman, D. A. (1988). The Design of Everyday Things. Originally published: The psychology of everyday things.&lt;br/&gt;Okazaki, S., &amp;amp; Mendez, F. (2013). Perceived ubiquity in mobile services. Journal of Interactive Marketing, 27(2), 98-111.&lt;br/&gt;Oulasvirta, A., Raento, M., &amp;amp; Tiitta, S. (2005). ContextContacts: re-designing SmartPhone's contact book to support mobile awareness and collaboration. In Proceedings of the 7th international conference on Human computer interaction with mobile devices &amp;amp; services, 167-174.&lt;br/&gt;Oulasvirta, A., Petit, R., Raento, M., &amp;amp; Tiitta, S. (2007). Interpreting and acting on mobile awareness cues. Human–Computer Interaction, 22(1-2), 97-135.&lt;br/&gt;Pitt, L. F., Parent, M., Junglas, I., Chan, A., &amp;amp; Spyropoulou, S. (2011). Integrating the smartphone into a sound environmental information systems strategy: Principles, practices and a research agenda. Journal of Strategic Information Systems, 20 (1), 27–37.&lt;br/&gt;Polycarpou, E., Lambrinos, L., &amp;amp; Protopapadakis, E. (2013). Smart parking solutions for urban areas. In World of Wireless, Mobile and Multimedia Networks (WoWMoM), 2013 IEEE 14th International Symposium and Workshops, 1-6.&lt;br/&gt;Preece, J. (1993). A Guide to Usability: human factors in computing. Addison Wesley, the Open University.&lt;br/&gt;Rafaeli, S. (1988). Interactivity: From new media to communication. InR. P. Hawkins, JM Wiemann, &amp;amp; S. Pingree (Eds.), Advancing communication science: Merging mass and interpersonal processes, 110-134.&lt;br/&gt;Rafaeli, S., &amp;amp; Sudweeks, F. (1997). Networked interactivity. Journal of Computer- Mediated Communication, 2(4).&lt;br/&gt;Rogers, Y., Sharp, H., Preece, J., &amp;amp; Tepper, M. (2007). Interaction design: beyond human-computer interaction. netWorker: The Craf&lt;/div&gt;</t>
+        </is>
+      </c>
       <c r="Z14" t="inlineStr">
-        <is>
-          <t>&lt;div style="padding:10px;text-align:left;"&gt;
-中文文獻&lt;br/&gt;小松原明哲(1992)。對話型認知人間工學設計。東京:技報堂出版。 王石番(1989)。傳播內容分析法-理論與實證。台北:幼獅文化。 王琮惠(2007)。質性研究的信度與效度。&lt;br/&gt;黃光玉、劉念夏、陳清文(譯)(2004)。媒介與傳播研究方法:質化與量化途徑。 台北:風雲論壇。(原著:Arthur Asa Berger, Media and Communication Research Methods)&lt;br/&gt;陳建雄(譯) (2006)。互動設計:跨越人-電腦互動。台北:全華。(原著:Jennifer Preece, Yvonne Rogers, Helen Sharp)&lt;br/&gt;賴錦慧(譯)(2010)。人機介面設計第五版。台北:東華出版社。(原著 Shneiderman &amp;amp; Plaisant(2009)&lt;br/&gt;&lt;br/&gt;英文文獻&lt;br/&gt;Abolfazli, S., Sanaei, Z., Gani, A., Xia, F., &amp;amp; Yang, L. T. (2014). Rich mobile applications: genesis, taxonomy, and open issues. Journal of Network and Computer Applications, 40, 345-362.&lt;br/&gt;Adams, F. M. and Osgood, C. E., 1973, “A cross-cultural study of the affective meanings of color.” Journal of Cross-Cultural Psychology, 4(2), 135-156.&lt;br/&gt;Alba, J., Lynch, J., Weitz, B., Janiszewski, C., Lutz, R., Sawyer, A. and Wood, S. (1997). Interactive home shopping: consumer, retailer, and manufacturer incentives to participate in electronic marketplaces. Journal of Marketing, 61(3), 38-53.&lt;br/&gt;Allam, S., Flowerday, S. V., &amp;amp; Flowerday, E. (2014). Smartphone information security awareness: A victim of operational pressures. Computers &amp;amp; Security, 42, 56–65.&lt;br/&gt;Altrichter, H., Posch, P., &amp;amp; Somekh, B. (1993). Teachers investigate their work: An introduction to the methods of action research. Psychology Press.&lt;br/&gt;Arnott, R., &amp;amp; Inci, E. (2006). An integrated model of downtown parking and traffic congestion. Journal of Urban Economics, 60(3), 418-442.&lt;br/&gt;Balasubramanian, S., Peterson, R. A., &amp;amp; Jarvenpaa, S. L. (2002). Exploring the implica- tions of m-commerce for markets and marketing. Journal of the Academy of Marketing Science, 30(4), 348–361.&lt;br/&gt;Ballagas, R., Borchers, J., Rohs, M., &amp;amp; Sheridan, J. G. (2006). The smart phone: a ubiquitous input device. IEEE Pervasive Computing, 5(1), 70-77.&lt;br/&gt;Bangor, A. (2009) Determining what individual SUS scores mean: Adding an adjective rating scale.Journal of Usability Studies, 114-123&lt;br/&gt;Barnes, S. J. (2002). Wireless digital advertising: nature and implications. International Journal of Advertising, 21(3), 399-420.&lt;br/&gt;Baskerville, R., &amp;amp; Myers, M. D. (2004). Special issue on action research in information systems: Making IS research relevant to practice: Foreword. MIS Quarterly, 28(3), 329-335.&lt;br/&gt;Bauer, H. H., Reichardt, T., Barnes, S. J., &amp;amp; Neumann, M. M. (2005). Driving consumer acceptance of mobile marketing: A theoretical framework and empirical study. Journal of electronic commerce research, 6(3), 181.&lt;br/&gt;Bezjian-Avery, A., Calder, B., &amp;amp; Iacobucci, D. (1998). New media interactive advertising vs. traditional advertising. Journal of advertising research, 38, 23-32.&lt;br/&gt;Broekhuizen, T., &amp;amp; Hoffmann, A. (2012). Interactivity perceptions and online newspaper preference. Journal of Interactive Advertising, 12(2), 29-43.&lt;br/&gt;Brooke, J. (1986). System usability scale (SUS): a quick-and-dirty method of system evaluation user information. Reading, UK: Digital Equipment Co Ltd.&lt;br/&gt;Chang, Y. F., Chen, C. S., &amp;amp; Zhou, H. (2009). Smart phone for mobile commerce. Computer Standards &amp;amp; Interfaces, 31(4), 740-747.&lt;br/&gt;Chen, K., &amp;amp; Yen, D. C. (2004). Improving the quality of online presence through interactivity. Information &amp;amp; Management, 42(1), 217-226.&lt;br/&gt;Cheong, S. N., Ling, H. C., &amp;amp; Teh, P. L. (2014). Secure encrypted steganography graphical password scheme for near field communication smartphone access control system. Expert Systems with Applications, 41(7), 3561–3568.&lt;br/&gt;Cheung, S. Y., &amp;amp; Varaiya, P. P. (2007). Traffic surveillance by wireless sensor networks: Final report. California PATH Program, Institute of Transportation Studies, University of California at Berkeley.&lt;br/&gt;Chhablani, J., Kaja, S., &amp;amp; Shah, V. A. (2012). Smartphones in ophthalmology. Indian Journal of Ophthalmology, 60(2), 127–131.&lt;br/&gt;Chou, S. Y., Lin, S. W., &amp;amp; Li, C. C. (2008). Dynamic parking negotiation and guidance using an agent-based platform. Expert Systems with Applications, 35(3), 805-817.&lt;br/&gt;Chung, K. S., &amp;amp; Lee, J. E. (2012). Design and development of m-learning service based on 3G cellular phones. Journal of Information Process Systems, 8(3), 521–538.&lt;br/&gt;Cusumano, M. A. (2010). Platforms and services: Understanding the resurgence of Ap- ple. Communications of the ACM, 53(10), 22–24.&lt;br/&gt;Cyr, D., Head, M., &amp;amp; Ivanov, A. (2009). Perceived interactivity leading to e-loyalty: Development of a model for cognitive–affective user responses. International Journal of Human-computer studies, 67(10), 850-869.&lt;br/&gt;Davis, G. B. (2002). Anytime/anyplace computing and the future of knowledge work. Communications of the ACM, 45(12), 67-73.&lt;br/&gt;Day, G. S. (1998). Organizing for interactivity. Journal of Interactive Marketing, 12(1), 47-53.&lt;br/&gt;Deighton, J. (1996). The future of interactive marketing. Harvard Business Review, 74(6), 151-160.&lt;br/&gt;Dholakia, R. R., Zhao, M., Dholakia, N., &amp;amp; Fortin, D. (2000). Interactivity and revisits to websites: A theoretical framework. In American Marketing Association. Conference Proceedings 12, 108.&lt;br/&gt;Displays, V. (1983). Work, and Vision, National Research Council.&lt;br/&gt;Emmanouilidis, C., Koutsiamanis, R. A., &amp;amp; Tasidou, A. (2013). Mobile guides: Taxonomy of architectures, context awareness, technologies and applications. Journal of Network and Computer Applications, 36(1), 103-125.&lt;br/&gt;Fortin, D. R. (1997). The impact of interactivity on advertising effectiveness in the new media. Unpublished Dissertation.&lt;br/&gt;Fortin, D. R., &amp;amp; Dholakia, R. R. (2005). Interactivity and vividness effects on social presence and involvement with a web-based advertisement. Journal of business research, 58(3), 387-396.&lt;br/&gt;Fraternali, P., Rossi, G., &amp;amp; Sánchez-Figueroa, F. (2010). Rich internet applications. IEEE Internet Computing, 14(3), 9-12.&lt;br/&gt;Galitz, W. O. (2007). The essential guide to user interface design: An introduction to GUI design principles and techniques. Indianapolis, IN: Wiley&lt;br/&gt;Gao, Q., Rau, P. L. P., &amp;amp; Salvendy, G. (2009). Perception of interactivity: Affects of four key variables in mobile advertising. International Journal of Human- Computer Interaction, 25(6), 479-505.&lt;br/&gt;Ghose, S., &amp;amp; Dou, W. (1998). Interactive functions and their impacts on the appeal of Internet presence sites. Journal of Advertising research, 38, 29-44.&lt;br/&gt;Grade rankings of SUS scores from “Determining What Individual SUS Scores Mean: Adding an Adjective Rating Scale,” by A. Bangor, P.T. Kortum, and J.T. Miller, 2009, Journal of Usability Studies, 4(3), 114-123. Reprinted with permission.&lt;br/&gt;Grodi, R., Rawat, D. B., &amp;amp; Rios-Gutierrez, F. (2016). Smart parking: Parking occupancy monitoring and visualization system for smart cities. 1-5. IEEE.&lt;br/&gt;Ha, L., &amp;amp; James, E. L. (1998). Interactivity reexamined: A baseline analysis of early business web sites. Journal of Broadcasting &amp;amp; Electronic Media, 42(4), 457-474.&lt;br/&gt;Hair, J. F., Ringle, C. M., &amp;amp; Sarstedt, M. (2011). PLS-SEM: Indeed a silver bullet. Journal of Marketing theory and Practice, 19(2), 139-152.&lt;br/&gt;Hamka, F., Bouwman, H., de Reuver, M., &amp;amp; Kroesen, M. (2014). Mobile customer segmentation based on smartphone measurement. Telematics and Informatics, 31(2), 220–227.&lt;br/&gt;Hess, T., Fuller, M., &amp;amp; Campbell, D. (2009). Designing interfaces with social presence: Using vividness and extraversion to create social recommendation agents. Journal of the Association for Information Systems, 10(12), 889.&lt;br/&gt;Hodel, T. B., &amp;amp; Cong, S. (2003). Parking space optimization services, a uniformed web application architecture. In ITS World Congress Proceedings, 16-20.&lt;br/&gt;Hoffman, D. L., &amp;amp; Novak, T. P. (1996). Marketing in hypermedia computer-mediated environments: Conceptual foundations. The Journal of Marketing, 50-68.&lt;br/&gt;Hsu, J. S. C. (2014). Understanding the role of satisfaction in the formation of perceived switching value. Decision Support Systems, 59, 152–162.&lt;br/&gt;Hwang, R. J., Shiau, S. H., &amp;amp; Jan, D. F. (2007). A new mobile payment scheme for roaming services. Electronic Commerce Research and Applications, 6(2), 184-191.&lt;br/&gt;Idris, M. Y. I., Leng, Y. Y., Tamil, E. M., Noor, N. M., &amp;amp; Razak, Z. (2009). Саг park system: a review of smart parking system and its technology. Inf. Technol. J, 8(2), 101-113.&lt;br/&gt;Jensen, J. F. (1999). Interactivity'-Tracking a New Concept in Media and Communication Studies. Computer Media and Communication.&lt;br/&gt;Johnson, J. (2000). Gui bookers: Don’t and do’s for software developers and web designers. MA: Morgan Kaufmann.&lt;br/&gt;Kannan, P. K., Chang, A. M., &amp;amp; Whinston, A. B. (2001). Wireless commerce: marketing issues and possibilities. Proceedings of the 34th Annual Hawaii International Conference on IEEE.&lt;br/&gt;Kinney, J. A. S., Neri, D. F., Mercado, D. T., &amp;amp; Ryan, A. P. (1983). Visual Fatigue In Sonar Control Rooms Lighted By Red, White, Or Blue Illumination.&lt;br/&gt;Ko, E., Kim, E. Y., &amp;amp; Lee, E. K. (2009). Modeling consumer adoption of mobile shopping for fashion products in Korea. Psychology and Marketing, 26(7), 669- 687.&lt;br/&gt;Kwon, Y., Kang, K., &amp;amp; Bae, C. (2014). Unsupervised learning for human activity recognition using smartphone sensors. Expert Systems with Applications, 41(14), 6067–6074.&lt;br/&gt;Lee, C. H., Wen, M. G., Han, C. C., &amp;amp; Kou, D. C. (2005). An automatic monitoring approach for unsupervised parking lots in outdoors. IEEE. In Proceedings 39th Annual 2005 International Carnahan Conference on Security Technology, 271- 274.&lt;br/&gt;Lee, J. S., &amp;amp; Hoh, B. (2010). Sell your experiences: a market mechanism based incentive for participatory sensing. In Pervasive Computing and Communications (PerCom), 2010 IEEE International Conference, 60-68.&lt;br/&gt;Lee, S. J., Lee, W. N., Kim, H., &amp;amp; Stout, P. A. (2004). A comparison of objective characteristics and user perception of web sites. Journal of Interactive Advertising, 4(2), 61-75.&lt;br/&gt;Lewin, K. (1946). Action research and minority problems. Journal of social issues, 2(4), 34-46.&lt;br/&gt;Li, D., Serizawa, Y., &amp;amp; Kiuchi, M. (2002, October). Extension of client-server applications to the Internet. IEEE Region 10 Conference on Computers, Communications, Control and Power Engineering, 1,355-358.&lt;br/&gt;Lin, F., &amp;amp; Ye, W. (2009). Operating system battle in the ecosystem of smartphone industry. Paper presented at the International Symposium on Information Engineering and Electronic Commerce&lt;br/&gt;Lindgren, R., Henfridsson, O., &amp;amp; Schultze, U. (2004). Design principles for competence management systems: a synthesis of an action research study. MIS Quarterly, 435- 472&lt;br/&gt;Liu, Y., &amp;amp; Shrum, L. J. (2002). What is interactivity and is it always such a good thing? Implications of definition, person, and situation for the influence of interactivity on advertising effectiveness. Journal of Advertising, 31(4), 53-64.&lt;br/&gt;Liu, Y. (2003). Developing a scale to measure the interactivity of websites. Journal of advertising research, 43(02), 207-216.&lt;br/&gt;Malykhina, A. P. (2007). Neural mechanisms of pelvic organ cross-sensitization. Neuroscience, 149(3), 660-672.&lt;br/&gt;Mahnke, F. H., &amp;amp; Mahnke, R. H. (1987). Color and light in man-made environments. New York: Van Nostrand Reinhold.&lt;br/&gt;Masaki, I. (1998). Machine-vision systems for intelligent transportation systems. IEEE Intelligent systems, 13(6), 24-31.&lt;br/&gt;McGill, I., &amp;amp; Beaty, L. (1992). Action Learning: A Practioner’s Guide.&lt;br/&gt;Mckernan, J.(1991). Curriculum action research:A handbook of methods and&lt;br/&gt;resources for the reflective practitioner, NY:St. Martin’ s Press Inc.&lt;br/&gt;McMillan, S. J., &amp;amp; Hwang, J. S. (2002). Measures of perceived interactivity: An exploration of the role of direction of communication, user control, and time in shaping perceptions of interactivity. Journal of Advertising, 31(3), 29-42.&lt;br/&gt;McNiff, J. L. P. &amp;amp; Whitehead, J.(1996) You and your action research project. London: Toutledge.&lt;br/&gt;Mimbela, L. E. Y., &amp;amp; Klein, L. A. (2000). Summary of vehicle detection and surveillance technologies used in intelligent transportation systems.&lt;br/&gt;Monzon, A. (2015). Smart cities concept and challenges: Bases for the assessment of smart city projects. In International Conference on Smart Cities and Green ICT Systems,17-31. Springer International Publishing.&lt;br/&gt;Newhagen, J.E., J.W. Cordes, and M.R. Levy (1995). Nightly@nbc.com: Audience Scope and the Perception of Interactivity in Viewer Mail on the Internet. Journal of Communication 45(3), 164–75.&lt;br/&gt;Nielsen, J. (1993). Usability engineering. San Francisco, CA: Morgan Kaufmann Publishers Inc.&lt;br/&gt;Nielsen, J., &amp;amp; Loranger, H. (2006). Prioritizing web usability. Pearson Education. Norman, K. L. (1991). The psychology of menu selection: Designing cognitive control&lt;br/&gt;at the human computer interface. Intellect Books.&lt;br/&gt;Norman, D. A. (2013). The design of everyday things: Revised and expanded edition.&lt;br/&gt;Basic books.&lt;br/&gt;Norman, D. A. (1983). Some observations on mental models. Mental models, 7(112), 7-14.&lt;br/&gt;Norman, D. A. (1986). Cognitive engineering. User centered system design: New perspectives on human-computer interaction, 3161.&lt;br/&gt;Norman, D. A. (1988). The Design of Everyday Things. Originally published: The psychology of everyday things.&lt;br/&gt;Okazaki, S., &amp;amp; Mendez, F. (2013). Perceived ubiquity in mobile services. Journal of Interactive Marketing, 27(2), 98-111.&lt;br/&gt;Oulasvirta, A., Raento, M., &amp;amp; Tiitta, S. (2005). ContextContacts: re-designing SmartPhone's contact book to support mobile awareness and collaboration. In Proceedings of the 7th international conference on Human computer interaction with mobile devices &amp;amp; services, 167-174.&lt;br/&gt;Oulasvirta, A., Petit, R., Raento, M., &amp;amp; Tiitta, S. (2007). Interpreting and acting on mobile awareness cues. Human–Computer Interaction, 22(1-2), 97-135.&lt;br/&gt;Pitt, L. F., Parent, M., Junglas, I., Chan, A., &amp;amp; Spyropoulou, S. (2011). Integrating the smartphone into a sound environmental information systems strategy: Principles, practices and a research agenda. Journal of Strategic Information Systems, 20 (1), 27–37.&lt;br/&gt;Polycarpou, E., Lambrinos, L., &amp;amp; Protopapadakis, E. (2013). Smart parking solutions for urban areas. In World of Wireless, Mobile and Multimedia Networks (WoWMoM), 2013 IEEE 14th International Symposium and Workshops, 1-6.&lt;br/&gt;Preece, J. (1993). A Guide to Usability: human factors in computing. Addison Wesley, the Open University.&lt;br/&gt;Rafaeli, S. (1988). Interactivity: From new media to communication. InR. P. Hawkins, JM Wiemann, &amp;amp; S. Pingree (Eds.), Advancing communication science: Merging mass and interpersonal processes, 110-134.&lt;br/&gt;Rafaeli, S., &amp;amp; Sudweeks, F. (1997). Networked interactivity. Journal of Computer- Mediated Communication, 2(4).&lt;br/&gt;Rogers, Y., Sharp, H., Preece, J., &amp;amp; Tepper, M. (2007). Interaction design: beyond human-computer interaction. netWorker: The Craft of Network Computing, 11(4), 34.&lt;br/&gt;Sanaei, Z., Abolfazli, S., Gani, A., &amp;amp; Buyya, R. (2014). Heterogeneity in mobile cloud computing: taxonomy and open challenges. IEEE Communications Surveys &amp;amp; Tutorials, 16(1), 369-392.&lt;br/&gt;Sarker, S., &amp;amp; Wells, J. D. (2003). Understanding mobile handheld device use and adoption. Communications of the ACM, 46(12), 35-40.&lt;br/&gt;Sheng, H., Nah, F. F. H., &amp;amp; Siau, K. (2005). Values of silent commerce: A study using value-focused thinking approach. Paper presented at the In Proceedings of the Eleventh Americas Conference on Information Systems.&lt;br/&gt;Shneiderman, B., &amp;amp; Plaisant, C. (2005). Design the user interface-strategies for effective human-computer interaction. Boston, MA: Addison-Wesley.&lt;br/&gt;Shneiderman, B. (2010). Designing the user interface: strategies for effective human- computer interaction. Pearson Education India.&lt;br/&gt;Siuhi, S., &amp;amp; Mwakalonge, J. (2016). Opportunities and challenges of smart mobile applications in transportation. Journal of Traffic and Transportation Engineering (English Edition), 1-11.&lt;br/&gt;Song, J. H., &amp;amp; Zinkhan, G. M. (2008). Determinants of perceived web site interactivity. Journal of Marketing, 72(2), 99-113.&lt;br/&gt;Steuer, J. (1992). Defining virtual reality: Dimensions determining telepresence. Journal of communication, 42(4), 73-93.&lt;br/&gt;Street, C. T., &amp;amp; Meister, D. B. (2004). Small business growth and internal transparency: The role of information systems. MIS Quarterly, 473-506.&lt;br/&gt;Tidwell, J. (2010). Designing interfaces. O'Reilly Media, Inc..&lt;br/&gt;Toda, M., Monden, K., Kubo, K., &amp;amp; Morimoto, K. (2006). Mobile phone dependence and health-related lifestyle of university students. Social Behavior and Person- ality: An International Journal, 34 (10), 1277–1284.&lt;br/&gt;Tsai, C. L., Chen, C. J. &amp;amp; Zhuang, D. J. (2012). Trusted M-banking verification scheme based on a combination of OTP and biometrics. Journal of Convergence, 3(3), 23– 30.&lt;br/&gt;Tse, A. C., &amp;amp; Chan, C. F. (2004). The relationship between interactive functions and website ranking. Journal of Advertising Research, 44(4), 369-374.&lt;br/&gt;Wang, T., Cardone, G., Corradi, A., Torresani, L., &amp;amp; Campbell, A. T. (2012). WalkSafe: a pedestrian safety app for mobile phone users who walk and talk while crossing roads. In Proceedings of the Twelfth Workshop on Mobile Computing Systems &amp;amp; Applications 5. ACM.&lt;br/&gt;Waterson, B. J., Hounsell, N. B., &amp;amp; Chatterjee, K. (2001). Quantifying the potential savings in travel time resulting from parking guidance systems—a simulation case study. Journal of the Operational Research Society, 52(10), 1067-1077.&lt;br/&gt;Weston, H. C. (1949). Sight, Light and Efficiency. Sight, Light and Efficiency. Wiener, N. (1948). Cybernetics. New York: J.&lt;br/&gt;Williams, F., Rice, R. E., &amp;amp; Rogers, E. M. (1988). Research methods and the new media. Simon and Schuster.&lt;br/&gt;Wobbrock, J. O., Myers, B. A., &amp;amp; Aung, H. H. (2008). The performance of hand postures in front-and back-of-device interaction for mobile computing. International Journal of Human-Computer Studies, 66(12), 857-875.&lt;br/&gt;Wu, H. K., Lee, S. W. Y., Chang, H. Y., &amp;amp; Liang, J. C. (2013). Current status, opportunities and challenges of augmented reality in education. Computers &amp;amp; Education, 62, 41-49.&lt;br/&gt;Xu, D. J., Liao, S. S., &amp;amp; Li, Q. (2008). Combining empirical experimentation and modeling techniques: A design research approach for personalized mobile advertising applications. Decision Support Systems, 44(3), 710–724.&lt;br/&gt;Yadav, M. S., &amp;amp; Varadarajan, R. (2005). Interactivity in the Electronic Marketplace: an Exposition of the Concept and Implications for Research. Journal of the Academy of Marketing Science, 33(4), 585-603.&lt;br/&gt;Yoo, W. S., Lee, Y., &amp;amp; Park, J. (2010). The role of interactivity in e-tailing: Creating value and increasing satisfaction. Journal of Retailing and Consumer Services, 17(2), 89-96.&lt;br/&gt;Zheng, P., &amp;amp; Ni, L. M. (2006). Spotlight: the rise of the smart phone. IEEE Distributed Systems Online, 7(3), 3.&lt;br/&gt;&lt;br/&gt;網站&lt;br/&gt;Adjust (2014). A look at the Apple App Store in July 2014. Retrieved December 1, 2016, from https://www.adjust.com/assets/downloads/AppleAppStore_Report2014.pdf&lt;br/&gt;Apple (2013). iOS User Experience. Retrieved December 1, 2016, from http://developer.apple.com/library/ios/#documentation/UserExperience/Concept ual/MobileHIG/Introduction/Introduction.html&lt;br/&gt;Canarie, Inc. (1997). Towards a Canadian health IWAY. Retrieved December 1, 2016, from http://www.canarie.ca/press/publications/pdf/ health/ healthvision.doc&lt;br/&gt;Clabaugh, J. (2013). Tablet ownership reaches 40%. Washington Business Journal. Retrieved December 1, 2016, from http://www.bizjournals.com/washington/blog/techflash/2013/04/tablet-ownershi p-reaches-40.html&lt;br/&gt;Gartner (2016). Gartner Says Global Smartphone Sales to Only Grow 7 Per Cent in 2016. Retrieved December 1, 2016, from http://www.gartner.com/newsroom/id/3270418&lt;br/&gt;Google (2016a). Principles of mobile app design introduction. Retrieved December 1, 2016, from http://apac.thinkwithgoogle.com/intl/zh-TW_ALL/articles/principles- of-mobile-app-design-introduction.html&lt;br/&gt;Google (2016b). Mobile applications analytics. Retrieved December 1, https://www.google.com.tw/intl/zh-TW/analytics/features/mobile-app- analytics.html&lt;br/&gt;Hamburger, E. (2013). Samsung designer Golden Krishna: 'Our love for the digital interface is out of control', Retrieved December 1, 2016, from http://www.theverge.com/2013/3/10/4086392/samsung-golden-krishna-the- bestinterface-is-no-interface&lt;br/&gt;Phonearena (2016). Google Play Store had 11.1 billion downloads in the first quarter of 2016. Retrieved December 1, 2016, from http://www.phonearena.com/news/Google-Play-Store-had-11.1-billion- downloads-in-the-first-quarter-of-2016_id80328&lt;br/&gt;QUIS (2012). Questionnaire for User Interaction Satisfaction(QUIS). Retrieved December 1, 2016, from http://lap.umd.edu/quis/&lt;br/&gt;The Telegraph. (2011). Brits spend nearly an hour using smartphones during nights out. Retrieved December 1, 2016, from http://www.telegraph.co.uk/technology/mobile-phones/8806277/Brits-spend- nearly-an-hour-using-smartphones-during-nights-out.html.&lt;br/&gt;United Nations. (2014). 2014 Revision of World Population Prospects. United Nations report. Retrieved December 1, 2016, from https://esa.un.org/unpd/wup/publications/files/wup2014-highlights.Pdf&lt;br/&gt;&lt;/div&gt;</t>
-        </is>
-      </c>
-      <c r="AA14" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/69r4pm</t>
         </is>
@@ -2390,35 +2371,34 @@
         </is>
       </c>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>點閱:227</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>點閱:227</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr">
         <is>
           <t xml:space="preserve">
 由於近幾年社會與人口的急遽變遷，我國老年人口也正在快速的增長，在2014年底65歲以上老人所占比例已達12.0%，我國國民健康與保健型態亦漸漸轉變為慢性疾病與慢性功能障礙盛行的時代，且我國在2015年通過長期照護保險草案的影響，因此對長期醫療照護的需求也隨之成長，長期照護相關議題成為重要的議題。隨著長照醫療環境的日趨競爭，長期照護機構經營者已經將焦點放在經營成本的控制良好，且能維持一定水準的醫療品質。許多資訊管理相關的研究指出，使用資訊科技對於組織績效的提升有相當正面的助益，McCandless and Norretranders (2013)更指出，在所有感官中，視覺對於資訊的反應速度是最快的，使用視覺化的圖表更能增加12%的網路流量。本研究使用商業軟體QlikView，實作以長照機構為例並以可視覺化、連動式呈現的系統，資料來源為某護理之家資料庫，以視覺化、連動式的方式，針對長期照護資料，進行大數據分析，提供即時性且多構面的內容，其中構面包括長期照護住戶基本資料、住戶照護量表、照護品管指標、院內收支情況等，研究目的期望本系統能協助管理者決策、控制管理成本、對於組織內資訊的訊獲取速度更快更直覺性，最終達成提升管理品質進而提升醫療品質。</t>
         </is>
       </c>
-      <c r="Z15" t="inlineStr">
+      <c r="Y15" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 Ma, R., &amp;amp; Singh, G. (2004, October). Large-scale infographic image downsizing. In Image Processing, 2004. ICIP'04. 2004 International Conference on (Vol. 3, pp. 1661-1664). IEEE.&lt;br/&gt;Hart, G. (2013). Effective Infographics: Telling Stories in the Technical Communication Context. Downloaded October, 1, 2013.&lt;br/&gt;Meeusah, N., &amp;amp; Tangkijviwat, U. (2013). Effect of data set and hue on a content understanding of infographic.&lt;br/&gt;Siricharoen, W. V., &amp;amp; Siricharoen, N. How Infographic should be evaluated?.&lt;br/&gt;Choi, B., Lee, Y., &amp;amp; Park, S. (2006). A Research on Interactive Infographics for Effective Visual Communication. Journal of Korean Society of Design Science,19(2), 229-240.&lt;br/&gt;Diakopoulos, N., Kivran-Swaine, F., &amp;amp; Naaman, M. (2011, May). Playable data: characterizing the design space of game-y infographics. In Proceedings of the SIGCHI Conference on Human Factors in Computing Systems (pp. 1717-1726). ACM.&lt;br/&gt;Kane, R. A., Kane, R. L., &amp;amp; Ladd, R. C. (1998). The heart of long term care. Oxford University Press.&lt;br/&gt;Brunelli, J. (2010). SHOWCASING TWENTY YEARS OF VENICE PROJECT CENTER RESULTS USING INTERACTIVE ONLINE INFOGRAPHICS(Doctoral dissertation, WORCESTER POLYTECHNIC INSTITUTE).&lt;br/&gt;Bubela, T., Nisbet, M. C., Borchelt, R., Brunger, F., Critchley, C., Einsiedel, E., ... &amp;amp; Jandciu, E. W. (2009). Science communication reconsidered. Nature biotechnology, 27(6), 514-518.&lt;br/&gt;Pipps, V., Walter, H., Endres, K., &amp;amp; Tabatcher, P. (2009). Information recall of internet news: does design make a difference? A pilot study. Journal of Magazine &amp;amp; New Media Research, 11(1), 1-20.&lt;br/&gt;Schmidt, A. (2013). Bachelor Thesis Interactive Visualization of Software Defined Networks (Doctoral dissertation, Saarland University).&lt;br/&gt;Kernisan, Leslie.　(2015) "Activities of Daily Living: What Are ADLs and IADLs?". Caring.&lt;br/&gt;Hogan, M. (2013) What is Big Data&lt;br/&gt;Gupta, A., &amp;amp; Gupta, A. (2015). AD-HOC EP CURVE CALCULATION USING MAP-REDUCE AND UI INTEGRATION WITH QLIKVIEW. International Journal of Advances in Engineering &amp;amp; Technology, 8(5), 823.&lt;br/&gt;Michael, K., &amp;amp; Miller, K. (2013). Big data: New opportunities and new challenges [guest editors' introduction]. Computer, 46(6), 22-24.&lt;br/&gt;Sagiroglu, S., &amp;amp; Sinanc, D. (2013, May). Big data: A review. In Collaboration Technologies and Systems (CTS), 2013 International Conference on (pp. 42-47). IEEE.&lt;br/&gt;黃斯聖. (2008). 老年失智症之照顧者的負荷及憂鬱的相關因素探討. 中山醫學大學醫學研究所學位論文, (2008 年), 1-108.&lt;br/&gt;林惠文, 楊博仁, 楊宜瑱, 陳俊傑, 陳宣志, 顏啟華, ... &amp;amp; 李孟智. (2010). 台灣地區老年人憂鬱之預測因子探討-十年追蹤結果分析. 台灣老年醫學暨老年學雜誌,5(4), 257-265.&lt;br/&gt;葉濬彰. (2011). 社區老人的主觀社會地位, 自尊, 自我掌控信念與憂鬱之關係. 中原大學心理學研究所學位論文, 1-77.&lt;br/&gt;王珊瑜. (2007). 台北市小型安養護機構老人認知功能之探討: 簡易智能狀態量表 (MMSE) 之運用. 臺灣大學社會工作學研究所學位論文, 1-127.&lt;br/&gt;鍾雪珍. (2008). 新版 EBSCOhost2. 0 資訊視覺化檢索簡介.&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005898939" target="_blank"&gt;吳淑瓊. (2005). 人口老化與長期照護政策. 國家政策季刊, 4(4), 5-24.&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005868405" target="_blank"&gt;廖士程, 李明濱, 謝博生, &amp;amp; 李源德，(2005)。醫病關係與醫療滿意度之全國性普查。醫學教育 9(2)，149-161。&lt;/a&gt;&lt;br/&gt;楊志良.(2000)‧老人照護政策之規劃‧二十一世紀老人照護研討會講義‧台灣台北。&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA15" t="inlineStr">
+      <c r="Z15" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/5f4ebc</t>
         </is>
@@ -2523,35 +2503,34 @@
           <t>QlikView、nursing home、big data technique、visualization chart</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>點閱:1159</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>點閱:1159</t>
+          <t>59</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>4</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="Y16" t="inlineStr">
         <is>
           <t xml:space="preserve">
 隨著時代的進步，科技越來越發達，電腦軟硬體設備的進步，資訊產品可以儲存的資料量越來越大，而越來越大的資料量已經不足以資料來稱呼，故將這些龐大的資料群，稱之為巨量資料、大數據等名稱，這些大數據資料，傳統的資料分析軟體已經無法負荷，必須使用專門的大數據分析軟體才能輕鬆的達成從前的資料分析工作。在眾多資料軟體當中，本研究挑選出一套免費又簡單的軟體QlikView作為研究用數據分析工具，希望藉由此軟體，為雜亂無章且不易分析整理的護理之家資料庫資料，做成令人淺而易懂的可視化圖表，而且可以透過簡單的操作，將所需要的資訊在幾下簡單的點選中呈現出來。因目前學術界上，很少有人以QlikView做大數據分析為討論範圍做研究，大部分是介紹此軟體的相關功能，本研究希望能做到一個承先啟後的效果，承襲前人將此軟體發掘出來，開啟後進對QlikView這套軟體做大數據分析的研究興趣，可以對QlikView與大數據分析開啟各個面向的探討與研究。</t>
         </is>
       </c>
-      <c r="Z16" t="inlineStr">
+      <c r="Y16" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 中文部份&lt;br/&gt;大數據可視化產品選型(民104年4月17日)。民104年12月19日，取自：中國統計網：https://read01.com/3G3zo4.html&lt;br/&gt;&lt;br/&gt;商業智能解決方案之政府醫療保健機構(無日期)。民104年12月5日，取自：QlikView官網：http://global.qlik.com/cn/explore/solutions/industries/public-sector/government-healthcare&lt;br/&gt;&lt;br/&gt;資料庫(民104年7月20日)。民104年12月5日，取自：維基百科：https://zh.wikipedia.org/wiki/%E6%95%B0%E6%8D%AE%E5%BA%93&lt;br/&gt;&lt;br/&gt;資料視覺化(民105年2月日)。民104年7月2日，取自：維基百科：https://zh.wikipedia.org/wiki/%E6%95%B0%E6%8D%AE%E5%8F%AF%E8%A7%86%E5%8C%96&lt;br/&gt;&lt;br/&gt;數位資料整理術(民96年1月8日)，民104年12月19日，取自：經理人月刊：&lt;br/&gt;http://www.managertoday.com.tw/index.php/articles/view/538&lt;br/&gt;&lt;br/&gt;數據分析(無日期)。民104年12月5日，取自：MBA智庫百科：http://wiki.mbalib.com/zh-tw/%E6%95%B0%E6%8D%AE%E5%88%86%E6%9E%90&lt;br/&gt;&lt;br/&gt;關聯式資料庫(民98年7月6日)。民104年12月5日，取自：維基百科：https://zh.wikipedia.org/wiki/%E5%85%B3%E7%B3%BB%E6%95%B0%E6%8D%AE%E5%BA%93&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;英文部份&lt;br/&gt;Bryant, R., Katz, R. H., &amp;amp; Lazowska, E. D. (2008). Big-data computing: Creating revolutionary breakthroughs in commerce, science and society.&lt;br/&gt;Bughin, J., Chui, M., &amp;amp; Manyika, J. (2010). Clouds, big data, and smart assets: Ten tech-enabled business trends to watch. McKinsey Quarterly, 56(1), 75-86.&lt;br/&gt;Chen, C. P., &amp;amp; Zhang, C. Y. (2014). Data-intensive applications, challenges, techniques and technologies: A survey on Big Data. Information Sciences, 275, 314-347.&lt;br/&gt;Cukier, K., &amp;amp; Mayer-Schoenberger, V. (2013). Rise of Big Data: How it's Changing the Way We Think about the World, The. Foreign Aff., 92, 28.&lt;br/&gt;Lopatenko, A. (2015). QlikView as a Data Management Solution.&lt;br/&gt;Nielsen, E. W., Hovland, A., &amp;amp; Stromsnes, O. (2006). [A new tool for retrieving clinical data from various sources]. Tidsskrift for den Norske laegeforening: tidsskrift for praktisk medicin, ny raekke, 126(5), 605-607.&lt;br/&gt;Golfarelli, M., Rizzi, S., &amp;amp; Proli, A. (2006, November). Designing what-if analysis: towards a methodology. In Proceedings of the 9th ACM international workshop on Data warehousing and OLAP (pp. 51-58). ACM.&lt;br/&gt;Groves, P., et al., (2013). The ‘big data’revolution in healthcare. McKinsey Quarterly.&lt;br/&gt;Gupta, A., &amp;amp; Gupta, A. (2015). AD-HOC EP CURVE CALCULATION USING MAP-REDUCE AND UI INTEGRATION WITH QLIKVIEW. International Journal of Advances in Engineering &amp;amp; Technology, 8(5), 823.&lt;br/&gt;Herodotou, H., et al., (2011, January). Starfish: A Self-tuning System for Big Data Analytics. In CIDR (Vol. 11, pp. 261-272).&lt;br/&gt;Kaisler, S., et al., (2013, January). Big data: Issues and challenges moving forward. In System Sciences (HICSS), 2013 46th Hawaii International Conference on (pp. 995-1004). IEEE.&lt;br/&gt;Michael, K., &amp;amp; Miller, K. (2013). Big data: New opportunities and new challenges [guest editors' introduction]. Computer, 46(6), 22-24.&lt;br/&gt;Sagiroglu, S., &amp;amp; Sinanc, D. (2013, May). Big data: A review. In Collaboration Technologies and Systems (CTS), 2013 International Conference on (pp. 42-47). IEEE.&lt;br/&gt;Schuette, M. (2013). Evolution of Research Reporting–From Excel to QlikView. Planning for Research Excellence in the Era of Analytics, 62.&lt;br/&gt;Serbanescu, L. (2009). Business Intelligence Solutions For Human Resource Management. The Annals of the" Stefan cel Mare" University of Suceava. Fascicle of The Faculty of Economics and Public Administration, 9(Special), 162-168.&lt;br/&gt;Tene, O., &amp;amp; Polonetsky, J. (2012). Privacy in the age of big data: a time for big decisions. Stanford Law Review Online, 64, 63.&lt;br/&gt;Zeng, J., &amp;amp; Zhang, J. (2013). Using Dashboard for Lean Revenue Cycle Management. iBusiness, 5(03), 100.&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA16" t="inlineStr">
+      <c r="Z16" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/fh3dy2</t>
         </is>
@@ -2656,35 +2635,34 @@
           <t>Mathematical Logic、Propositional logic、First-order logic、Software testing、Data verification</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>點閱:123</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>點閱:123</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr">
         <is>
           <t xml:space="preserve">
 以電腦系統程式來取代人工處理各種龐大的資料量，是現今社會普遍常見的作法。但系統程式在處理大量資料過程中，如何確保其處理結果是正確無誤；尤其程式設計師所撰寫的程式碼中，還是會存在某些無法預期的邏輯性錯誤。因此我們必須透過各種檢核機制，來確認程式執行結果是否與預期相同。在程式設計領域中，很多程式設計師的解決問題思維，往往被既有的程式開發工具所限制住，形成盲點自我設限。若能強化程式設計師的數理邏輯概念，在遇到問題時，可以先換個方向來分析和整理，很多重大突破，往往就是這樣產生的。本研究建立一套資料處理後的檢核驗證程式，著重在檢核條件需先以數理邏輯進行分析，發展出檢核條件的邏輯表示式，並與使用者共同討論檢視後，才能依據邏輯表示式進行程式開發，確保在開發程式時，不會偏離原有的檢核條件需求。本研究以大學繁星推薦招生之分發比序結果來進行個案研究，透過本次研究所提出的作業模式和具代表性的檢核程式，其測試結果達到當初預期的目的，同時也讓試務單位對於檢核程式有相當大的信任感。但未來亦需持續增加檢核程式的建立和因應招生規則的變動來修正檢核條件，以達到分發檢核經驗的延續和傳承。</t>
         </is>
       </c>
-      <c r="Z17" t="inlineStr">
+      <c r="Y17" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 一、中文文獻&lt;br/&gt;人工智慧：現代方法(3版) (歐崇明、時文中、陳龍 編譯) (民100)。 臺北市：台灣培生教育出版。 (原著出版年：2009年)&lt;br/&gt;大考中心基金會 (民98)。 大學入學考試中心20周年特輯：選才文摘大學入學考試制度類。 臺北市：大考中心基金會。&lt;br/&gt;大學甄選入學委員會 (民103)。 104學年度大學「繁星推薦」入學招生簡章。嘉義縣：大學甄選入學委員會。&lt;br/&gt;大學甄選入學委員會 (民102)。 103學年度大學「繁星推薦」入學招生簡章。嘉義縣：大學甄選入學委員會。&lt;br/&gt;李宗翰 (民104年7月19日)。 在軟體開發期間就能找出安全性漏洞。 iThome電腦報週刊，669期，36-37。&lt;br/&gt;李家同 (民100)。 人人都能學會寫程式:李家同教你用邏輯思考學程式設計。 台北市：聯經。&lt;br/&gt;修斐士‧席爾 (民77)。 初級數理邏輯。 (劉福增 評著)。 臺北市：水牛。 (原著出版年﹕1963年)&lt;br/&gt;陳瑞麟 (民94)。 邏輯與思考(2版)。 臺北市：學富文化。&lt;br/&gt;彭孟堯 (民89)。 符號邏輯。 臺北市：心理。&lt;br/&gt;項潔 (民104)。布爾與電腦。科學月刊，551，858-861。&lt;br/&gt;黃西川 (民102)。 簡易離散數學。 臺北市：五南。&lt;br/&gt;黃中彥 (民100)。 基礎離散數學。 新北市：新文京開發。&lt;br/&gt;董世平 (民104)。布爾與邏輯。科學月刊，551，852-857。&lt;br/&gt;齊斯‧德福林 (民103)。 這個問題，你用數學方式想過嗎?。 (洪萬生、黃俊瑋、蘇惠玉、陳彥宏、葉吉海 譯)。 臺北市：城邦文化事業股份有限公司。 (原著出版年：2012年)&lt;br/&gt;劉福增 (民92)。 邏輯思考。 臺北市：心理。&lt;br/&gt;離散數學 (呂威甫、施文慈 譯) (民98)。 臺北市：碁峰資訊。 (原著出版年：2003年)&lt;br/&gt; &lt;br/&gt;二、英文文獻&lt;br/&gt;Boris Beizer (1990). Software Testing Techniques. New York: Van Nostrand Reinhold.&lt;br/&gt;Elliott Mendelson (1997). Introduction to Mathematical Logic. Chapman &amp;amp; Hall.&lt;br/&gt;Keith Devlin (2012). Introduction to Mathematical Thinking. USA: Keith Devlin.&lt;br/&gt;Klement, Kevin C. (2006). Propositional Logic. James Fieser and Bradley Dowden (eds.). Internet Encyclopedia of Philosophy. Eprint.&lt;br/&gt;Myers, G. J. (1979). The art of software testing, New York: Wiley.&lt;br/&gt;&lt;br/&gt;三、網路資料&lt;br/&gt;大學招生委員會聯合會(無日期)，大學招生委員會聯合會組織架構【公告】。民國103年7月15日，取自：http://www.jbcrc.edu.tw/index1.htm&lt;br/&gt;大學招生委員會聯合會(無日期)。 入學管道【公告】。 民國103年7月15日，取自：http://www.jbcrc.edu.tw/left-31.htm&lt;br/&gt;大學甄選入學委員會 (民102)。 統計資料【公告】。 民國103年7月10日，取自：https://www.caac.ccu.edu.tw/cacportal/index.php&lt;br/&gt;吳維漢 (2012-09-07)。 數學與程式設計。 國立中央大學數學系。 民103年2月10日，取自：http://www.ziyou.math.ncu.edu.tw/~ziyou/c++/downloads/math.pdf&lt;br/&gt;教育部全球資訊網高等教育司 (民103年4月21日)。 103學年度大學日間學制各學系（組）招生名額分配核定表【公告】。 民國103年9月8日，取自：http://www.edu.tw/userfiles/url/20140421091752/1030415_103%E5%90%8D%E9%A1%8D%E6%97%A5%E5%AD%B8%E6%A0%B8%E5%AE%9A%E8%A1%A8_%E4%B8%8A%E5%82%B3%E7%89%88.pdf&lt;br/&gt;教育部全球資訊網高等教育司 (無日期)。 102學年度大學日間學制各學系（組）招生名額分配核定表【公告】。 民國103年9月8日，取自：http://www.edu.tw/FileUpload/1075-17585/Documents/1020107_102%E5%90%8D%E9%A1%8D%E6%97%A5%E5%AD%B8%E6%A0%B8%E5%AE%9A%E8%A1%A8po%E7%B6%B2.xlsx&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA17" t="inlineStr">
+      <c r="Z17" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/atp8ck</t>
         </is>
@@ -2789,35 +2767,34 @@
           <t>Patient safety、Incident、Warning indicators、Detection</t>
         </is>
       </c>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>點閱:171</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>點閱:171</t>
+          <t>2</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y18" t="inlineStr">
         <is>
           <t xml:space="preserve">
 IOM(Institute of Medicine)出版的「To error is human 」一書對全世界醫療產業產生莫大衝擊，透過合理的估計，全美於 1997 年病人死於醫療失誤，可列入第八大死亡原因，年損失最多約 290 億美金。病人安全的議題就此被廣泛討論，整個醫療產業開始傾注大量的資源來推動病人安全。資訊科技介入可以在三方面可以減少錯誤發生的比例：預防錯誤與不良事件發生；在不良事件發生時可以快速的回應；針對不良事件進行追蹤與提供後續的回饋。（許明暉、李友專，民98）。利用資訊系統來減少醫療錯誤及預防錯誤的發生是現今的趨勢。本研究提出在病人安全事件中，可作為預警偵測指標、監控的方法。開發行動裝置即時通訊應用軟體（Application software; APP）並結合醫院資訊系統平台，藉由行動裝置即時通訊APP，及時通知重要相關訊息給予醫療照護團隊，針對病人安全要求，以防止醫療人員於醫療照護過程，讓病人從安全狀態進入至不安全的狀態，途中能有完善的預警監控，使得事件減少或阻止進入危機、危險狀態，甚至阻擋醫療疏失事件的發生。系統開發後經問卷調查醫療人員使用進行評估，顯示開發行動裝置即時通訊應用軟體（APP）結合醫院資訊系統，其成效滿足使用者其需求及重要性。期許導入「病人安全事件預警監控模式」以防止醫療人員於醫療照護過程中，當病人從安全狀態進入至不安全的狀態時，途中有完善的智慧預警監控，讓事件不進入危機或危險狀態。系統能有效、正確、即時偵測，適切將資訊傳達至該醫療相關照護人員，以利作為病人正確處置，以提昇醫療照護品質與安全。</t>
         </is>
       </c>
-      <c r="Z18" t="inlineStr">
+      <c r="Y18" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 中文文獻&lt;br/&gt;王文科、王智弘（民95）。教育研究方法（增訂10版）。台北市：五南圖書出版股份有限公司。&lt;br/&gt;王淑惠（民96）。從院內感染談病人安全與醫療照護品質。重症醫學雜誌，1(4)，166-174。&lt;br/&gt;尹祚芊（民103，5月）。醫院暴力事件調查報告。2015年5月27日取自http://www.cy.gov.tw/AP_HOME/Op_Upload/eDoc/調查報告/103/1030001661020800461醫院暴力案調查報告-對外。&lt;br/&gt;許明暉、李友專（民98，5月）。醫院資訊系統與病人安全。2016年5月27日取自http://libir.tmu.edu.tw/bitstream/987654321/18165/1/%E7%97%85%E4%&lt;br/&gt;BA%BA%E5%AE%89%E5%85%A8.pdf。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22094NTU05529011%22.&amp;amp;searchmode=basic" target="_blank"&gt;石崇良（民95）。急診醫療不良事件之流行病學研究。國立台灣大學醫療機構管理研究所博士論文，台北。&lt;/a&gt;&lt;br/&gt;朱樹勳（民100）。醫療機構品質與病安管理-理念與實務。台北：華杏。&lt;br/&gt;吳德朗總校閱（民95）。哈里遜內科學。（合記圖書出版社譯）。臺北市：麥格羅希爾。(原著出版年：2001年)&lt;br/&gt;邱弘毅 (民97)。腦中風之現況與流行病學特徵。台灣腦中風學會會訊，15 (3)，2-4。&lt;br/&gt;胡漢華主編 (民97)。台灣腦中風防治指引。台北：台灣腦中風學會。&lt;br/&gt;財團法人醫院評鑑既醫療品質策進會（民102）。2013年台灣病人安全通報年度報表。台北：財團法人醫院評鑑暨醫療品質策進會。&lt;br/&gt;陳岩碧、胡勝川（民94）。發燒及感染急症之評估與處置。慈濟醫學，17(5)，27-30。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22102NCKU5457035%22.&amp;amp;searchmode=basic" target="_blank"&gt;陳義憲（民103）。醫院處理急診暴力事件因應措施之研究。成功大學高階管理碩士在職專班(EMBA)學位論文，1-124。&lt;/a&gt;&lt;br/&gt;詹廖明義編譯(民92)。醫療事故的風險管理。新北市：安立。&lt;br/&gt;鄭貴月、邱素真、孫漬官、葉淑惠、張谷州(民95)。台灣地區神經科醫護人員對美國國家衛生研究院腦中風評估量表之臨床應用。實證護理，2(3)，189-200。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006798778" target="_blank"&gt;賴尚儀、魏玉雲、吳美慧、林綉珠、石富元（民103）。醫療暴力之樣態與防範。澄清醫護管理雜誌，10 (4)，5-11。&lt;/a&gt;&lt;br/&gt;酈欽菁、蔡秀鸞、葉炳強、蘇慧芳（民91）。缺血性腦中風臨床路徑成效。台灣醫學，6，672-681。&lt;br/&gt;&lt;br/&gt;英文文獻&lt;br/&gt;Adams HP Jr, Leclerc JR, Bluhmki E, et al.(2004). Measuring outcomes as a function of baseline severity of ischemic stroke. Cerebrovasc Dis , 18, 124-129.&lt;br/&gt;Barach P, Smaii S(2000) . Reporting and preventing medical mishaps: lessons from non-medical near miss reporting system. BMJ , 320, 759-763.&lt;br/&gt;Barratt, E. S., Stanford, M. S., Dowdy, L., Liebman, M. J., &amp;amp; Kent, T. A. (1999). Impulsive and premeditated aggression: A factor analysis of self-reported acts. Psychiatry Research, 86(2), 163-173.&lt;br/&gt;Chassin MR, Galvin RW.(1998). The urgent need to improve health care quality. Institute of Medicine National Roundtable on Health Care Quality. JAMA. Sep 16, 280(11), 1000-1005.&lt;br/&gt;C.P. Subbe, M. Kruger, P. Rutherford and L Gemmel(2001). Validation of a modified Early Warning Score in medical admissions.QJM, 94 , 521-526.&lt;br/&gt;Esteban A, Frutos-Vivar F, Ferguson ND, et al. (2007). Sepsis incidence and outcome: contrasting the intensive care unit with the hospital ward. Crit Care Med , 35(5), 1284-1289.&lt;br/&gt;Guidet B, Aegerter P, Gauzit R, Meshaka P, Dreyfuss D.(2005). Incidence and impact of organ dysfunctions associated with sepsis. Chest , 127(3), 942- 951.&lt;br/&gt;Hausfater P, Juillien G. Serum(2007). Procalcitonin Measurement As Diagnostic and Prognostic Marker in Febrile, Adult Patients Presenting to the Emergency Department. Critical Care , 11, 60-68.&lt;br/&gt;Heidi Wald.Kaveh G Shojania (2001). Incident reporting making health care safer, Acritical Analysis of Patient Safety Practice, 4-22-30.&lt;br/&gt;Hermans M.A., Leffers P, Jansen LM, Keulemans YC, Stassen PM.( 2012). The value of the Mortality in Emergency Department Sepsis (MEDS) score, C reactive protein and lactate in predicting 28-day mortality of sepsis in a Dutch emergency department. Emerg Med J, 29(4), 295-300.&lt;br/&gt;Heinrich H.W. (1931),Industrial Accident Prevention,4th ed.New York：MCGrew-Hill。&lt;br/&gt;Jauch, E. C., Saver, J. L., Adams, H. P., Bruno, A., Connors, J. J., Demaerschalk, B.,Yonas, H. (2013). Guidelines for the early management of patients with acuteischemic stroke a guideline for healthcare professionals from the American Heart Association/American Stroke Association. Stroke, 44(3), 870-947.&lt;br/&gt;Kohn L.T., Corrign J.M., Donaldson M.S. (1999). To err is human: building a safer health system (ed).Washington, DC: National Academy Press.&lt;br/&gt;Kowalenko, T., Walters, B.L., Khare, R.K., Compton, S.(2005). Workplace violence: a survey of emergency physicians in the state of Michigan. Ann Emerg Med, 46,142-147.&lt;br/&gt;Lavoie, F.W., Carter, G.L., Danzl, D.F., et al.(1988). Emergency department violence in United States teaching hospitals. Ann Emerg Med, 17, 1227-1233.&lt;br/&gt;Leape, L., Lawthers, A. G., Brennan, T. A., Johnson W.G.(1993). Preventing medical injury. Qual Rev Bull, 19(5), 144-149.&lt;br/&gt;Meisner M.(2005). Biomarkers of sepsis: clinically useful? Curr Opin Crit Care ,11, 473-480.&lt;br/&gt;Polly E. Parsons, Jeanine P. Wiener-Kronish.(2012). Critical Care Secrets, 5e.Louis,Missouri. : Mosby.&lt;br/&gt;R.C. Bone, R.A. Balk, F. B. Cerra, R. P. Dellinger, A. M. Fein, W. A. Knaus., et al.(1992). Definitions for sepsis and organ failure and guidelines for the use of innovative therapies in sepsis. The ACCP/SCCM Consensus Conference Committee. American College of Chest Physicians/Society of Critical Care Medicine. Chest, 101(6), 1644-1655.&lt;br/&gt;Reason, J.(2000). Human error: Model and management. BMJ, 320, 768-770.&lt;br/&gt;Reason, J.(1995). Understanding adverse events: Human factor. Quality in Health care,4, 80-89.&lt;br/&gt;Rivers E, Nguyen B, Havstad S, et al.(2001). Early goal-directed therapy in the treatment of severe sepsis and septic shock. N Engl J Med , 345(19), 1368-1377.&lt;br/&gt;Smith-Pittman M.H., McKoy Y.D. (1999). Workplace violence in healthcare environments. Nursing Forum y,34, 5-13.&lt;br/&gt;The National Institute of Neurological Disorders and Stroke rt-PA Stroke Study Group: Tissue plasminogen activator for acute ischemic stroke.(1995). N Engl J Med;333, 1581-1587.&lt;br/&gt;Thomas, E. J. , Petersen, L. A. (2003). Measuring errors and adverse events in health care. Journal of General Internal Medicine, 18, 61-67.&lt;br/&gt;Whittington J, White R, et al.(2007). Rapid response systems: the stories: using an automated risk assessment report to identify patients au risk for clinical deterioration. The Joint Commission Journal on Quality and patient safety,33(9), 569-574.&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA18" t="inlineStr">
+      <c r="Z18" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/9m4r47</t>
         </is>
@@ -2914,35 +2891,33 @@
           <t>Internet Of Things、Platform for Remote Caring、ZigBee、Home</t>
         </is>
       </c>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>點閱:610</t>
+        </is>
+      </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>點閱:610</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr">
         <is>
           <t xml:space="preserve">
 依據衛福部在2016年的統計資料顯示，目前台灣65歲以上人口佔總人口數的12%以上，台灣儼然已成為高齡化社會，再加上少子化問題日益嚴重，平均每2位青壯年需負擔照顧1位老人及1位幼童的責任。且台灣已於2015年6月通過長期照顧服務法，預計2017年實施，以現行照護人力評估，實施後照護人力將嚴重不足，所以若能透過物聯網技術與網通科技的結合，將可協助解決照護人力不足的問題。本研究利用生命徵象量測、臥床偵測及室內定位等技術，避免使用網路攝影機等侵犯隱私的工具，來達到遠距照護的目的，讓長者也可選擇居住在自己家中，透過此遠距照護系統的幫助，讓關懷者可以隨時掌握長者的居家狀態，使其達到就地安養、在地老化的目的。關鍵字：物聯網、遠距照護、ZigBee、居家</t>
         </is>
       </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="Z19" t="inlineStr">
-        <is>
-          <t>&lt;div style="padding:10px;text-align:left;"&gt;
-中文文獻&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006537211" target="_blank"&gt;呂寶靜、陳正芬（民98）。我國居家照顧服務員職業證照與培訓制度之探究：從英國和日本的作法反思台灣。社會政策與社會工作學刊，13（1），185-233。&lt;/a&gt;&lt;br/&gt;林甫俊（民103）。物聯網國際規格標準及發展。科學月刊 201404-388期，科技產業／科技報導。&lt;br/&gt;林金立（民97）。遠距照顧技術應用於居家老人照顧服務之探討。社會福利專題研習教材第14輯，內政部社會福利研習中心，2008年8月。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006769009" target="_blank"&gt;林澂、羅孟宗（民103）。睡眠監測技術的新發展。臺灣醫學，18（2），172-180。&lt;/a&gt;&lt;br/&gt;周洪波、李吉生、趙曉波（民99）。輕鬆讀懂物聯網—技術、應用、標準和商業模式。台灣：博碩出版社發行。&lt;br/&gt;施秋蘭（民102）。我國長期照顧專業人力培育現況與困境。銀髮世紀第56期-201306。&lt;br/&gt;徐業良（民97）。老人福祉科技與遠距居家照護技術。台灣：滄海書局出版。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006742389" target="_blank"&gt;莊祐軒、羅乃維（民102）。物聯網安全的現況與挑戰。資訊安全通訊，19（4），16-29。&lt;/a&gt;&lt;br/&gt;系統分析與設計（初版） （陳盈潔譯）（民92）。台北市：台灣培生教育：儒林出版社發行。（原著出版年：2003年）&lt;br/&gt;系統分析與設計概論（潘冠宇譯） （民92）。台灣培生教育出版集團:碁峰資訊股份有限公司發行。（原著出版年：2003年）&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22100NUUM0396003%22.&amp;amp;searchmode=basic" target="_blank"&gt;黃廣台（民101）。應用ZigBee無線網路進行室內定位之研究。國立聯合大學資訊管理學系碩士班，未出版，苗栗縣。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0004720749" target="_blank"&gt;黃興進（民91）。醫療資訊管理系統研究議題之探討。資訊管理學報，9（S），101-116。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006121745" target="_blank"&gt;蔡宗宏、黃暉庭（民96）。醫療資訊系統成功模型之研究。醫務管理期刊，8（4），281-300。&lt;/a&gt;&lt;br/&gt;鄧凱元、許言（民104）。物聯網與服務創新應用探討。工業設計（131），26-32。&lt;br/&gt; &lt;br/&gt;英文文獻&lt;br/&gt;Atzori, L., Iera, A., &amp;amp; Morabito, G. （2010）. The internet of things: A survey. Computer networks, 54（15）, 2787-2805.&lt;br/&gt;Bekkali, A., Sanson, H., &amp;amp; Matsumoto, M. （2007）. RFID indoor positioning based on probabilistic RFID map and Kalman filtering. Paper presented at the Wireless and Mobile Computing, Networking and Communications, 2007. WiMOB 2007. Third IEEE International Conference on.&lt;br/&gt;Boulos, M. N. K., &amp;amp; Berry, G. （2012）. Real-time locating systems （RTLS） in healthcare: a condensed primer. International journal of health geographics, 11（1）, 25.&lt;br/&gt;Chen, Y.-P. T. C.-Y., &amp;amp; Lin, C.-T. ZigBee Technology Development for Smart Home Appliance Application.&lt;br/&gt;Chesson Jr, M., Coleman, M., Lee-Chiong, M., &amp;amp; Pancer, D. （2007）. Practice parameters for the use of actigraphy in the assessment of sleep and sleep disorders: an update for 2007. Sleep, 30（4）, 519.&lt;br/&gt;Da Xu, L., He, W., &amp;amp; Li, S. （2014）. Internet of Things in industries: A survey. Industrial Informatics, IEEE Transactions on, 10（4）, 2233-2243.&lt;br/&gt;Doughty, K., Cameron, K., &amp;amp; Garner, P. （1996）. Three generations of telecare of the elderly. Journal of Telemedicine and Telecare,2（2）, 71-80.&lt;br/&gt;Doll, W. J., &amp;amp; Torkzadeh, G. (1988). The measurement of end-user computing satisfaction. MIS quarterly, 259-274.&lt;br/&gt;Evennou, F., &amp;amp; Marx, F. （2006）. Advanced integration of WiFi and inertial navigation systems for indoor mobile positioning. Eurasip journal on applied signal processing, 2006, 164-164.&lt;br/&gt;Gerber, B. S., &amp;amp; Eiser, A. R. （2001）. The patient-physician relationship in the Internet age: future prospects and the research agenda. Journal of Medical Internet Research, 3（2）.&lt;br/&gt;Gubbi, J., Buyya, R., Marusic, S., &amp;amp; Palaniswami, M. （2013）. Internet of Things （IoT）: A vision, architectural elements, and future directions. Future Generation Computer Systems, 29（7）, 1645-1660.&lt;br/&gt;Khan, J. Y., Yuce, M. R., &amp;amp; Karami, F. （2008）. Performance evaluation of a wireless body area sensor network for remote patient monitoring. Paper presented at the Engineering in Medicine and Biology Society, 2008. EMBS 2008. 30th Annual International Conference of the IEEE.&lt;br/&gt;Lee, J.-S., Su, Y.-W., &amp;amp; Shen, C.-C. （2007）. A comparative study of wireless protocols: Bluetooth, UWB, ZigBee, and Wi-Fi. Paper presented at the Industrial Electronics Society, 2007. IECON 2007. 33rd Annual Conference of the IEEE.&lt;br/&gt;Newman, N. （2014）. Apple ibeacon technology briefing. Journal of Direct, Data and Digital Marketing Practice, 15（3）, 222-225.&lt;br/&gt;Powell, J. A., Darvell, M., &amp;amp; Gray, J. （2003）. The doctor, the patient and the world-wide web: how the internet is changing healthcare. Journal of the Royal Society of Medicine, 96（2）, 74-76.&lt;br/&gt;Rohokale, V. M., Prasad, N. R., &amp;amp; Prasad, R. （2011）. A cooperative Internet of Things （IoT） for rural healthcare monitoring and control. Paper presented at the Wireless Communication, Vehicular Technology, Information Theory and Aerospace &amp;amp; Electronic Systems Technology （Wireless VITAE）, 2011 2nd International Conference on.&lt;br/&gt;Tan, L., &amp;amp; Wang, N. （2010）. Future internet: The internet of things. Paper presented at the Advanced Computer Theory and Engineering （ICACTE）, 2010 3rd International Conference on.&lt;br/&gt;Walker, A. （1983）. A Caring Community. In H. Glennerster ed., The Future of the Welfare State. London: Heinemann Educational Books, 157-172.&lt;br/&gt;Xia, F., Yang, L. T., Wang, L., &amp;amp; Vinel, A. （2012）. Internet of things. International Journal of Communication Systems, 25（9）, 1101.&lt;br/&gt;Zorzi, M., Gluhak, A., Lange, S., &amp;amp; Bassi, A. （2010）. From today's intranet of things to a future internet of things: a wireless-and mobility-related view. Wireless Communications, IEEE, 17（6）, 44-51.&lt;br/&gt; &lt;br/&gt;網站資料&lt;br/&gt;內政部統計處（民105）。台灣人口相關統計。台北市：內政部。民104年6月至105年4月，取自：http://www.moi.gov.tw/stat/index.aspx&lt;br/&gt;中央研究院 社會學研究所(民100年10月28日)。台灣社會變遷全記錄。民104年7月25日，取自：&lt;br/&gt;http://www.ios.sinica.edu.tw/TSCpedia/index.php/%E5%8F%B0%E7%81%A3%E7%A4%BE%E6%9C%83%E8%AE%8A%E9%81%B7%E5%85%A8%E8%A8%98%E9%8C%84&lt;br/&gt;吳其勳、陳思翰、鄭逸寧（民99）。用RFID打通醫療安全與效率的任督二脈。&lt;br/&gt;iThome，民104年10月2日，取自：http://www.ithome.com.tw/node/64356&lt;br/&gt;陳韋哲（民101）。解析室內定位五大技術。CTIMES電子產業社群平台。民104年8月12日，取自：http://www.hope.com.tw/DispNews-tw.asp?O=HJWC6A09T98SAA0MEP&lt;br/&gt;蔡麗雅（無日期）。生命徵象與危機處理。民104年9月18日，&lt;br/&gt;取自：http://163.13.224.25/~yama/data/94a/31.htm&lt;br/&gt;衛生福利部社會保險司（民104）。衛生福利相關統計。台北市：衛生福利部。民104年7月至8月，取自：http://www.mohw.gov.tw/CHT/DOSI/DM1_P.aspx?f_list_no=98&amp;amp;fod_list_no=5390&amp;amp;doc_no=51548&lt;br/&gt;衛生福利部統計處（民104）。衛生福利相關統計。台北市：衛生福利部。民104年7月至9月，取自：http://www.mohw.gov.tw/cht/DOS/Statistic.aspx?f_list_no=312&lt;br/&gt;衛生福利部(民104)。台灣病人安全資訊網。台北市：衛生福利部。民104年8月23日，取自：&lt;br/&gt;http://www.patientsafety.mohw.gov.tw/Content/Messagess/Contents.aspx?SiteID=1&amp;amp;MmmID=621273303575146267&lt;br/&gt;衛生福利部(民105)。台灣病人安全資訊網-TPR統計報表。台北市：衛生福利部。民105年6月3日，取自：&lt;br/&gt;http://www.patientsafety.mohw.gov.tw/Content/Downloads/List01.aspx?SiteID=1&amp;amp;MmmID=621273303702500244&lt;br/&gt;新貝比-婦幼專科巡房APP。民104年9月18日，&lt;br/&gt;取自：https://www.microsoft.com/zh-TW/store/apps/新貝比-婦幼專科巡房APP/9NBLGGH0Z1DB&lt;br/&gt;Google專利查詢。民104年8月12日，取自：http://www.google.com/patents/&lt;br/&gt;&lt;/div&gt;</t>
-        </is>
-      </c>
-      <c r="AA19" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/yb3g93</t>
         </is>
@@ -3047,10 +3022,14 @@
           <t>Database、Table Normalization Theory、Denormalization、User satisfaction</t>
         </is>
       </c>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>點閱:143</t>
+        </is>
+      </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>點閱:143</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -3059,23 +3038,18 @@
         </is>
       </c>
       <c r="X20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y20" t="inlineStr">
         <is>
           <t xml:space="preserve">
     資料庫無疑是迄今科技應用最基礎之根本，諸多科技演進無不以資料庫作為其資料探勘或分析之根基。隨著時代變遷，資料庫已由DOS模式指令方式，演進至資料庫管理系統(Database Managerment System - DBMS)模式，換句話說，從1980年代初期後，許多資料庫大廠紛紛推出圖形化管理工具與結構化查詢語言(Structured Query Language - SQL)。至今，目前市面上大多數資料庫系統都已是ANSI / SPARC三層資料庫系統架構所組成，其架構分別為內部層(Internal level)、概念層(Conceptual level)或稱為邏輯層(Logical level)，和外部層(External level)。    Tupper, C.(1998)之資料庫邏輯模組與開發設計研究指出，藉由移動和合併實體物件，或是創建新的實體物件與屬性來達成特殊客製要求，並且透過合成鍵來控制實體層資料異動或結構改變；本文以Tupper, C之研究作為研究基礎，並提出與實作一套整合DBMS概念層和外部層概念之研究，用以增強使用者對於資料掌握度與縮短異常資料處理時間，並將資料有效率地回復成正確的資料。本文透過使用者滿意度問卷調查方式，共回收93份有效問卷，針對「內容」、「格式」、「正確性」、「及時性」、「易用性」五種向度使用Qlikview分析，其結果顯示使用者對於使用資料庫後台應用意願是顯著的，此一研究可作為產官學界資料庫應用之研究提供參考。</t>
         </is>
       </c>
-      <c r="Z20" t="inlineStr">
+      <c r="Y20" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 【英文文獻】&lt;br/&gt;Aggelidis, V. P., &amp;amp; Chatzoglou, P. D. (2012). Hospital information systems: Measuring end user computing&lt;br/&gt;satisfaction (EUCS). Journal of biomedical informatics, 45(3), 566-579.&lt;br/&gt;Aguilera, M. K., Leners, J. B., Kotla, R., &amp;amp; Walfish, M. (2015). Yesquel: scalable&lt;br/&gt;SQL storage for Web applications. In Proceedings of the 2015 International&lt;br/&gt;Conference on Distributed Computing and Networking (p. 40). ACM.&lt;br/&gt;Bogdanova, A. V., &amp;amp; Lwinb, T. K. (2015). Storage database in cloud processing.&lt;br/&gt;Computer, 7(3), 493-498.&lt;br/&gt;Chaudhari, M. R. R., &amp;amp; Bakal, J. W. (2015). Overview of Database Auditing for Oracle Database. International&lt;br/&gt;Journal of Application or Innovation in Engineering &amp;amp; Management, 4(7).&lt;br/&gt;Codd, E. F. (1972). Further normalization of the database relational model. Data base&lt;br/&gt;systems, 33-64.&lt;br/&gt;Corral, K., Schuff, D., &amp;amp; Louis, R. D. S. (2006). The impact of alternative diagrams&lt;br/&gt;on the accuracy of recall: A comparison of star-schema diagrams and entity-&lt;br/&gt;relationship diagrams. Decision Support Systems, 42(1), 450-468.&lt;br/&gt;Deka, G. C. (2014). A Survey of Cloud Database Systems. IEEE Transaction on IT&lt;br/&gt;Professional, (2), 50-57.&lt;br/&gt;Doll, W. J., &amp;amp; Torkzadeh, G. (1988). The measurement of end-user computing&lt;br/&gt;satisfaction. MIS quarterly, 259-274.&lt;br/&gt;Erturk, E., &amp;amp; Jyoti, K. (2015). Perspectives on a Big Data Application:What Database&lt;br/&gt;Engineers and IT Students Need to Know. Engineering, Technology &amp;amp; Applied&lt;br/&gt;Science Research, 5(5), pp-850.&lt;br/&gt;Graefe, G. (1993). Query evaluation techniques for large databases. ACM Computing&lt;br/&gt;Surveys (CSUR), 25(2), 73-169.&lt;br/&gt;Guo, Z., &amp;amp; Xu, L. (2015). Research of security structure model for web application&lt;br/&gt;systems based on the relational database. International Journal of Security and&lt;br/&gt;Networks, 10(4), 207-213.&lt;br/&gt;Hacigümüş, H., Iyer, B., Li, C., &amp;amp; Mehrotra, S. (2002, June). Executing SQL over&lt;br/&gt;encrypted data in the database-service-provider model. In Proceedings of the&lt;br/&gt;2002 ACM SIGMOD international conference on Management of data (pp. 216-&lt;br/&gt;227). ACM.&lt;br/&gt;Imielinski, T., &amp;amp; Mannila, H. (1996). A database perspective on knowledge discovery.&lt;br/&gt;Communications of the ACM, 39(11), 58-64.&lt;br/&gt;Imielinski, T., Virmani, A., &amp;amp; Abdulghani, A. (1996, August). DataMine:&lt;br/&gt;Application Programming Interface and Query Language for Database Mining.&lt;br/&gt;In KDD (Vol. 96, p. 256).&lt;br/&gt;Korytkowski, M., Scherer, R., Staszewski, P., &amp;amp; Woldan, P. (2015). Bag-of-&lt;br/&gt;Features Image Indexing and Classification in Microsoft SQL Server Relational&lt;br/&gt;Database. Institute of Computational Intelligence Cze¸stochowa University of&lt;br/&gt;Technology al, Cze¸stochowa, Poland.&lt;br/&gt;Lasasmeh, A. A. (2015). A Comparative Study on Filtered, Vertical and Horizontal&lt;br/&gt;Inheritance Mapping in Database. International Journal of Database Theory &amp;amp;&lt;br/&gt;Application, 8(2).&lt;br/&gt;Ling, T. W. (1985). A Normal Form for Entity-Relationship Diagrams. ER, 1985,&lt;br/&gt;24-35.&lt;br/&gt;Martin, D., Fowlkes, C., Tal, D., &amp;amp; Malik, J. (2001). A database of human segmented&lt;br/&gt;natural images and its application to evaluating segmentation algorithms and&lt;br/&gt;measuring ecological statistics. In Computer Vision, 2001. ICCV 2001. Proceedings.&lt;br/&gt;Eighth IEEE International Conference on (Vol. 2, pp. 416-423). IEEE.&lt;br/&gt;Sanders, G. L., &amp;amp; Shin, S. (2001, January). Denormalization effects on performance&lt;br/&gt;of RDBMS. In System Sciences, 2001. Proceedings of the 34th Annual Hawaii&lt;br/&gt;International Conference on (pp. 9-pp). IEEE.&lt;br/&gt;Shin, S. K., &amp;amp; Sanders, G. L. (2006). Denormalization strategies for data retrieval&lt;br/&gt;from data warehouses. Decision Support Systems, 42(1), 267-282.&lt;br/&gt;Tanaka, S., &amp;amp; Kobayashi, H. (2015). Trigger Based Assertion Tool in Software&lt;br/&gt;Development. Lecture Notes on Software Engineering, 3(2).&lt;br/&gt;Tupper, C. (1998). The Physics of Logical Modeling. Database Programming &amp;amp;&lt;br/&gt;Design, 11(9).&lt;br/&gt;Vijayprasath, S., &amp;amp; Rajan, S. P. (2015). Design of a Simple Graphical User Interface&lt;br/&gt;to the Relational Database Management System. International Journal of&lt;br/&gt;Computer Science and Mobile Computing, 4(1), 354-359.&lt;br/&gt;&lt;br/&gt;【英文參考書籍】&lt;br/&gt;Donald R. Cooper, &amp;amp; Pamela S. Schindler (2015). Business Research Methods (12th&lt;br/&gt;edition). McGraw-Hill Education.&lt;br/&gt;Elmasri, R., &amp;amp; Navathe, S. B. (2010). Fundamentals of Database Systems (6th edition).&lt;br/&gt;Addison-Wesley Longman Publishing Co., Inc.&lt;br/&gt;Owens, K (2003). Programming Oracle Triggers and Stored Procedures Third Edition.&lt;br/&gt;Prentice Hall PTR.&lt;br/&gt;&lt;br/&gt;【中文參考書籍】&lt;br/&gt;陳會安 (2014). SQL Server 2014 資料庫設計與開發實務. 台北市：碁峯資訊股份有限公司.&lt;br/&gt;&lt;br/&gt;【網站資料】&lt;br/&gt;LinkedIn (2015)，資料庫反向正規化，Retrieved September 19, 2015 from&lt;br/&gt;http://www.slideshare.net/sohailhaiderbhatti/denormalization&lt;br/&gt;Microsoft Developer Network (2015)，資料庫正規化，Retrieved August 31, 2015 from&lt;br/&gt;https://msdn.microsoft.com/zh-tw/library/Aa291817(v=VS.71).aspx&lt;br/&gt;Microsoft Developer Network (2015)，資料庫反向正規化，Retrieved August 31, 2015 from&lt;br/&gt;https://msdn.microsoft.com/zh-tw/library/Aa291817(v=VS.71).aspx&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA20" t="inlineStr">
+      <c r="Z20" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/33phtc</t>
         </is>
@@ -3180,10 +3154,14 @@
           <t>Wormhole Attack、Communication Protocol</t>
         </is>
       </c>
-      <c r="U21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>點閱:126</t>
+        </is>
+      </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>點閱:126</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -3192,23 +3170,18 @@
         </is>
       </c>
       <c r="X21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y21" t="inlineStr">
         <is>
           <t xml:space="preserve">
     資訊安全在現在的網路時代中非常重要，一個不小心便會被懷有惡意的攻擊者監聽竊取資料，甚至偽裝偽造資料給任何人；其中在無線網路的環境中，由於移動節點的特性，使行動裝置在建立連線時更加容易被懷有惡意的人所攻擊，加上隨著智慧型手機的發展，人們依賴行動裝置上網的比例增多，當遭受到惡意攻擊時所受到的損傷也越來越大；在這麼多的攻擊當中，以蟲洞攻擊最為讓人難以防範與偵測，且一旦有蟲洞攻擊者存在與網路中，攻擊者便可以很容易的癱瘓網路、竊聽資料、偽造資料，非常輕易便能對網路造成重大影響。    本研究中針對網路攻擊中的蟲洞攻擊，提出在建立連線與傳送資料時，進行三階段的處理，分別為準備階段、交易階段與發佈操作階段。透過這三階段的進行，能夠達到預防未被授權的惡意攻擊者對連線的攻擊，也可以避免內部擁有授權的惡意攻擊者不能輕易的取得訊息內容，在新節點加入時也能快速的知道安全連線拓樸。提供一個新的協定使無線網路中的節點能夠免於受到蟲洞攻擊。</t>
         </is>
       </c>
-      <c r="Z21" t="inlineStr">
+      <c r="Y21" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 Abbasi, A. A., &amp;amp; Younis, M. (2007). A survey on clustering algorithms for wireless sensor networks. Computer communications, 30(14), 2826-2841.&lt;br/&gt;Acs, G., Buttyan, L., &amp;amp; Vajda, I. (2006). Provably secure on-demand source routing in mobile ad hoc networks. Mobile Computing, IEEE Transactions on,5(11), 1533-1546.&lt;br/&gt;Burmester, M., &amp;amp; de Medeiros, B. (2009). On the security of route discovery in manets. Mobile Computing, IEEE Transactions on, 8(9), 1180-1188.&lt;br/&gt;Chiu, H. S., &amp;amp; Lui, K. S. (2006, January). DelPHI: wormhole detection mechanism for ad hoc wireless networks. In Wireless pervasive computing, 2006 1st international symposium on (pp. 6-pp). IEEE.&lt;br/&gt;Cover, T. M., &amp;amp; Thomas, J. A. (2012). Elements of information theory. John Wiley &amp;amp; Sons.&lt;br/&gt;Dahlberg, T., Mallat, N., Ondrus, J., &amp;amp; Zmijewska, A. (2008). Past, present and future of mobile payments research: A literature review. Electronic Commerce Research and Applications, 7(2), 165-181.&lt;br/&gt;Fourati, A., Al Agha, K., &amp;amp; Ben Ayed, H. K. (2007). Secure and fair auctions over ad hoc networks. International Journal of Electronic Business, 5(3), 276-293.&lt;br/&gt;Galanxhi-Janaqi, H., &amp;amp; Nah, F. F. H. (2004). U-commerce: emerging trends and research issues. Industrial Management &amp;amp; Data Systems, 104(9), 744-755.&lt;br/&gt;Girault, M. (1991, January). Self-certified public keys. In Advances in Cryptology—EUROCRYPT’91 (pp. 490-497). Springer Berlin Heidelberg.&lt;br/&gt;Hankerson, D., Vanstone, S., &amp;amp; Menezes, A. J. (2004). Guide to elliptic curve cryptography. Springer.&lt;br/&gt;Hassinen, M., Hyppönen, K., &amp;amp; Trichina, E. (2008). Utilizing national public-key infrastructure in mobile payment systems. Electronic Commerce Research and Applications, 7(2), 214-231.&lt;br/&gt;Hu, Y. C., Perrig, A., &amp;amp; Johnson, D. B. (2003, April). Packet leashes: a defense against wormhole attacks in wireless networks. In INFOCOM 2003. Twenty-Second Annual Joint Conference of the IEEE Computer and Communications. IEEE Societies (Vol. 3, pp. 1976-1986). IEEE.&lt;br/&gt;Hu, Y. C., Perrig, A., &amp;amp; Johnson, D. B. (2005). Ariadne: A secure on-demand routing protocol for ad hoc networks. Wireless networks, 11(1-2), 21-38.&lt;br/&gt;Hu, Y. C., Perrig, A., &amp;amp; Johnson, D. B. (2006). Wormhole attacks in wireless networks. Selected Areas in Communications, IEEE Journal on, 24(2), 370-380.&lt;br/&gt;Hwang, R. J., Shiau, S. H., &amp;amp; Jan, D. F. (2007). A new mobile payment scheme for roaming services. Electronic Commerce Research and Applications, 6(2), 184-191.&lt;br/&gt;Jin, S., Park, C., Choi, D., Chung, K., &amp;amp; Yoon, H. (2005). Cluster-based trust evaluation scheme in an ad hoc network. ETRI journal, 27(4), 465-468.&lt;br/&gt;Kadhiwal, S., &amp;amp; Zulfiquar, A. U. S. (2007). Analysis of mobile payment security measures and different standards. Computer Fraud &amp;amp; Security, 2007(6), 12-16.&lt;br/&gt;Khabbazian, M., Mercier, H., &amp;amp; Bhargava, V. K. (2006, November). Nis02-1: Wormhole attack in wireless ad hoc networks: Analysis and countermeasure. In Global Telecommunications Conference, 2006. GLOBECOM'06. IEEE (pp. 1-6). IEEEKonheim, A. G. (2007). Computer security and cryptography. John Wiley &amp;amp; Sons.&lt;br/&gt;Kousaridas, A., Parissis, G., &amp;amp; Apostolopoulos, T. (2008). An open financial services architecture based on the use of intelligent mobile devices. Electronic Commerce Research and Applications, 7(2), 232-246.&lt;br/&gt;Leung, A., Sheng, Y., &amp;amp; Cruickshank, H. (2007). The security challenges for mobile ubiquitous services. Information security technical report, 12(3), 162-171.&lt;br/&gt;Lin, I. C., &amp;amp; Chang, C. C. (2007). A practical electronic payment system for message delivery service in the mobile environment. Wireless Personal Communications, 42(2), 247-261.&lt;br/&gt;Naït-Abdesselam, F., Bensaou, B., &amp;amp; Taleb, T. (2008). Detecting and avoiding wormhole attacks in wireless ad hoc networks. Communications Magazine, IEEE, 46(4), 127-133.&lt;br/&gt;Su, M. Y. (2010). WARP: A wormhole-avoidance routing protocol by anomaly detection in mobile ad hoc networks. computers &amp;amp; security, 29(2), 208-224.&lt;br/&gt;Vandana, C. P., &amp;amp; Devaraj, A. F. S.(2013). MLDW-A MultiLayered Detection mechanism for Wormhole attack in AODV based MANET. Privacy and Trust Management (IJSPTM) Vol, 2.&lt;br/&gt;Varshney, U. (2002). Multicast support in mobile commerce applications.Computer, 35(2), 115-117.&lt;br/&gt;Varshney, U. (2008). A middleware framework for managing transactions in group-oriented mobile commerce services. Decision Support Systems, 46(1), 356-365.&lt;br/&gt;Varshney, U., &amp;amp; Vetter, R. (2002). Mobile commerce: framework, applications and networking support. Mobile networks and Applications, 7(3), 185-198.&lt;br/&gt;Yu, J. Y., &amp;amp; Chong, P. H. J. (2005). A survey of clustering schemes for mobile ad hoc networks. IEEE Communications Surveys and Tutorials, 7(1-4), 32-48.&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA21" t="inlineStr">
+      <c r="Z21" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/du3dde</t>
         </is>
@@ -3313,35 +3286,34 @@
           <t>knowledge map、keywords of paper、trend analysis、data visualization、big data</t>
         </is>
       </c>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>點閱:367</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>點閱:367</t>
+          <t>8</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y22" t="inlineStr">
         <is>
           <t xml:space="preserve">
 本研究提出一個以論文關鍵字為基礎的知識地圖，藉此觀察與分析研究趨勢，由關鍵字作為研究觀察的目標，藉此了解關鍵字背後所屬的研究領域在不同年份之間受重視的程度。本研究以Decision Support Systems Journal為研究標的物，將2010~2014年之間的所有論文關鍵字視為節點(Node)透過連線(Link)表示關鍵字的關聯，同篇論文中關鍵字會組成完全圖(Complete Graph)，最終所有論文分別組成後完全圖之後就產生一個屬於該年度的知識地圖。透過知識地圖觀察關鍵字的連結情形與整體分佈藉此觀察期刊的研究趨勢與熱門關鍵字。除了知識地圖之外本研究結合長條圖與時間軸設計呈現熱門關鍵字與之連結的節點。透過該方法了解單一關鍵字與熱門關鍵字同時出現的次數，透過長條圖搭配時間軸可以了解單一關鍵字的歷史資訊。本研究最終結論得到熱門關鍵字與趨勢前三名分別為: Decision support system、Data mining、Electronic commerce。透過使用者評估，最後得到正面的使用者回饋。本研究以知識地圖觀察整體研究趨勢，對於後續的相關研究與資訊檢索系統功能設計方面本研究的方法是有幫助的。</t>
         </is>
       </c>
-      <c r="Z22" t="inlineStr">
+      <c r="Y22" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 Biuk-Aghai, R. P., Yang, M., Pang, P. C. I., Ao, W. H., Fong, S., &amp;amp; Si, Y. W. (2015). A map-like visualisation method based on liquid modelling. Journal of Visual Languages &amp;amp; Computing, 31, 87-103.&lt;br/&gt;Chen, N. S., Wei, C. W., &amp;amp; Chen, H. J. (2008). Mining e-Learning domain concept map from academic articles. Computers &amp;amp; Education, 50(3), 1009-1021.&lt;br/&gt;Choi, Jinho, Sangyoon Yi, and Kun Chang Lee. "Analysis of keyword networks in MIS research and implications for predicting knowledge evolution."Information &amp;amp; Management 48.8 (2011): 371-381.&lt;br/&gt;Cilibrasi, R. L., &amp;amp; Vitanyi, P. M. (2007). The google similarity distance.Knowledge        and Data Engineering, IEEE Transactions on, 19(3), 370-383.&lt;br/&gt;Claver, E., González, R., &amp;amp; Llopis, J. (2000). An analysis of research in information systems (1981–1997). Information &amp;amp; Management, 37(4), 181-195.&lt;br/&gt;Hao, J., Yan, Y., Gong, L., Wang, G., &amp;amp; Lin, J. (2014). Knowledge map-based method for domain knowledge browsing. Decision Support Systems, 61, 106-114.&lt;br/&gt;Harrathi, R., &amp;amp; Calabretto, S. (2007). A query graph for visual querying structured documents. In Digital Information Management, 2007. ICDIM'07. 2nd International Conference on (Vol. 1, pp. 116-120). IEEE.&lt;br/&gt;Holsapple, C. (Ed.). (2004). Handbook on knowledge management 1: Knowledge matters (Vol. 1). New York:Springer..&lt;br/&gt;Keim, D. A. (2002). Information visualization and visual data mining.Visualization and Computer Graphics, IEEE Transactions on, 8(1), 1-8.&lt;br/&gt;Lee, M. R., &amp;amp; Chen, T. T. (2012). Revealing research themes and trends in knowledge management: From 1995 to 2010. Knowledge-Based Systems, 28, 47-58.&lt;br/&gt;Liu, X., Guo, Z., Lin, Z., &amp;amp; Ma, J. (2013). A local social network approach for research management. Decision Support Systems, 56, 427-438.&lt;br/&gt;McCandless, D. (2010). The beauty of data visualization. Technology, Entertainment, Design(TED). URL :https://www.ted.com/talks/david_mccandless_the_beauty_of_data_visualization.&lt;br/&gt;Salton, G., &amp;amp; Buckley, C.(1988). Term-weighting approaches in automatic text retrieval. Information processing &amp;amp; management, 24(5), 513-523.&lt;br/&gt;Watthananon, J., &amp;amp; Mingkhwan, A. (2012). Optimizing knowledge management using knowledge map. Procedia Engineering, 32, 1169-1177.&lt;br/&gt;YongYue, C., &amp;amp; HuoSong, X. (2009). Research on the Auto-construction Methods of Concept Map. In Intelligent Human-Machine Systems and Cybernetics, 2009. IHMSC'09. International Conference on (Vol. 2, pp. 75-77). IEEE.&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22097MCU05396040%22.&amp;amp;searchmode=basic" target="_blank"&gt;王俊凱(民97)。資訊管理議題趨勢之研究。銘傳大學資訊管理學系碩士班碩士論文，桃園縣。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22095NTU05489146%22.&amp;amp;searchmode=basic" target="_blank"&gt;汪修斌(民96)。視覺化USPTO專利資料庫的線上搜尋結果。國立臺灣大學機械工程學系碩士論文，台北市。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22090NSYS5396042%22.&amp;amp;searchmode=basic" target="_blank"&gt;李律品(民91)。資訊管理研究之生態演化分析。國立中山大學資訊管理研究所碩士論文，高雄市。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22088CYCU0392020%22.&amp;amp;searchmode=basic" target="_blank"&gt;李紹群(民88) 。以關鍵字相關性為基礎之超本文資訊檢索系統。中原大學資訊工程學系碩士班碩士論文，桃園縣。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0006618800" target="_blank"&gt;侯榮英, 張文信, 蕭智維, &amp;amp; 江宜靜. (2010). 運用商業智慧系統建構視覺化會計圖表應用於醫院管理-以南部某醫院為例. 醫務管理期刊, 11(3), 75-87.&lt;/a&gt;&lt;br/&gt;梁定澎(民86)。資訊管理研究方法總論。資訊管理學報，4(1)，1-6。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22097MCU05396007%22.&amp;amp;searchmode=basic" target="_blank"&gt;陳畇安(民97)。資管頂級期刊趨勢分析-以MISQ 和ISR 為例。銘傳大學資訊管理學系碩士班碩士班碩士論文，桃園縣。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22102CCU00396047%22.&amp;amp;searchmode=basic" target="_blank"&gt;陳昱廷(民 103)。風險圖像行動化與視覺化對企業風險管理的影響-以食品安全為例。國立中正大學資訊管理研究所碩士論文(尚未對外公開) ，嘉義縣。&lt;/a&gt;&lt;br/&gt;蕭聖哲(民97)。管理科學趨勢之研究—以Management Science為例。銘傳大學資訊傳播工程學系碩士班碩士論文，桃園縣。&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA22" t="inlineStr">
+      <c r="Z22" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/k9s6za</t>
         </is>
@@ -3446,35 +3418,34 @@
           <t>medical information systems、cloud computing、SaaS、Microsoft Azure、MVC</t>
         </is>
       </c>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>點閱:275</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>點閱:275</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y23" t="inlineStr">
         <is>
           <t xml:space="preserve">
 隨著雲端運算技術的發展，各行各業紛紛的導入與應用雲端技術於資訊系統中。醫療相關產業也紛紛的應用雲端運算技術開發各式週邊產品與系統。例如行動化的個人生理紀錄系統、雲端藥局等。健保局的雲端藥歷、健康護照等等。但台灣醫療產業隨著健保實施後整個醫療大環境劇烈的改變，診所雖增加快速但其資訊系統卻還保留在20年前的技術架構。但因資料安全、作業系統更版問題，導致原資訊系統在往後將面臨系統不容問題。本研究希望藉著ASP.NET MVC、WCF(Windows Communication Foundation)、Microsoft Azure與HTML 5.0等相關技術開發建構於雲端運算平台的新一代醫療資訊系統。探討相關技術的運用及診所對於雲端醫療資訊系統的接受度。同時探討診所對於架設於公有雲及混合雲兩種不同雲端運算的SaaS服務模式的可行性分析。做為資訊廠商發展下一世代醫療資訊系統的參考，提供診所一個便宜、便利的醫療資訊系統。</t>
         </is>
       </c>
-      <c r="Z23" t="inlineStr">
+      <c r="Y23" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 參考文獻&lt;br/&gt;中文部分:&lt;br/&gt;1.中華電信。HiCloud 雲運算。上網日期：2012年11月28日 檢自：http://hicloud.hinet.net/caas/specifications.html。&lt;br/&gt;2.凌群電子報。論Windows Communication Foundation。史印辰，上網日期 : 2015年11月25日，檢自:http://www.syscom.com.tw/ePaper.aspx?id=170&lt;br/&gt;3.行政院資訊網，上網日期：2012年3月1日，檢自http://www.ey.gov.tw/mp?mp=1。&lt;br/&gt;4.吳武明 (民83)。邁向21世紀的資訊管理。台北市: 松岡圖書有限公司。&lt;br/&gt;5.吳政澤(民 99)。以雲端運算建構健康管理平台之研究，未出版論文。臺北醫學大學醫學資訊研究所，台北市。&lt;br/&gt;6.黃興進、佘明玲、劉忠峰(2006)。醫療資訊管理。台北市:台灣健康資訊管理學會出版。&lt;br/&gt;7.陳偉霖(民 99)。雲端運算平台服務之策略分析，未出版論文。國立交通大學科技管理研究所，新竹市。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005553244" target="_blank"&gt;8.楊澤泉、彭啟釗、張音(1997)。台灣診所採用資訊科技之關鍵因素研究。管理學報，14(4)，507-531。&lt;/a&gt;&lt;br/&gt;9.楊文誌(2010)。雲端運算 Cloud Computing技術指南。松岡圖書，台北市。&lt;br/&gt;10.葉偉 等(2010)。互聯網時代的軟件革命: SaaS架構設計。電子工業出版社。北京市。&lt;br/&gt;11.蔡文正、龔佩珍(2003)。民眾對基層診所評價與就醫選擇影響因素。台灣衛誌，22(3)，181-193。&lt;br/&gt;12.鄧瑋敦(2010)。雲端運算大解密。城邦文化。台北市。&lt;br/&gt;13.鮑世穎(民 99)。以雲端服務建構貿易資訊系統之研究，未出版論文。國立台北科技大學商業自動化與管理研究所，台北市。&lt;br/&gt;14.鍾文勻(民 99)。雲端服務在物業資訊管理之應用-以社區大樓為例，未出版論文。國立台北科技大學土木與防災研究所，台北市。&lt;br/&gt;15.台灣大學計算機及資訊網路中心 電子報 。服務導向架構(Service-Oriented Architecture, SOA) 簡介。曾保彰，&lt;br/&gt;上網日期:2015年11月25日 ，檢自:http://www.cc.ntu.edu.tw/chinese/epaper/20070620_1008.htm&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;英文部分:&lt;br/&gt;16.Bharadwaj, A. S. (2000). A resource-based perspective on information technology capability and firm performance: An empirical investigation. MIS Quarterly, 24(1), 169-196.&lt;br/&gt;17.Charles Babcock.(2010). Management Strategies for the Cloud Revolution. New York: McGraw-Hill.&lt;br/&gt;18.Edward J.Giniat. Cloud Computing :Innovating the business of health care. Healthcare financial management, (MAY 2011), 130-131.&lt;br/&gt;19.Ethan, K.&amp;amp; Norman, S. &amp;amp; Prashila, D. &amp;amp; Samuel, S.(2011) Is There An App For That? Electronic Health Records(EHRS) And A New Environment of Conflict Prevention and Resolution, April 17, 2012, from http://www.law.duke.edu/journals/lcp 。&lt;br/&gt;20.McPhee, S. J., Brid J.A. and Fordham D.(1989). Promoting cancer screening: a randomized, controlled trial of three interventions. Arch. Inter. Med.,149, 1866-1872.&lt;br/&gt;21.Miller, M.(2008). Cloud Computing: Web-Based Applications That Change the Way You Work and Collaborate Online. IN: QUE Pub.&lt;br/&gt;22.Michael Armbrust, Armando Fox, Rean Griffith, Anthony D. Joseph, Randy Katz, Andy Konwinski, Gunho Lee, David Patterson, Ariel Rabkin, Ion Stoica, and Matei Zaharia(2009) Above the Clouds: A Berkeley View of Cloud Computing.  UC Berkeley Reliable Adaptive Distributed System Laboratory。February 10, 2012 , form http://www.eecs.berkeley.edu/Pubs/TechRpts/2009/EECS-2009-28.html。&lt;br/&gt;23.Mircosoft.com。Windows Azure。2012/11/28 form: http://www.windowsazure.com/zh-tw/pricing/calculator/?scenario=cloud。&lt;br/&gt;24.Microsoft MSDN。2012/5/1 form: http://msdn.microsoft.com/library。&lt;br/&gt;25.Microsoft TechNet。[雲端運算] 第二章:深入雲端-Windows Azure 平台。2012/5/27, form : http://blogs.technet.com/b/technet_taiwan/archive/2010/05/26/windows-azure.aspx 。&lt;br/&gt;26.Nori, A., &amp;amp; Gunn, J. (1998). Data in general practice. Aust Fam Physician, 27(Suppl 2), S110-S111.&lt;br/&gt;27.Stratmann WC.(1975). A Study of Consumer Attitudes about Health Care: The Delivery of Ambulatory Services. Med Care 1975,13(5) ,37-48.&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA23" t="inlineStr">
+      <c r="Z23" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/f5kp2t</t>
         </is>
@@ -3579,35 +3550,34 @@
           <t>ISO27001、Information Security System、Document Management</t>
         </is>
       </c>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>點閱:420</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>點閱:420</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Y24" t="inlineStr">
         <is>
           <t xml:space="preserve">
 資訊安全議題已被廣泛的研究，ISO27001是資訊安全研究必討論的議題，國際標準ISO27001，是目前在資訊安全中最為大眾參考的標準，在探討標準ISO27001的研究中，大多在探討如何完成ISO27001的風險管理以及管理的規範，來達到資訊安全標準，但達到資訊安全標準卻少了系統的支撐，對資訊安全來說是不完善的。本研究探討醫院資訊安全系統，目的在於針對ISO27001技術條例做系統的建置，讓欲建置資訊系統的醫院，可以參考此系統方法，來對自身的文件以及員工的使用狀況權限得以監看，保護醫院的病患資料，對於中小型的醫院或診所，推動資訊安全，必須考量的不僅只有資訊安全的規範，還要考量到建置上硬體的設備，軟體的需求，才能無慮的建置資訊安全，因此，本研究在建置上，對於硬體的需求減輕中小型醫院或診所的壓力，讓中小型醫院也能擁有一套遵守ISO27001標準的資訊安全系統。</t>
         </is>
       </c>
-      <c r="Z24" t="inlineStr">
+      <c r="Y24" t="inlineStr">
         <is>
           <t>&lt;div style="padding:10px;text-align:left;"&gt;
 Ahmad, S., Alam, K. M. R., Rahman, H., &amp;amp; Tamura, S. (2015). A comparison between symmetric and asymmetric key encryption algorithm based decryption mixnets. 2015 International Conference on Networking Systems and Security (NSysS).1-5. IEEE.&lt;br/&gt;Al Housani, H.,Baek, J.,&amp;amp; Chan Yeob Yeun.(2011). Survey on certificateless public key cryptography. International Conference for Internet Technology and Secured Transactions (ICITST). 53-58.&lt;br/&gt;Barrows, R. C., &amp;amp; Clayton, P. D. (1996). Privacy, confidentiality, and electronic medical records. Journal of the American Medical Informatics Association, 3(2), 139-148.&lt;br/&gt;Calder, A. (2013). Information Security &amp;amp; ISO 27001-An Introduction. United Kingdom：IT Governance Green.&lt;br/&gt;Fanfara, P., Danková, E., &amp;amp; Dufala, M. (2012). Usage of asymmetric encryption algorithms to enhance the security of sensitive data in secure communication. 2012 IEEE 10th International Symposium on Applied Machine Intelligence and Informatics (SAMI), 213-217. IEEE.&lt;br/&gt;Fluhrer, S., Mantin, I., &amp;amp; Shamir, A. (2001). Weaknesses in the key scheduling algorithm of RC4. In Selected areas in cryptography (pp. 1-24). Springer Berlin Heidelberg.&lt;br/&gt;Garfinkel, S., Spafford, G., &amp;amp; Schwartz, A. (2003). Practical UNIX and Internet security. Sebastopol,California：O'reilly&amp;amp;Associates,Inc.&lt;br/&gt;Garg, R.M.,&amp;amp;Singh, M.(2013). Evolving profligate and conspicuous web applications using reverse AJAX. International Conference on Computing, Communications and Networking Technologies (ICCCNT).1-5.&lt;br/&gt;Hutt, A. E. (1995). Management's Role in Computer Security. Computer Security Handbook. New York: Wiley.&lt;br/&gt;ISO, B. (2000). IEC 17799: 2000. Information technology-Code of practice for information security management, BSI.&lt;br/&gt;Kenning, M. (2001). "Security management standard—iso 17799/bs 7799." BT Technology Journal 19(3): 132-136.&lt;br/&gt;Ku, C.-Y., Chang, Y.-W., &amp;amp; Yen, D. C. (2009). National information security policy and its implementation: A case study in Taiwan. Telecommunications Policy, 33(7), 371-384.&lt;br/&gt;Liao, K. H., &amp;amp; Chueh, H. E. (2012). Medical Organization Information Security Management Based on ISO27001 Information Security Standard. Journal of Software, 7(4), 792-797.&lt;br/&gt;Lillywhite, T. P. (2004). Implementing BS7799 in the UK National Health Service. Computer Fraud &amp;amp; Security, 2004(2), 4-8.&lt;br/&gt;Miao, Q. G., Wang, Y., Cao, Y., Zhang, X. G., &amp;amp; Liu, Z. L. (2010). APICapture-a tool for monitoring the behavior of malware. 2010 3rd International Conference on Advanced Computer Theory and Engineering (ICACTE), (Vol. 4, pp. V4-390). IEEE.&lt;br/&gt;Pimentel, V., &amp;amp; Nickerson, B. G. (2012). Communicating and displaying real-time data with WebSocket. Internet Computing, IEEE, 16(4), 45-53.&lt;br/&gt;Qiang, Z., Xinqian, W., Meng, Z., &amp;amp; Ertao, L. (2012, August). Wind Farm SCADA System's Web Implementation Based on the Comet Technology. InComputer Science &amp;amp; Service System (CSSS), 2012 International Conference on (pp. 750-753). IEEE.&lt;br/&gt;Russell, D., &amp;amp; Gangemi, G. (1991). Computer security basics.Sebastopol,California：O'reilly&amp;amp;Associates,Inc.&lt;br/&gt;Saint-Germain,R.&amp;amp; René. (2005). Information Security Management Best Practice Based on ISO/IEC 17799. Information Management Journal, 39(4), 60-66.&lt;br/&gt;Sharif, S.O.&amp;amp; Mansoor, S.P.(2010).Performance analysis of stream and block cipher algorithms. International Conference on Advanced Computer Theory and Engineering (ICACTE).V1-522-V1525.&lt;br/&gt;Singh, G., &amp;amp; Supriya, A. (2013). A Study of Encryption Algorithms (RSA, DES, 3DES and AES) for Information Security. International Journal of Computer Applications, 67(19), 33-38.&lt;br/&gt;Skvorc, D., Horvat, M., &amp;amp; Srbljic, S. (2014, May). Performance evaluation of Websocket protocol for implementation of full-duplex web streams. InInformation and Communication Technology, Electronics and Microelectronics (MIPRO), 2014 37th International Convention on (pp. 1003-1008). IEEE.&lt;br/&gt;Smith, M. (1989). Computer security-threats, vulnerabilities and countermeasures. Information Age, 11(4), 205-210.&lt;br/&gt;Von Solms, R. (1996). Information security management: the second generation. Computers &amp;amp; Security, 15(4), 281-288.&lt;br/&gt;Von Solms, R., van der Haar, H., von Solms, S. H., &amp;amp; Caelli, W. J. (1994). A framework for information security evaluation. Information &amp;amp; Management, 26(3), 143-153.&lt;br/&gt;Watkins, S. (2013). An Introduction to Information Security and ISO27001: 2013: A Pocket Guide. United Kingdom：IT Governance Publishing.&lt;br/&gt;Yang, W. C., &amp;amp; Lee, J. X. (2013). Implementation of stream cipher service in JCA. 2013 IEEE International Symposium On Next-Generation Electronics (ISNE), (pp. 557-561). IEEE.&lt;br/&gt;Yoshihara, K., Sugiyama, K., Horiuchi, H., &amp;amp; Obana, S. (1999). Dynamic polling scheme based on time variation of network management information values. In Integrated Network Management, 1999. Distributed Management for the Networked Millennium. Proceedings of the Sixth IFIP/IEEE International Symposium on (pp. 141-154). IEEE&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22098CCU05777013%22.&amp;amp;searchmode=basic" target="_blank"&gt;王天健(2010)。植基於ISO27001: 2005 之跨產業資訊安全管理系統比較--以高科技產業與傳統產業為例，國立中正大學資訊管理研究所碩士論文。&lt;/a&gt;&lt;br/&gt;王全民、周清、 劉宇明、朱二夫(2010)。文件透明加密技術研究。計算機技術與發展， 3，147-150。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005509514" target="_blank"&gt;吳琮璠(1996)。國外政府機構資訊系統安全稽核制度。存款保險資訊季刊，2，21-40。&lt;/a&gt;&lt;br/&gt;吳琮璠、謝清佳(2003)。資訊管理理論與實務，台北市：智勝文化事業有限公司。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22094NCKU5028045%22.&amp;amp;searchmode=basic" target="_blank"&gt;杜偉欽(2006)。結合HIPAA與ISO27001為基礎探討醫療院所資訊安全管理之研究，國立成功大學工程科學系碩士在職專班學位論文。&lt;/a&gt;&lt;br/&gt;季延平、郭鴻志(1995)。系統分析與設計，台北市：華泰書局。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22092NCKU5028112%22.&amp;amp;searchmode=basic" target="_blank"&gt;侯皇熙(2004)。植基於BS7799探討政府部門的資訊安全管理─以海關資訊部門為例，國立成功大學工程科學系碩士在職專班學位論文。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0004795963" target="_blank"&gt;洪國興、季延平、趙榮耀(2003)。資訊安全評估準則層級結構之研究，圖書館學與資訊科學，29，22-44。&lt;/a&gt;&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22100NCU05396064%22.&amp;amp;searchmode=basic" target="_blank"&gt;張正宏(2012)。探討銀行業ISO/IEC 27001: 2005資訊安全管理現況-以 T 銀行為例，國立中央大學資訊管理學系碩士在職專班學位論文。&lt;/a&gt;&lt;br/&gt;張小川、陳最、凃飛(2013)。基於過濾驅動的透明加密文件系统研究與實現，計算機運用與軟體，44-47。&lt;br/&gt;葉乃菁、李順仁(2004)。網路安全理論與實務，台北市：文魁資訊。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22101NCCU5769003%22.&amp;amp;searchmode=basic" target="_blank"&gt;楊雅竹(2012)。營業秘密合理保密措施之研究，國立政治大學智慧財產研究所碩士論文。&lt;/a&gt;&lt;br/&gt;趙銘偉、毛銳、江榮安(2009)。基於過濾驅動的透明加密文件系统模型，計算機工程, 1, 150-152。&lt;br/&gt;&lt;a href="http://ndltd.ncl.edu.tw/cgi-bin/gs32/gsweb.cgi?o=dnclcdr&amp;amp;s=id=%22092NTPU0121114%22.&amp;amp;searchmode=basic" target="_blank"&gt;劉智敏(2004)。運用BS 7799 建構資訊安全風險管理指標，國立台北大學企業管理學系碩士論文。&lt;/a&gt;&lt;br/&gt;樊國楨、楊晉寧(1996)。互連網(Internet)電子信息交換安全-以電子公文交換作業安全為本，電腦稽核，14-25。&lt;br/&gt;&lt;a href="http://readopac2.ncl.edu.tw/nclJournal/search/detail.jsp?dtdId=000040&amp;amp;search_type=detail&amp;amp;la=ch&amp;amp;checked=&amp;amp;unchecked=&amp;amp;sysId=0005592579" target="_blank"&gt;賴溪松(1998)。資訊安全國家標準之應用與發展，資訊安全通訊，4，29-33。&lt;/a&gt;&lt;br/&gt;&lt;br/&gt;&lt;/div&gt;</t>
         </is>
       </c>
-      <c r="AA24" t="inlineStr">
+      <c r="Z24" t="inlineStr">
         <is>
           <t>https://hdl.handle.net/11296/fzfpp9</t>
         </is>

</xml_diff>